<commit_message>
Code Version 07052020 17:50
</commit_message>
<xml_diff>
--- a/Prime_Job_Automation/Configuration/RuleFactory/Master Rule Factory.xlsx
+++ b/Prime_Job_Automation/Configuration/RuleFactory/Master Rule Factory.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Prime_Job_Automation\Configuration\RuleFactory\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\PJA\Prime_Job_Automation\Configuration\RuleFactory\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED91F2DB-FBC4-4C89-91F6-181D8AD1805F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C648451-9879-4FF6-A0A7-0A8813EC3691}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" tabRatio="351" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$N$39</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$N$40</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="235">
   <si>
     <t>Password</t>
   </si>
@@ -104,9 +104,6 @@
     <t>Bayantel Enrollment</t>
   </si>
   <si>
-    <t>Upload Installment - Email</t>
-  </si>
-  <si>
     <t>Upload Reversal</t>
   </si>
   <si>
@@ -188,18 +185,9 @@
     <t>No</t>
   </si>
   <si>
-    <t>Test</t>
-  </si>
-  <si>
     <t>Yes</t>
   </si>
   <si>
-    <t>giri</t>
-  </si>
-  <si>
-    <t>play</t>
-  </si>
-  <si>
     <t>Bayantel123</t>
   </si>
   <si>
@@ -698,9 +686,6 @@
     <t xml:space="preserve"> ' - _ space</t>
   </si>
   <si>
-    <t>tmfinstallmentcosmos</t>
-  </si>
-  <si>
     <t>/prime/UBP_ubp/payment_files</t>
   </si>
   <si>
@@ -723,13 +708,40 @@
   </si>
   <si>
     <t>/tsys/prime/UBP_ubp/mastercard_incoming_files</t>
+  </si>
+  <si>
+    <t>Upload Installment</t>
+  </si>
+  <si>
+    <t>\\10.19.81.248\rpa\PMU\PCIDSS\Upload Installment Cosmos</t>
+  </si>
+  <si>
+    <t>ccod@mmddyy</t>
+  </si>
+  <si>
+    <t>^upload_installment[2][0-9][0-1][0-9][0-3][0-9]a.txt$|^upload _installment[2][0-9][0-1][0-9][0-3][0-9]b.txt$</t>
+  </si>
+  <si>
+    <t>cosmostmffile</t>
+  </si>
+  <si>
+    <t>SMPyyddmm</t>
+  </si>
+  <si>
+    <t>Upload Installment - Cosmos Email</t>
+  </si>
+  <si>
+    <t>Staging\Upload Installment Cosmos Email</t>
+  </si>
+  <si>
+    <t>Archive\Upload Installment Cosmos Email</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -765,8 +777,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -782,12 +800,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -823,7 +835,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -853,12 +865,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -866,6 +872,19 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1205,14 +1224,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N48"/>
+  <dimension ref="A1:N49"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.140625" style="5" customWidth="1"/>
-    <col min="2" max="2" width="28.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.5703125" style="5" customWidth="1"/>
+    <col min="2" max="2" width="34" style="5" customWidth="1"/>
     <col min="3" max="3" width="28.140625" style="5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="28.42578125" style="5"/>
     <col min="5" max="5" width="4.7109375" style="5" bestFit="1" customWidth="1"/>
@@ -1223,1459 +1242,1487 @@
     <col min="10" max="10" width="14.85546875" style="5" customWidth="1"/>
     <col min="11" max="11" width="23.85546875" style="5" customWidth="1"/>
     <col min="12" max="12" width="25" style="5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="45.42578125" style="5" customWidth="1"/>
+    <col min="13" max="13" width="44.140625" style="5" customWidth="1"/>
     <col min="14" max="14" width="30" style="5" customWidth="1"/>
     <col min="15" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="H1" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="C1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>64</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>68</v>
       </c>
       <c r="J1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="L1" s="4" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="M1" s="4" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="N1" s="4" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="7"/>
       <c r="D2" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
       <c r="G2" s="7" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="I2" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="L2" s="7" t="s">
+        <v>218</v>
+      </c>
+      <c r="M2" s="7" t="s">
         <v>183</v>
       </c>
-      <c r="J2" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="K2" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="L2" s="7" t="s">
-        <v>223</v>
-      </c>
-      <c r="M2" s="7" t="s">
-        <v>187</v>
-      </c>
       <c r="N2" s="10" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="C3" s="7"/>
       <c r="D3" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
       <c r="G3" s="7" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>228</v>
-      </c>
-      <c r="J3" s="7" t="s">
-        <v>54</v>
-      </c>
+        <v>223</v>
+      </c>
+      <c r="J3" s="7"/>
       <c r="K3" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L3" s="7" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="M3" s="7" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="N3" s="10" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="7"/>
       <c r="D4" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
       <c r="G4" s="7" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>183</v>
-      </c>
-      <c r="J4" s="7">
-        <v>1234</v>
-      </c>
+        <v>179</v>
+      </c>
+      <c r="J4" s="7"/>
       <c r="K4" s="7" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="L4" s="7" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="M4" s="7" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="N4" s="10" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>18</v>
       </c>
       <c r="C5" s="7"/>
       <c r="D5" s="8" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E5" s="6"/>
       <c r="F5" s="6"/>
       <c r="G5" s="7" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="J5" s="7"/>
       <c r="K5" s="7" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="L5" s="7" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="M5" s="7" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="N5" s="10" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="C6" s="7"/>
       <c r="D6" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
       <c r="G6" s="7" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="J6" s="7"/>
       <c r="K6" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L6" s="7" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="M6" s="7" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="N6" s="10" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>3</v>
       </c>
       <c r="C7" s="7"/>
       <c r="D7" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E7" s="6"/>
       <c r="F7" s="6"/>
       <c r="G7" s="7" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="J7" s="7"/>
       <c r="K7" s="7" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="L7" s="7" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="M7" s="7" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="N7" s="10" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>4</v>
       </c>
       <c r="C8" s="7"/>
       <c r="D8" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
       <c r="G8" s="7" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="J8" s="7"/>
       <c r="K8" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L8" s="7" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="M8" s="7" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="N8" s="10" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B9" s="7" t="s">
         <v>5</v>
       </c>
       <c r="C9" s="7"/>
       <c r="D9" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
       <c r="G9" s="7" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="J9" s="7"/>
       <c r="K9" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L9" s="7" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="M9" s="7" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="N9" s="10" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B10" s="7" t="s">
         <v>6</v>
       </c>
       <c r="C10" s="7"/>
       <c r="D10" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
       <c r="G10" s="7" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="I10" s="7" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="J10" s="7"/>
       <c r="K10" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L10" s="7" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="M10" s="7" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="N10" s="10" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B11" s="7" t="s">
         <v>7</v>
       </c>
       <c r="C11" s="7"/>
       <c r="D11" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E11" s="6"/>
       <c r="F11" s="6"/>
       <c r="G11" s="7" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="I11" s="7" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="J11" s="7"/>
       <c r="K11" s="7" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="L11" s="7" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="M11" s="7" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="N11" s="10" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="12" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B12" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C12" s="7"/>
       <c r="D12" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
       <c r="G12" s="7" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="H12" s="7" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="I12" s="7" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="J12" s="7"/>
       <c r="K12" s="7" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="L12" s="7" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="M12" s="7" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="N12" s="10" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="13" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B13" s="7" t="s">
         <v>9</v>
       </c>
       <c r="C13" s="7"/>
       <c r="D13" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E13" s="6"/>
       <c r="F13" s="6"/>
       <c r="G13" s="7" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="H13" s="7" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="I13" s="7" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="J13" s="7"/>
       <c r="K13" s="7" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="L13" s="7" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="M13" s="7" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="N13" s="10" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B14" s="7" t="s">
         <v>10</v>
       </c>
       <c r="C14" s="7"/>
       <c r="D14" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
       <c r="G14" s="7" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="H14" s="7" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="I14" s="7" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="J14" s="7"/>
       <c r="K14" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L14" s="7" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="M14" s="7" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="N14" s="10" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="15" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B15" s="7" t="s">
         <v>11</v>
       </c>
       <c r="C15" s="7"/>
       <c r="D15" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
       <c r="G15" s="7" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="H15" s="7" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="I15" s="7" t="s">
-        <v>229</v>
-      </c>
-      <c r="J15" s="7" t="s">
-        <v>208</v>
-      </c>
+        <v>224</v>
+      </c>
+      <c r="J15" s="7"/>
       <c r="K15" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L15" s="7" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="M15" s="7" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="N15" s="10" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="16" spans="1:14" ht="105" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B16" s="7" t="s">
         <v>13</v>
       </c>
       <c r="C16" s="7"/>
       <c r="D16" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
       <c r="G16" s="7" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="H16" s="7" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="I16" s="7" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="J16" s="7"/>
       <c r="K16" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L16" s="7" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="M16" s="7" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="N16" s="10" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="17" spans="1:14" ht="75" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C17" s="7"/>
       <c r="D17" s="9" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="E17" s="6"/>
       <c r="F17" s="6"/>
       <c r="G17" s="7" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="H17" s="7" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="I17" s="7" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="J17" s="7"/>
       <c r="K17" s="7" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="L17" s="7" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="M17" s="7" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="N17" s="10" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="18" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C18" s="7"/>
       <c r="D18" s="9" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="E18" s="6"/>
       <c r="F18" s="6"/>
       <c r="G18" s="7" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="H18" s="7" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="I18" s="7" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="J18" s="7"/>
       <c r="K18" s="7" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="L18" s="7" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="M18" s="7" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="N18" s="10" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="19" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C19" s="7"/>
       <c r="D19" s="9" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="7" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="H19" s="7" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="I19" s="7" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="J19" s="7"/>
       <c r="K19" s="7" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="L19" s="7" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="M19" s="7" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="N19" s="10" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="20" spans="1:14" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="12" t="s">
-        <v>60</v>
+      <c r="A20" s="18" t="s">
+        <v>56</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>203</v>
-      </c>
-      <c r="C20" s="13"/>
+        <v>199</v>
+      </c>
+      <c r="C20" s="11"/>
       <c r="D20" s="9" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="7" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="H20" s="7" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="I20" s="7" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="J20" s="7"/>
       <c r="K20" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L20" s="7" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="M20" s="7" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="N20" s="10" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="21" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="1" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="E21" s="1">
         <v>22</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="I21" s="7" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="J21" s="1"/>
       <c r="K21" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="L21" s="7" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="M21" s="1" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="N21" s="10" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="22" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="C22" s="1"/>
       <c r="D22" s="1" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="E22" s="1">
         <v>22</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="I22" s="7" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="J22" s="1"/>
       <c r="K22" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L22" s="7" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="M22" s="1" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="N22" s="10" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="23" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C23" s="1"/>
       <c r="D23" s="1" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="E23" s="1">
         <v>22</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="I23" s="7" t="s">
-        <v>183</v>
-      </c>
-      <c r="J23" s="1" t="s">
-        <v>15</v>
-      </c>
+        <v>179</v>
+      </c>
+      <c r="J23" s="1"/>
       <c r="K23" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="L23" s="7" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="M23" s="1" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="N23" s="10" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="24" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C24" s="1"/>
       <c r="D24" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E24" s="1">
         <v>22</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="I24" s="7" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="J24" s="1"/>
       <c r="K24" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="L24" s="7" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="M24" s="1" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="N24" s="10" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="25" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C25" s="1"/>
       <c r="D25" s="1" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="E25" s="1">
         <v>22</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="I25" s="7" t="s">
-        <v>184</v>
-      </c>
-      <c r="J25" s="1"/>
+        <v>180</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>231</v>
+      </c>
       <c r="K25" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="L25" s="7" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="M25" s="1" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="N25" s="10" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="26" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C26" s="1"/>
       <c r="D26" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E26" s="1">
         <v>22</v>
       </c>
       <c r="F26" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="I26" s="7" t="s">
+        <v>223</v>
+      </c>
+      <c r="J26" s="1"/>
+      <c r="K26" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="G26" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="H26" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="I26" s="7" t="s">
-        <v>228</v>
-      </c>
-      <c r="J26" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="K26" s="1" t="s">
-        <v>51</v>
-      </c>
       <c r="L26" s="7" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="M26" s="1" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="N26" s="10" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="27" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
       <c r="G27" s="1" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="I27" s="7" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="L27" s="7" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="M27" s="1" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="N27" s="1"/>
     </row>
     <row r="28" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
       <c r="G28" s="1" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="I28" s="7" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="J28" s="1">
         <v>1234</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="L28" s="7" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="M28" s="1" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="N28" s="1"/>
     </row>
     <row r="29" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
       <c r="G29" s="1" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="I29" s="7" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="J29" s="1" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="K29" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="L29" s="7" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="M29" s="1" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="N29" s="1"/>
     </row>
-    <row r="30" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
       <c r="G30" s="1" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="I30" s="7" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="K30" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L30" s="7" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="M30" s="1" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="N30" s="1"/>
     </row>
     <row r="31" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>24</v>
+        <v>226</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
       <c r="F31" s="2"/>
       <c r="G31" s="1" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="I31" s="7" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="J31" s="7" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="K31" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L31" s="7" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="M31" s="3" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="N31" s="1"/>
     </row>
     <row r="32" spans="1:14" ht="45" x14ac:dyDescent="0.25">
-      <c r="A32" s="11" t="s">
-        <v>62</v>
+      <c r="A32" s="2" t="s">
+        <v>58</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>199</v>
+        <v>232</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>222</v>
+        <v>230</v>
       </c>
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
       <c r="F32" s="2"/>
       <c r="G32" s="1" t="s">
-        <v>200</v>
+        <v>233</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>201</v>
+        <v>234</v>
       </c>
       <c r="I32" s="7" t="s">
+        <v>223</v>
+      </c>
+      <c r="J32" s="17" t="s">
         <v>228</v>
       </c>
-      <c r="J32" s="1"/>
       <c r="K32" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L32" s="7" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="M32" s="3" t="s">
-        <v>202</v>
+        <v>229</v>
       </c>
       <c r="N32" s="1"/>
     </row>
     <row r="33" spans="1:14" ht="45" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
-        <v>62</v>
+      <c r="A33" s="16" t="s">
+        <v>56</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="D33" s="2"/>
+        <v>195</v>
+      </c>
+      <c r="C33" s="1"/>
+      <c r="D33" s="15" t="s">
+        <v>227</v>
+      </c>
       <c r="E33" s="2"/>
       <c r="F33" s="2"/>
       <c r="G33" s="1" t="s">
-        <v>104</v>
+        <v>196</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>135</v>
+        <v>197</v>
       </c>
       <c r="I33" s="7" t="s">
-        <v>228</v>
-      </c>
-      <c r="J33" s="7" t="s">
-        <v>208</v>
-      </c>
+        <v>223</v>
+      </c>
+      <c r="J33" s="1"/>
       <c r="K33" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L33" s="7" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="M33" s="3" t="s">
-        <v>196</v>
-      </c>
-      <c r="N33" s="1"/>
-    </row>
-    <row r="34" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+        <v>198</v>
+      </c>
+      <c r="N33" s="10" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="D34" s="2"/>
       <c r="E34" s="2"/>
       <c r="F34" s="2"/>
       <c r="G34" s="1" t="s">
-        <v>172</v>
+        <v>100</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>174</v>
+        <v>131</v>
       </c>
       <c r="I34" s="7" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="J34" s="7" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="K34" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L34" s="7" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="M34" s="3" t="s">
-        <v>158</v>
+        <v>192</v>
       </c>
       <c r="N34" s="1"/>
     </row>
-    <row r="35" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="D35" s="2"/>
       <c r="E35" s="2"/>
       <c r="F35" s="2"/>
       <c r="G35" s="1" t="s">
-        <v>105</v>
+        <v>168</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>136</v>
+        <v>170</v>
       </c>
       <c r="I35" s="7" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="J35" s="7" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="K35" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L35" s="7" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="M35" s="3" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="N35" s="1"/>
     </row>
     <row r="36" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
       <c r="F36" s="2"/>
       <c r="G36" s="1" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="I36" s="7" t="s">
-        <v>225</v>
-      </c>
-      <c r="J36" s="1"/>
+        <v>223</v>
+      </c>
+      <c r="J36" s="7" t="s">
+        <v>204</v>
+      </c>
       <c r="K36" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L36" s="7" t="s">
-        <v>225</v>
-      </c>
-      <c r="M36" s="1" t="s">
-        <v>197</v>
+        <v>223</v>
+      </c>
+      <c r="M36" s="3" t="s">
+        <v>155</v>
       </c>
       <c r="N36" s="1"/>
     </row>
     <row r="37" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C37" s="3" t="s">
-        <v>218</v>
+        <v>27</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>215</v>
       </c>
       <c r="D37" s="2"/>
       <c r="E37" s="2"/>
       <c r="F37" s="2"/>
       <c r="G37" s="1" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="I37" s="7" t="s">
-        <v>226</v>
-      </c>
-      <c r="J37" s="14" t="s">
-        <v>59</v>
-      </c>
+        <v>220</v>
+      </c>
+      <c r="J37" s="1"/>
       <c r="K37" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L37" s="7" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="M37" s="1" t="s">
-        <v>162</v>
+        <v>193</v>
       </c>
       <c r="N37" s="1"/>
     </row>
     <row r="38" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="D38" s="2"/>
       <c r="E38" s="2"/>
       <c r="F38" s="2"/>
       <c r="G38" s="1" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="I38" s="7" t="s">
-        <v>224</v>
-      </c>
-      <c r="J38" s="1">
-        <v>1234</v>
+        <v>219</v>
+      </c>
+      <c r="J38" s="12" t="s">
+        <v>55</v>
       </c>
       <c r="K38" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L38" s="7" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="M38" s="7" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="N38" s="1"/>
     </row>
     <row r="39" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>221</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="D39" s="2"/>
       <c r="E39" s="2"/>
       <c r="F39" s="2"/>
       <c r="G39" s="1" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="I39" s="7" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="J39" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="K39" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="L39" s="7" t="s">
+        <v>221</v>
+      </c>
+      <c r="M39" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="N39" s="1"/>
+    </row>
+    <row r="40" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="K39" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="L39" s="7" t="s">
-        <v>224</v>
-      </c>
-      <c r="M39" s="7" t="s">
-        <v>161</v>
-      </c>
-      <c r="N39" s="1"/>
-    </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="C48" s="15"/>
+      <c r="B40" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="E40" s="2"/>
+      <c r="F40" s="2"/>
+      <c r="G40" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="H40" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="I40" s="7" t="s">
+        <v>219</v>
+      </c>
+      <c r="J40" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="K40" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="L40" s="7" t="s">
+        <v>219</v>
+      </c>
+      <c r="M40" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="N40" s="1"/>
+    </row>
+    <row r="49" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C49" s="13"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2693,8 +2740,9 @@
     <hyperlink ref="N4:N26" r:id="rId12" display="rrhamachandran@unionbankph.com" xr:uid="{0B09F3EC-2224-4918-843C-25097DD2A45B}"/>
     <hyperlink ref="N20" r:id="rId13" xr:uid="{AE271E2F-CCDD-4C24-9900-396BBF58413A}"/>
     <hyperlink ref="D20" r:id="rId14" xr:uid="{CCBA97EB-AA4C-4510-8CF5-C3BEF6F5096A}"/>
+    <hyperlink ref="N33" r:id="rId15" xr:uid="{6E7A3F64-9C89-45CF-B813-F7656E9F4231}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId15"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId16"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Code Version 07052020 22:25
</commit_message>
<xml_diff>
--- a/Prime_Job_Automation/Configuration/RuleFactory/Master Rule Factory.xlsx
+++ b/Prime_Job_Automation/Configuration/RuleFactory/Master Rule Factory.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\PJA\Prime_Job_Automation\Configuration\RuleFactory\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14C89CF7-07C7-4242-A625-4AB385647929}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6FC294E-0D40-448B-8B26-5606B57D37DF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" tabRatio="351" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,8 +29,44 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Divakar Ragupathy</author>
+  </authors>
+  <commentList>
+    <comment ref="M2" authorId="0" shapeId="0" xr:uid="{39ACA343-E88B-4897-9561-9AAEBA9E2255}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Maynilad and Vecco billing shares same folder</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M4" authorId="0" shapeId="0" xr:uid="{20C86102-3E0A-4364-A306-E92F2660C190}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Maynilad and Vecco billing shares same folder</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="234">
   <si>
     <t>Password</t>
   </si>
@@ -581,15 +617,9 @@
     <t>^LUMINAVISAUNIONBANKC-[2][0][0-9][0-9][0-1][0-9][0-3][0-9].txt$|^LUMINAVISAUNIONBANKCARD-[2][0][0-9][0-9][0-1][0-9][0-3][0-9].txt$|^UBP-[2][0][0-9][0-9][0-1][0-9][0-3][0-9].txt$</t>
   </si>
   <si>
-    <t>^UNION_[2][0][2][0-9][0-1][0-9][0-3][0-9].TXT$</t>
-  </si>
-  <si>
     <t>^UNIONENROLL_[2][0][2][0-9][0-1][0-9][0-3][0-9]_RET.TXT$</t>
   </si>
   <si>
-    <t>^UBC[0-9][0-9][0-9][0-9][0-9]BRF.DAT$</t>
-  </si>
-  <si>
     <t>^UBC[0-9][0-9][0-9][0-9][0-9].ERF.DAT$</t>
   </si>
   <si>
@@ -653,9 +683,6 @@
     <t>luminaautocharge</t>
   </si>
   <si>
-    <t>billingfilenotificationbayantelecommunicationdecemberthcutoffubpbillmanagermanager</t>
-  </si>
-  <si>
     <t>enr/canfilenotificationbayantelecommunication</t>
   </si>
   <si>
@@ -735,13 +762,19 @@
   </si>
   <si>
     <t>Archive\Upload Installment Cosmos Email</t>
+  </si>
+  <si>
+    <t>^UNION_[2][0][2][0-9][0-1][0-9][0-3][0-9].TXT$|^UBC[0-9][0-9][0-9][0-9][0-9]BRF.DAT$</t>
+  </si>
+  <si>
+    <t>billingfilenotificationbayantelecommunication</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -781,6 +814,12 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -1223,7 +1262,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N49"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
@@ -1318,10 +1357,10 @@
         <v>51</v>
       </c>
       <c r="L2" s="7" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="M2" s="7" t="s">
-        <v>183</v>
+        <v>232</v>
       </c>
       <c r="N2" s="10" t="s">
         <v>159</v>
@@ -1347,17 +1386,17 @@
         <v>171</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="J3" s="7"/>
       <c r="K3" s="7" t="s">
         <v>50</v>
       </c>
       <c r="L3" s="7" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="M3" s="7" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="N3" s="10" t="s">
         <v>159</v>
@@ -1390,10 +1429,10 @@
         <v>51</v>
       </c>
       <c r="L4" s="7" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="M4" s="7" t="s">
-        <v>185</v>
+        <v>232</v>
       </c>
       <c r="N4" s="10" t="s">
         <v>159</v>
@@ -1426,7 +1465,7 @@
         <v>51</v>
       </c>
       <c r="L5" s="7" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="M5" s="7" t="s">
         <v>138</v>
@@ -1455,17 +1494,17 @@
         <v>172</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="J6" s="7"/>
       <c r="K6" s="7" t="s">
         <v>50</v>
       </c>
       <c r="L6" s="7" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="M6" s="7" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="N6" s="10" t="s">
         <v>159</v>
@@ -1498,10 +1537,10 @@
         <v>51</v>
       </c>
       <c r="L7" s="7" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="M7" s="7" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="N7" s="10" t="s">
         <v>159</v>
@@ -1527,14 +1566,14 @@
         <v>110</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="J8" s="7"/>
       <c r="K8" s="7" t="s">
         <v>50</v>
       </c>
       <c r="L8" s="7" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="M8" s="7" t="s">
         <v>139</v>
@@ -1563,17 +1602,17 @@
         <v>111</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="J9" s="7"/>
       <c r="K9" s="7" t="s">
         <v>50</v>
       </c>
       <c r="L9" s="7" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="M9" s="7" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="N9" s="10" t="s">
         <v>159</v>
@@ -1599,17 +1638,17 @@
         <v>112</v>
       </c>
       <c r="I10" s="7" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="J10" s="7"/>
       <c r="K10" s="7" t="s">
         <v>50</v>
       </c>
       <c r="L10" s="7" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="M10" s="7" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="N10" s="10" t="s">
         <v>159</v>
@@ -1642,7 +1681,7 @@
         <v>51</v>
       </c>
       <c r="L11" s="7" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="M11" s="7" t="s">
         <v>140</v>
@@ -1678,7 +1717,7 @@
         <v>51</v>
       </c>
       <c r="L12" s="7" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="M12" s="7" t="s">
         <v>141</v>
@@ -1714,7 +1753,7 @@
         <v>51</v>
       </c>
       <c r="L13" s="7" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="M13" s="7" t="s">
         <v>142</v>
@@ -1743,17 +1782,17 @@
         <v>116</v>
       </c>
       <c r="I14" s="7" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="J14" s="7"/>
       <c r="K14" s="7" t="s">
         <v>50</v>
       </c>
       <c r="L14" s="7" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="M14" s="7" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="N14" s="10" t="s">
         <v>159</v>
@@ -1779,14 +1818,14 @@
         <v>117</v>
       </c>
       <c r="I15" s="7" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="J15" s="7"/>
       <c r="K15" s="7" t="s">
         <v>50</v>
       </c>
       <c r="L15" s="7" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="M15" s="7" t="s">
         <v>143</v>
@@ -1815,17 +1854,17 @@
         <v>118</v>
       </c>
       <c r="I16" s="7" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="J16" s="7"/>
       <c r="K16" s="7" t="s">
         <v>50</v>
       </c>
       <c r="L16" s="7" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="M16" s="7" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="N16" s="10" t="s">
         <v>159</v>
@@ -1858,7 +1897,7 @@
         <v>51</v>
       </c>
       <c r="L17" s="7" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="M17" s="7" t="s">
         <v>182</v>
@@ -1894,7 +1933,7 @@
         <v>51</v>
       </c>
       <c r="L18" s="7" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="M18" s="7" t="s">
         <v>144</v>
@@ -1930,7 +1969,7 @@
         <v>51</v>
       </c>
       <c r="L19" s="7" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="M19" s="7" t="s">
         <v>145</v>
@@ -1944,32 +1983,32 @@
         <v>56</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C20" s="11"/>
       <c r="D20" s="9" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="7" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="H20" s="7" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="I20" s="7" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="J20" s="7"/>
       <c r="K20" s="7" t="s">
         <v>50</v>
       </c>
       <c r="L20" s="7" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="M20" s="7" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="N20" s="10" t="s">
         <v>159</v>
@@ -2006,7 +2045,7 @@
         <v>51</v>
       </c>
       <c r="L21" s="7" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="M21" s="1" t="s">
         <v>146</v>
@@ -2039,14 +2078,14 @@
         <v>173</v>
       </c>
       <c r="I22" s="7" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="J22" s="1"/>
       <c r="K22" s="1" t="s">
         <v>50</v>
       </c>
       <c r="L22" s="7" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="M22" s="1" t="s">
         <v>147</v>
@@ -2086,7 +2125,7 @@
         <v>51</v>
       </c>
       <c r="L23" s="7" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="M23" s="1" t="s">
         <v>148</v>
@@ -2126,7 +2165,7 @@
         <v>51</v>
       </c>
       <c r="L24" s="7" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="M24" s="1" t="s">
         <v>149</v>
@@ -2162,16 +2201,16 @@
         <v>180</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="K25" s="1" t="s">
         <v>51</v>
       </c>
       <c r="L25" s="7" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="M25" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="N25" s="10" t="s">
         <v>159</v>
@@ -2201,14 +2240,14 @@
         <v>126</v>
       </c>
       <c r="I26" s="7" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="J26" s="1"/>
       <c r="K26" s="1" t="s">
         <v>50</v>
       </c>
       <c r="L26" s="7" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="M26" s="1" t="s">
         <v>150</v>
@@ -2225,7 +2264,7 @@
         <v>20</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
@@ -2246,7 +2285,7 @@
         <v>51</v>
       </c>
       <c r="L27" s="7" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="M27" s="1" t="s">
         <v>174</v>
@@ -2261,7 +2300,7 @@
         <v>21</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
@@ -2282,14 +2321,14 @@
         <v>51</v>
       </c>
       <c r="L28" s="7" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="M28" s="1" t="s">
         <v>181</v>
       </c>
       <c r="N28" s="1"/>
     </row>
-    <row r="29" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>58</v>
       </c>
@@ -2297,7 +2336,7 @@
         <v>22</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>207</v>
+        <v>233</v>
       </c>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
@@ -2318,7 +2357,7 @@
         <v>51</v>
       </c>
       <c r="L29" s="7" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="M29" s="1" t="s">
         <v>151</v>
@@ -2333,7 +2372,7 @@
         <v>23</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
@@ -2345,7 +2384,7 @@
         <v>169</v>
       </c>
       <c r="I30" s="7" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="J30" s="1" t="s">
         <v>53</v>
@@ -2354,7 +2393,7 @@
         <v>50</v>
       </c>
       <c r="L30" s="7" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="M30" s="1" t="s">
         <v>152</v>
@@ -2366,10 +2405,10 @@
         <v>58</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
@@ -2381,16 +2420,16 @@
         <v>130</v>
       </c>
       <c r="I31" s="7" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="J31" s="7" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="K31" s="1" t="s">
         <v>50</v>
       </c>
       <c r="L31" s="7" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="M31" s="3" t="s">
         <v>153</v>
@@ -2402,34 +2441,34 @@
         <v>58</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
       <c r="F32" s="2"/>
       <c r="G32" s="1" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="I32" s="7" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="J32" s="17" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="K32" s="1" t="s">
         <v>50</v>
       </c>
       <c r="L32" s="7" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="M32" s="3" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="N32" s="1"/>
     </row>
@@ -2438,32 +2477,32 @@
         <v>56</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C33" s="1"/>
       <c r="D33" s="15" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="E33" s="2"/>
       <c r="F33" s="2"/>
       <c r="G33" s="1" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="I33" s="7" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="J33" s="1"/>
       <c r="K33" s="1" t="s">
         <v>50</v>
       </c>
       <c r="L33" s="7" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="M33" s="3" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="N33" s="10" t="s">
         <v>159</v>
@@ -2477,7 +2516,7 @@
         <v>24</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="D34" s="2"/>
       <c r="E34" s="2"/>
@@ -2489,19 +2528,19 @@
         <v>131</v>
       </c>
       <c r="I34" s="7" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="J34" s="7" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="K34" s="1" t="s">
         <v>50</v>
       </c>
       <c r="L34" s="7" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="M34" s="3" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="N34" s="1"/>
     </row>
@@ -2513,7 +2552,7 @@
         <v>25</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="D35" s="2"/>
       <c r="E35" s="2"/>
@@ -2525,16 +2564,16 @@
         <v>170</v>
       </c>
       <c r="I35" s="7" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="J35" s="7" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="K35" s="1" t="s">
         <v>50</v>
       </c>
       <c r="L35" s="7" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="M35" s="3" t="s">
         <v>154</v>
@@ -2549,7 +2588,7 @@
         <v>26</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
@@ -2561,16 +2600,16 @@
         <v>132</v>
       </c>
       <c r="I36" s="7" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="J36" s="7" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="K36" s="1" t="s">
         <v>50</v>
       </c>
       <c r="L36" s="7" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="M36" s="3" t="s">
         <v>155</v>
@@ -2585,7 +2624,7 @@
         <v>27</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="D37" s="2"/>
       <c r="E37" s="2"/>
@@ -2597,17 +2636,17 @@
         <v>133</v>
       </c>
       <c r="I37" s="7" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="J37" s="1"/>
       <c r="K37" s="1" t="s">
         <v>50</v>
       </c>
       <c r="L37" s="7" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="M37" s="1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="N37" s="1"/>
     </row>
@@ -2619,7 +2658,7 @@
         <v>28</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="D38" s="2"/>
       <c r="E38" s="2"/>
@@ -2631,7 +2670,7 @@
         <v>134</v>
       </c>
       <c r="I38" s="7" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="J38" s="12" t="s">
         <v>55</v>
@@ -2640,7 +2679,7 @@
         <v>50</v>
       </c>
       <c r="L38" s="7" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="M38" s="7" t="s">
         <v>156</v>
@@ -2655,7 +2694,7 @@
         <v>12</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="D39" s="2"/>
       <c r="E39" s="2"/>
@@ -2667,7 +2706,7 @@
         <v>136</v>
       </c>
       <c r="I39" s="7" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="J39" s="14" t="s">
         <v>55</v>
@@ -2676,7 +2715,7 @@
         <v>50</v>
       </c>
       <c r="L39" s="7" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="M39" s="1" t="s">
         <v>158</v>
@@ -2691,10 +2730,10 @@
         <v>29</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="E40" s="2"/>
       <c r="F40" s="2"/>
@@ -2705,7 +2744,7 @@
         <v>135</v>
       </c>
       <c r="I40" s="7" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="J40" s="12" t="s">
         <v>54</v>
@@ -2714,7 +2753,7 @@
         <v>50</v>
       </c>
       <c r="L40" s="7" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="M40" s="7" t="s">
         <v>157</v>
@@ -2744,5 +2783,6 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId16"/>
+  <legacyDrawing r:id="rId17"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Code Version 080520 13:30
</commit_message>
<xml_diff>
--- a/Prime_Job_Automation/Configuration/RuleFactory/Master Rule Factory.xlsx
+++ b/Prime_Job_Automation/Configuration/RuleFactory/Master Rule Factory.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\PJA\Prime_Job_Automation\Configuration\RuleFactory\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6FC294E-0D40-448B-8B26-5606B57D37DF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB83D2D6-0643-45BC-AD74-A7E562DD0377}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" tabRatio="351" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="231">
   <si>
     <t>Password</t>
   </si>
@@ -206,9 +206,6 @@
     <t>/Sun/</t>
   </si>
   <si>
-    <t>/PlayEveryday/</t>
-  </si>
-  <si>
     <t>Port</t>
   </si>
   <si>
@@ -638,9 +635,6 @@
     <t>^MSAS_DSR_FILE_[0-3][0-9]-[0-1][0-9]-[2][0][2][0-9]_[0-9][0-9]_[0-9][0-9]_[0-9][0-9].txt$</t>
   </si>
   <si>
-    <t>^CCOD TMF [0-1][0-9][0-3][0-9][2][0-9].txt$|^CCOD TMF REVERSAL UPLOAD [0-1][0-9][0-3][0-9][2][0-9].txt$</t>
-  </si>
-  <si>
     <t>^NON_AIR_TRN_[2][0][2][0-9][0-1][0-9][0-3][0-9]_[0-9][0-9]_[0-9][0-9]_[0-9][0-9]_UNIONCD.out$</t>
   </si>
   <si>
@@ -683,9 +677,6 @@
     <t>luminaautocharge</t>
   </si>
   <si>
-    <t>enr/canfilenotificationbayantelecommunication</t>
-  </si>
-  <si>
     <t>tmfinstallmentupload</t>
   </si>
   <si>
@@ -704,39 +695,12 @@
     <t>collectionsreturnfileforupload</t>
   </si>
   <si>
-    <t>cebupacificcreditcardunioncdnonair</t>
-  </si>
-  <si>
     <t>collectionsreassignmentupload</t>
   </si>
   <si>
-    <t xml:space="preserve"> ' - _ space</t>
-  </si>
-  <si>
     <t>/prime/UBP_ubp/payment_files</t>
   </si>
   <si>
-    <t>/tsys/prime/UBP_ubp/collector_incoming_files</t>
-  </si>
-  <si>
-    <t>/tsys/prime/UBP_ubp/interfaces_incoming</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> /tsys/prime/UBP_ubp/collector_incoming_files</t>
-  </si>
-  <si>
-    <t>/tsys/prime/UBP_ubp/visa_incoming_files</t>
-  </si>
-  <si>
-    <t>/tsys/prime/UBP_ubp/payment_files</t>
-  </si>
-  <si>
-    <t>/tsys/prime/UBP_ubp/bridgefiles</t>
-  </si>
-  <si>
-    <t>/tsys/prime/UBP_ubp/mastercard_incoming_files</t>
-  </si>
-  <si>
     <t>Upload Installment</t>
   </si>
   <si>
@@ -768,6 +732,33 @@
   </si>
   <si>
     <t>billingfilenotificationbayantelecommunication</t>
+  </si>
+  <si>
+    <t>enr/canfilenotificationbayantelcommunication</t>
+  </si>
+  <si>
+    <t>cebupacific</t>
+  </si>
+  <si>
+    <t>^CCOD TMF [0-1][0-9][0-3][0-9][2][0-9].txt$|^CCOD TMF REVERSAL UPLOAD [0-1][0-9][0-3][0-9][2][0-9].txt$|^CCOD TMF REVERSALS [0-1][0-9][0-3][0-9][2][0-9] 1.txt$</t>
+  </si>
+  <si>
+    <t>\\10.19.81.248\rpa\PMU\PCIDSS\PlayEveryday</t>
+  </si>
+  <si>
+    <t>/prime/UBP_ubp/interfaces_incoming</t>
+  </si>
+  <si>
+    <t>/prime/UBP_ubp/bridgefiles</t>
+  </si>
+  <si>
+    <t>/prime/UBP_ubp/visa_incoming_files</t>
+  </si>
+  <si>
+    <t>/prime/UBP_ubp/mastercard_incoming_files</t>
+  </si>
+  <si>
+    <t>/prime/UBP_ubp/collector_incoming_files</t>
   </si>
 </sst>
 </file>
@@ -874,7 +865,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -923,6 +914,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1271,10 +1265,10 @@
   <cols>
     <col min="1" max="1" width="7.5703125" style="5" customWidth="1"/>
     <col min="2" max="2" width="34" style="5" customWidth="1"/>
-    <col min="3" max="3" width="28.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32" style="5" customWidth="1"/>
     <col min="4" max="4" width="28.42578125" style="5"/>
     <col min="5" max="5" width="4.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.85546875" style="5" customWidth="1"/>
     <col min="7" max="7" width="22.28515625" style="5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="22.42578125" style="5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="25" style="5" bestFit="1" customWidth="1"/>
@@ -1288,51 +1282,51 @@
   <sheetData>
     <row r="1" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="G1" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="E1" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>63</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>64</v>
       </c>
       <c r="J1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="L1" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="M1" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="N1" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>1</v>
@@ -1344,34 +1338,34 @@
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
       <c r="G2" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="J2" s="7"/>
       <c r="K2" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L2" s="7" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="M2" s="7" t="s">
-        <v>232</v>
+        <v>220</v>
       </c>
       <c r="N2" s="10" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C3" s="7"/>
       <c r="D3" s="8" t="s">
@@ -1380,31 +1374,31 @@
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
       <c r="G3" s="7" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>220</v>
+        <v>210</v>
       </c>
       <c r="J3" s="7"/>
       <c r="K3" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="L3" s="7" t="s">
-        <v>220</v>
+        <v>210</v>
       </c>
       <c r="M3" s="7" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="N3" s="10" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>2</v>
@@ -1416,70 +1410,70 @@
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
       <c r="G4" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="J4" s="7"/>
       <c r="K4" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L4" s="7" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="M4" s="7" t="s">
-        <v>232</v>
+        <v>220</v>
       </c>
       <c r="N4" s="10" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>18</v>
       </c>
       <c r="C5" s="7"/>
       <c r="D5" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E5" s="6"/>
       <c r="F5" s="6"/>
       <c r="G5" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="J5" s="7"/>
       <c r="K5" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L5" s="7" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="M5" s="7" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="N5" s="10" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C6" s="7"/>
       <c r="D6" s="8" t="s">
@@ -1488,31 +1482,31 @@
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
       <c r="G6" s="7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>217</v>
+        <v>226</v>
       </c>
       <c r="J6" s="7"/>
       <c r="K6" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="L6" s="7" t="s">
-        <v>217</v>
+        <v>226</v>
       </c>
       <c r="M6" s="7" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="N6" s="10" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>3</v>
@@ -1524,31 +1518,31 @@
       <c r="E7" s="6"/>
       <c r="F7" s="6"/>
       <c r="G7" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="J7" s="7"/>
       <c r="K7" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L7" s="7" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="M7" s="7" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="N7" s="10" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>4</v>
@@ -1560,31 +1554,31 @@
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
       <c r="G8" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>221</v>
+        <v>227</v>
       </c>
       <c r="J8" s="7"/>
       <c r="K8" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="L8" s="7" t="s">
-        <v>221</v>
+        <v>227</v>
       </c>
       <c r="M8" s="7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="N8" s="10" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B9" s="7" t="s">
         <v>5</v>
@@ -1596,31 +1590,31 @@
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
       <c r="G9" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>219</v>
+        <v>228</v>
       </c>
       <c r="J9" s="7"/>
       <c r="K9" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="L9" s="7" t="s">
-        <v>219</v>
+        <v>228</v>
       </c>
       <c r="M9" s="7" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="N9" s="10" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B10" s="7" t="s">
         <v>6</v>
@@ -1632,31 +1626,31 @@
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
       <c r="G10" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I10" s="7" t="s">
-        <v>222</v>
+        <v>229</v>
       </c>
       <c r="J10" s="7"/>
       <c r="K10" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="L10" s="7" t="s">
-        <v>222</v>
+        <v>229</v>
       </c>
       <c r="M10" s="7" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="N10" s="10" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B11" s="7" t="s">
         <v>7</v>
@@ -1668,31 +1662,31 @@
       <c r="E11" s="6"/>
       <c r="F11" s="6"/>
       <c r="G11" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I11" s="7" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="J11" s="7"/>
       <c r="K11" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L11" s="7" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="M11" s="7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="N11" s="10" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="12" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B12" s="7" t="s">
         <v>8</v>
@@ -1704,31 +1698,31 @@
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
       <c r="G12" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H12" s="7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="I12" s="7" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="J12" s="7"/>
       <c r="K12" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L12" s="7" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="M12" s="7" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="N12" s="10" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="13" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B13" s="7" t="s">
         <v>9</v>
@@ -1740,31 +1734,31 @@
       <c r="E13" s="6"/>
       <c r="F13" s="6"/>
       <c r="G13" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H13" s="7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="I13" s="7" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="J13" s="7"/>
       <c r="K13" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L13" s="7" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="M13" s="7" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="N13" s="10" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="14" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B14" s="7" t="s">
         <v>10</v>
@@ -1776,31 +1770,31 @@
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
       <c r="G14" s="7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H14" s="7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="I14" s="7" t="s">
-        <v>220</v>
+        <v>210</v>
       </c>
       <c r="J14" s="7"/>
       <c r="K14" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="L14" s="7" t="s">
-        <v>220</v>
+        <v>210</v>
       </c>
       <c r="M14" s="7" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="N14" s="10" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="15" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B15" s="7" t="s">
         <v>11</v>
@@ -1812,31 +1806,31 @@
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
       <c r="G15" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H15" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="I15" s="7" t="s">
-        <v>221</v>
+        <v>227</v>
       </c>
       <c r="J15" s="7"/>
       <c r="K15" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="L15" s="7" t="s">
-        <v>221</v>
+        <v>227</v>
       </c>
       <c r="M15" s="7" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="N15" s="10" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="16" spans="1:14" ht="105" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B16" s="7" t="s">
         <v>13</v>
@@ -1848,295 +1842,295 @@
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
       <c r="G16" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H16" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I16" s="7" t="s">
-        <v>216</v>
+        <v>230</v>
       </c>
       <c r="J16" s="7"/>
       <c r="K16" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="L16" s="7" t="s">
-        <v>216</v>
+        <v>230</v>
       </c>
       <c r="M16" s="7" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="N16" s="10" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="17" spans="1:14" ht="75" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C17" s="7"/>
       <c r="D17" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E17" s="6"/>
       <c r="F17" s="6"/>
       <c r="G17" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H17" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="I17" s="7" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="J17" s="7"/>
       <c r="K17" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L17" s="7" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="M17" s="7" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="N17" s="10" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="18" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C18" s="7"/>
       <c r="D18" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E18" s="6"/>
       <c r="F18" s="6"/>
       <c r="G18" s="7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H18" s="7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I18" s="7" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="J18" s="7"/>
       <c r="K18" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L18" s="7" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="M18" s="7" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="N18" s="10" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="19" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C19" s="7"/>
       <c r="D19" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H19" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="I19" s="7" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="J19" s="7"/>
       <c r="K19" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L19" s="7" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="M19" s="7" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="N19" s="10" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="20" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="18" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C20" s="11"/>
       <c r="D20" s="9" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="7" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="H20" s="7" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="I20" s="7" t="s">
-        <v>220</v>
+        <v>210</v>
       </c>
       <c r="J20" s="7"/>
       <c r="K20" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="L20" s="7" t="s">
-        <v>220</v>
+        <v>210</v>
       </c>
       <c r="M20" s="7" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="N20" s="10" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="21" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E21" s="1">
         <v>22</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="I21" s="7" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="J21" s="1"/>
       <c r="K21" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L21" s="7" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="M21" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="N21" s="10" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="22" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C22" s="1"/>
       <c r="D22" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E22" s="1">
         <v>22</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="I22" s="7" t="s">
-        <v>217</v>
+        <v>226</v>
       </c>
       <c r="J22" s="1"/>
       <c r="K22" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="L22" s="7" t="s">
-        <v>217</v>
+        <v>226</v>
       </c>
       <c r="M22" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="N22" s="10" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="23" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C23" s="1"/>
       <c r="D23" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E23" s="1">
         <v>22</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="I23" s="7" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="J23" s="1"/>
       <c r="K23" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L23" s="7" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="M23" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="N23" s="10" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="24" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>16</v>
@@ -2149,614 +2143,608 @@
         <v>22</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="I24" s="7" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="J24" s="1"/>
       <c r="K24" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L24" s="7" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="M24" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="N24" s="10" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="25" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C25" s="1"/>
       <c r="D25" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E25" s="1">
         <v>22</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I25" s="7" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>228</v>
+        <v>216</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L25" s="7" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="M25" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="N25" s="10" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="26" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C26" s="1"/>
-      <c r="D26" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E26" s="1">
-        <v>22</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>49</v>
-      </c>
+      <c r="D26" s="19" t="s">
+        <v>225</v>
+      </c>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
       <c r="G26" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I26" s="7" t="s">
-        <v>220</v>
+        <v>210</v>
       </c>
       <c r="J26" s="1"/>
       <c r="K26" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="L26" s="7" t="s">
-        <v>220</v>
+        <v>210</v>
       </c>
       <c r="M26" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="N26" s="10" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="27" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
       <c r="G27" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="I27" s="7" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="J27" s="1" t="s">
         <v>30</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L27" s="7" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="M27" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="N27" s="1"/>
     </row>
     <row r="28" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
       <c r="G28" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I28" s="7" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="J28" s="1">
         <v>1234</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L28" s="7" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="M28" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="N28" s="1"/>
     </row>
     <row r="29" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>233</v>
+        <v>221</v>
       </c>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
       <c r="G29" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I29" s="7" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="J29" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K29" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L29" s="7" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="M29" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="N29" s="1"/>
     </row>
     <row r="30" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>205</v>
+        <v>222</v>
       </c>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
       <c r="G30" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="I30" s="7" t="s">
-        <v>217</v>
+        <v>226</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K30" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="L30" s="7" t="s">
-        <v>217</v>
+        <v>226</v>
       </c>
       <c r="M30" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="N30" s="1"/>
     </row>
     <row r="31" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>223</v>
+        <v>211</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
       <c r="F31" s="2"/>
       <c r="G31" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="I31" s="7" t="s">
-        <v>220</v>
+        <v>210</v>
       </c>
       <c r="J31" s="7" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="K31" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="L31" s="7" t="s">
-        <v>220</v>
+        <v>210</v>
       </c>
       <c r="M31" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="N31" s="1"/>
     </row>
     <row r="32" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>229</v>
+        <v>217</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>227</v>
+        <v>215</v>
       </c>
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
       <c r="F32" s="2"/>
       <c r="G32" s="1" t="s">
-        <v>230</v>
+        <v>218</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>231</v>
+        <v>219</v>
       </c>
       <c r="I32" s="7" t="s">
-        <v>220</v>
+        <v>210</v>
       </c>
       <c r="J32" s="17" t="s">
-        <v>225</v>
+        <v>213</v>
       </c>
       <c r="K32" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="L32" s="7" t="s">
-        <v>220</v>
+        <v>210</v>
       </c>
       <c r="M32" s="3" t="s">
-        <v>226</v>
+        <v>214</v>
       </c>
       <c r="N32" s="1"/>
     </row>
     <row r="33" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A33" s="16" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C33" s="1"/>
       <c r="D33" s="15" t="s">
-        <v>224</v>
+        <v>212</v>
       </c>
       <c r="E33" s="2"/>
       <c r="F33" s="2"/>
       <c r="G33" s="1" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="I33" s="7" t="s">
-        <v>220</v>
+        <v>210</v>
       </c>
       <c r="J33" s="1"/>
       <c r="K33" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="L33" s="7" t="s">
-        <v>220</v>
+        <v>210</v>
       </c>
       <c r="M33" s="3" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="N33" s="10" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="34" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" ht="60" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>24</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="D34" s="2"/>
       <c r="E34" s="2"/>
       <c r="F34" s="2"/>
       <c r="G34" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="I34" s="7" t="s">
-        <v>220</v>
+        <v>210</v>
       </c>
       <c r="J34" s="7" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="K34" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="L34" s="7" t="s">
-        <v>220</v>
+        <v>210</v>
       </c>
       <c r="M34" s="3" t="s">
-        <v>190</v>
+        <v>224</v>
       </c>
       <c r="N34" s="1"/>
     </row>
     <row r="35" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="D35" s="2"/>
       <c r="E35" s="2"/>
       <c r="F35" s="2"/>
       <c r="G35" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="I35" s="7" t="s">
-        <v>220</v>
+        <v>210</v>
       </c>
       <c r="J35" s="7" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="K35" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="L35" s="7" t="s">
-        <v>220</v>
+        <v>210</v>
       </c>
       <c r="M35" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="N35" s="1"/>
     </row>
     <row r="36" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
       <c r="F36" s="2"/>
       <c r="G36" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="I36" s="7" t="s">
-        <v>220</v>
+        <v>210</v>
       </c>
       <c r="J36" s="7" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="K36" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="L36" s="7" t="s">
-        <v>220</v>
+        <v>210</v>
       </c>
       <c r="M36" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="N36" s="1"/>
     </row>
     <row r="37" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>27</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>212</v>
+        <v>223</v>
       </c>
       <c r="D37" s="2"/>
       <c r="E37" s="2"/>
       <c r="F37" s="2"/>
       <c r="G37" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I37" s="7" t="s">
-        <v>217</v>
+        <v>226</v>
       </c>
       <c r="J37" s="1"/>
       <c r="K37" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="L37" s="7" t="s">
-        <v>217</v>
+        <v>226</v>
       </c>
       <c r="M37" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="N37" s="1"/>
     </row>
     <row r="38" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="D38" s="2"/>
       <c r="E38" s="2"/>
       <c r="F38" s="2"/>
       <c r="G38" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="I38" s="7" t="s">
-        <v>216</v>
+        <v>230</v>
       </c>
       <c r="J38" s="12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="K38" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="L38" s="7" t="s">
-        <v>216</v>
+        <v>230</v>
       </c>
       <c r="M38" s="7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="N38" s="1"/>
     </row>
-    <row r="39" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="D39" s="2"/>
       <c r="E39" s="2"/>
       <c r="F39" s="2"/>
       <c r="G39" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="I39" s="7" t="s">
-        <v>218</v>
+        <v>230</v>
       </c>
       <c r="J39" s="14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="K39" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="L39" s="7" t="s">
-        <v>218</v>
+        <v>230</v>
       </c>
       <c r="M39" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="N39" s="1"/>
     </row>
     <row r="40" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>29</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>214</v>
-      </c>
+        <v>209</v>
+      </c>
+      <c r="D40" s="2"/>
       <c r="E40" s="2"/>
       <c r="F40" s="2"/>
       <c r="G40" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I40" s="7" t="s">
-        <v>216</v>
+        <v>230</v>
       </c>
       <c r="J40" s="12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K40" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="L40" s="7" t="s">
-        <v>216</v>
+        <v>230</v>
       </c>
       <c r="M40" s="7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="N40" s="1"/>
     </row>
@@ -2778,8 +2766,8 @@
     <hyperlink ref="N3" r:id="rId11" xr:uid="{4E1DDD8D-774A-4073-81D6-BEDB3EFCD079}"/>
     <hyperlink ref="N4:N26" r:id="rId12" display="rrhamachandran@unionbankph.com" xr:uid="{0B09F3EC-2224-4918-843C-25097DD2A45B}"/>
     <hyperlink ref="N20" r:id="rId13" xr:uid="{AE271E2F-CCDD-4C24-9900-396BBF58413A}"/>
-    <hyperlink ref="D20" r:id="rId14" xr:uid="{CCBA97EB-AA4C-4510-8CF5-C3BEF6F5096A}"/>
-    <hyperlink ref="N33" r:id="rId15" xr:uid="{6E7A3F64-9C89-45CF-B813-F7656E9F4231}"/>
+    <hyperlink ref="N33" r:id="rId14" xr:uid="{6E7A3F64-9C89-45CF-B813-F7656E9F4231}"/>
+    <hyperlink ref="D20" r:id="rId15" xr:uid="{CCBA97EB-AA4C-4510-8CF5-C3BEF6F5096A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId16"/>

</xml_diff>

<commit_message>
Code Version 080520 23:30
</commit_message>
<xml_diff>
--- a/Prime_Job_Automation/Configuration/RuleFactory/Master Rule Factory.xlsx
+++ b/Prime_Job_Automation/Configuration/RuleFactory/Master Rule Factory.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\PJA\Prime_Job_Automation\Configuration\RuleFactory\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB83D2D6-0643-45BC-AD74-A7E562DD0377}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63B102DA-E2ED-4BA7-9994-337588FE4865}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" tabRatio="351" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$N$40</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$P$40</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +35,7 @@
     <author>Divakar Ragupathy</author>
   </authors>
   <commentList>
-    <comment ref="M2" authorId="0" shapeId="0" xr:uid="{39ACA343-E88B-4897-9561-9AAEBA9E2255}">
+    <comment ref="O2" authorId="0" shapeId="0" xr:uid="{39ACA343-E88B-4897-9561-9AAEBA9E2255}">
       <text>
         <r>
           <rPr>
@@ -48,7 +48,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M4" authorId="0" shapeId="0" xr:uid="{20C86102-3E0A-4364-A306-E92F2660C190}">
+    <comment ref="O4" authorId="0" shapeId="0" xr:uid="{20C86102-3E0A-4364-A306-E92F2660C190}">
       <text>
         <r>
           <rPr>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="233">
   <si>
     <t>Password</t>
   </si>
@@ -203,9 +203,6 @@
     <t>\\10.19.81.248\rpa\PMU\PCIDSS\Ovl Return File</t>
   </si>
   <si>
-    <t>/Sun/</t>
-  </si>
-  <si>
     <t>Port</t>
   </si>
   <si>
@@ -524,15 +521,6 @@
     <t>^UBP[2][0-9][a-lA-L][0-3][0-9].erf$|^UBP[2][0-9][a-lA-L][0-3][0-9].enr$|^UBP[2][0-9][a-lA-L][0-3][0-9].can$</t>
   </si>
   <si>
-    <t>^CCOD TMF INSTALLMENT [0-1][0-9][0-3][0-9][2][0-9].txt$|^CCOD TMF INSTALLMENT [0-1][0-9][0-3][0-9][2][0-9] revised.txt$</t>
-  </si>
-  <si>
-    <t>^CCOD TMF [0-1][0-9][0-3][0-9][2][0-9] re-enrollment.txt$</t>
-  </si>
-  <si>
-    <t>^CCOD TMF return check [0-1][0-9][0-3][0-9][2][0-9].txt$|^CCOD TMF return check [0-1][0-9][0-3][0-9][2][0-9] batch 2.txt$</t>
-  </si>
-  <si>
     <t>^REMEDIALAGENCYEXTRACTFILE_[2][0][2][0-9][0-1][0-9][0-3][0-9]_[2][0][2][0-9][0-1][0-9][0-3][0-9][0-2][0-9][0-5][0-9][0-5][0-9].txt$</t>
   </si>
   <si>
@@ -545,9 +533,6 @@
     <t>rrhamachandran@unionbankph.com</t>
   </si>
   <si>
-    <t>/Meralco Enrollment/</t>
-  </si>
-  <si>
     <t>Meralco Enrollment</t>
   </si>
   <si>
@@ -590,15 +575,6 @@
     <t>^LUM[0-9][0-9][0-1][0-9][2][0-9].txt$</t>
   </si>
   <si>
-    <t>/Meralco Billing/</t>
-  </si>
-  <si>
-    <t>/Smart/</t>
-  </si>
-  <si>
-    <t>/SM Files/</t>
-  </si>
-  <si>
     <t>TSYS_PJAUpload_Location</t>
   </si>
   <si>
@@ -710,9 +686,6 @@
     <t>ccod@mmddyy</t>
   </si>
   <si>
-    <t>^upload_installment[2][0-9][0-1][0-9][0-3][0-9]a.txt$|^upload _installment[2][0-9][0-1][0-9][0-3][0-9]b.txt$</t>
-  </si>
-  <si>
     <t>cosmostmffile</t>
   </si>
   <si>
@@ -740,9 +713,6 @@
     <t>cebupacific</t>
   </si>
   <si>
-    <t>^CCOD TMF [0-1][0-9][0-3][0-9][2][0-9].txt$|^CCOD TMF REVERSAL UPLOAD [0-1][0-9][0-3][0-9][2][0-9].txt$|^CCOD TMF REVERSALS [0-1][0-9][0-3][0-9][2][0-9] 1.txt$</t>
-  </si>
-  <si>
     <t>\\10.19.81.248\rpa\PMU\PCIDSS\PlayEveryday</t>
   </si>
   <si>
@@ -759,13 +729,49 @@
   </si>
   <si>
     <t>/prime/UBP_ubp/collector_incoming_files</t>
+  </si>
+  <si>
+    <t>^CCOD_[0-1][0-9][0-3][0-9][2][0][2][0-9]_[0-9].txt$|^CCOD_[0-1][0-9][0-3][0-9][2][0][2][0-9]_[0-9][0-9].txt$</t>
+  </si>
+  <si>
+    <t>^upload_installment[0-1][0-9][0-3][0-9][2][0-9][a-z].txt$</t>
+  </si>
+  <si>
+    <t>^reversal_[0-1][0-9][0-3][0-9][2][0][2][0-9]_[0-9].txt$|^reversal_[0-1][0-9][0-3][0-9][2][0][2][0-9]_[0-9][0-9].txt$</t>
+  </si>
+  <si>
+    <t>^return_[0-1][0-9][0-3][0-9][2][0][2][0-9]_[0-9].txt$|^return_[0-1][0-9][0-3][0-9][2][0][2][0-9]_[0-9][0-9].txt$</t>
+  </si>
+  <si>
+    <t>^reenrollment_[0-1][0-9][0-3][0-9][2][0][2][0-9]_[0-9].txt$|^reenrollment_[0-1][0-9][0-3][0-9][2][0][2][0-9]_[0-9][0-9].txt$</t>
+  </si>
+  <si>
+    <t>/ADA_Billing/</t>
+  </si>
+  <si>
+    <t>/ADA_Encan_Feedback/</t>
+  </si>
+  <si>
+    <t>/Billing/</t>
+  </si>
+  <si>
+    <t>/</t>
+  </si>
+  <si>
+    <t>SFTP_UserId</t>
+  </si>
+  <si>
+    <t>SFTP_Password</t>
+  </si>
+  <si>
+    <t>sashankar</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -812,6 +818,13 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -865,7 +878,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -917,6 +930,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1257,7 +1273,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N49"/>
+  <dimension ref="A1:P49"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
   </sheetViews>
@@ -1268,65 +1284,71 @@
     <col min="3" max="3" width="32" style="5" customWidth="1"/>
     <col min="4" max="4" width="28.42578125" style="5"/>
     <col min="5" max="5" width="4.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.85546875" style="5" customWidth="1"/>
-    <col min="7" max="7" width="22.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="25" style="5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.85546875" style="5" customWidth="1"/>
-    <col min="11" max="11" width="23.85546875" style="5" customWidth="1"/>
-    <col min="12" max="12" width="25" style="5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="44.140625" style="5" customWidth="1"/>
-    <col min="14" max="14" width="30" style="5" customWidth="1"/>
-    <col min="15" max="16384" width="9.140625" style="5"/>
+    <col min="6" max="8" width="14.85546875" style="5" customWidth="1"/>
+    <col min="9" max="9" width="22.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="25" style="5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.85546875" style="5" customWidth="1"/>
+    <col min="13" max="13" width="23.85546875" style="5" customWidth="1"/>
+    <col min="14" max="14" width="25" style="5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="44.140625" style="5" customWidth="1"/>
+    <col min="16" max="16" width="30" style="5" customWidth="1"/>
+    <col min="17" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="D1" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>231</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="O1" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>177</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="N1" s="4" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="P1" s="4" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>1</v>
@@ -1337,35 +1359,37 @@
       </c>
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
-      <c r="G2" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>105</v>
-      </c>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
       <c r="I2" s="7" t="s">
-        <v>178</v>
-      </c>
-      <c r="J2" s="7"/>
+        <v>73</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>104</v>
+      </c>
       <c r="K2" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="L2" s="7" t="s">
-        <v>210</v>
-      </c>
+        <v>170</v>
+      </c>
+      <c r="L2" s="7"/>
       <c r="M2" s="7" t="s">
-        <v>220</v>
-      </c>
-      <c r="N2" s="10" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+      <c r="N2" s="7" t="s">
+        <v>202</v>
+      </c>
+      <c r="O2" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="P2" s="10" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="C3" s="7"/>
       <c r="D3" s="8" t="s">
@@ -1373,32 +1397,34 @@
       </c>
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
-      <c r="G3" s="7" t="s">
-        <v>163</v>
-      </c>
-      <c r="H3" s="7" t="s">
-        <v>170</v>
-      </c>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
       <c r="I3" s="7" t="s">
-        <v>210</v>
-      </c>
-      <c r="J3" s="7"/>
+        <v>158</v>
+      </c>
+      <c r="J3" s="7" t="s">
+        <v>165</v>
+      </c>
       <c r="K3" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="L3" s="7" t="s">
-        <v>210</v>
-      </c>
+        <v>202</v>
+      </c>
+      <c r="L3" s="7"/>
       <c r="M3" s="7" t="s">
-        <v>182</v>
-      </c>
-      <c r="N3" s="10" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+      <c r="N3" s="7" t="s">
+        <v>202</v>
+      </c>
+      <c r="O3" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="P3" s="10" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>2</v>
@@ -1409,71 +1435,75 @@
       </c>
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
-      <c r="G4" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="H4" s="7" t="s">
-        <v>106</v>
-      </c>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
       <c r="I4" s="7" t="s">
-        <v>178</v>
-      </c>
-      <c r="J4" s="7"/>
+        <v>74</v>
+      </c>
+      <c r="J4" s="7" t="s">
+        <v>105</v>
+      </c>
       <c r="K4" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="L4" s="7" t="s">
-        <v>210</v>
-      </c>
+        <v>170</v>
+      </c>
+      <c r="L4" s="7"/>
       <c r="M4" s="7" t="s">
-        <v>220</v>
-      </c>
-      <c r="N4" s="10" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+      <c r="N4" s="7" t="s">
+        <v>202</v>
+      </c>
+      <c r="O4" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="P4" s="10" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>18</v>
       </c>
       <c r="C5" s="7"/>
       <c r="D5" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E5" s="6"/>
       <c r="F5" s="6"/>
-      <c r="G5" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="H5" s="7" t="s">
-        <v>107</v>
-      </c>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
       <c r="I5" s="7" t="s">
-        <v>179</v>
-      </c>
-      <c r="J5" s="7"/>
+        <v>75</v>
+      </c>
+      <c r="J5" s="7" t="s">
+        <v>106</v>
+      </c>
       <c r="K5" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="L5" s="7" t="s">
-        <v>210</v>
-      </c>
+        <v>171</v>
+      </c>
+      <c r="L5" s="7"/>
       <c r="M5" s="7" t="s">
-        <v>137</v>
-      </c>
-      <c r="N5" s="10" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+      <c r="N5" s="7" t="s">
+        <v>202</v>
+      </c>
+      <c r="O5" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="P5" s="10" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="C6" s="7"/>
       <c r="D6" s="8" t="s">
@@ -1481,32 +1511,34 @@
       </c>
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
-      <c r="G6" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="H6" s="7" t="s">
-        <v>171</v>
-      </c>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
       <c r="I6" s="7" t="s">
-        <v>226</v>
-      </c>
-      <c r="J6" s="7"/>
+        <v>159</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>166</v>
+      </c>
       <c r="K6" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="L6" s="7" t="s">
-        <v>226</v>
-      </c>
+        <v>216</v>
+      </c>
+      <c r="L6" s="7"/>
       <c r="M6" s="7" t="s">
-        <v>183</v>
-      </c>
-      <c r="N6" s="10" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+      <c r="N6" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="O6" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="P6" s="10" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>3</v>
@@ -1517,32 +1549,34 @@
       </c>
       <c r="E7" s="6"/>
       <c r="F7" s="6"/>
-      <c r="G7" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="H7" s="7" t="s">
-        <v>108</v>
-      </c>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
       <c r="I7" s="7" t="s">
-        <v>179</v>
-      </c>
-      <c r="J7" s="7"/>
+        <v>76</v>
+      </c>
+      <c r="J7" s="7" t="s">
+        <v>107</v>
+      </c>
       <c r="K7" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="L7" s="7" t="s">
-        <v>210</v>
-      </c>
+        <v>171</v>
+      </c>
+      <c r="L7" s="7"/>
       <c r="M7" s="7" t="s">
-        <v>184</v>
-      </c>
-      <c r="N7" s="10" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+      <c r="N7" s="7" t="s">
+        <v>202</v>
+      </c>
+      <c r="O7" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="P7" s="10" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>4</v>
@@ -1553,32 +1587,34 @@
       </c>
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
-      <c r="G8" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="H8" s="7" t="s">
-        <v>109</v>
-      </c>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
       <c r="I8" s="7" t="s">
-        <v>227</v>
-      </c>
-      <c r="J8" s="7"/>
+        <v>77</v>
+      </c>
+      <c r="J8" s="7" t="s">
+        <v>108</v>
+      </c>
       <c r="K8" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="L8" s="7" t="s">
-        <v>227</v>
-      </c>
+        <v>217</v>
+      </c>
+      <c r="L8" s="7"/>
       <c r="M8" s="7" t="s">
-        <v>138</v>
-      </c>
-      <c r="N8" s="10" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+      <c r="N8" s="7" t="s">
+        <v>217</v>
+      </c>
+      <c r="O8" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="P8" s="10" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B9" s="7" t="s">
         <v>5</v>
@@ -1589,32 +1625,34 @@
       </c>
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
-      <c r="G9" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="H9" s="7" t="s">
-        <v>110</v>
-      </c>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
       <c r="I9" s="7" t="s">
-        <v>228</v>
-      </c>
-      <c r="J9" s="7"/>
+        <v>78</v>
+      </c>
+      <c r="J9" s="7" t="s">
+        <v>109</v>
+      </c>
       <c r="K9" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="L9" s="7" t="s">
-        <v>228</v>
-      </c>
+        <v>218</v>
+      </c>
+      <c r="L9" s="7"/>
       <c r="M9" s="7" t="s">
-        <v>185</v>
-      </c>
-      <c r="N9" s="10" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+      <c r="N9" s="7" t="s">
+        <v>218</v>
+      </c>
+      <c r="O9" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="P9" s="10" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B10" s="7" t="s">
         <v>6</v>
@@ -1625,32 +1663,34 @@
       </c>
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
-      <c r="G10" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="H10" s="7" t="s">
-        <v>111</v>
-      </c>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
       <c r="I10" s="7" t="s">
-        <v>229</v>
-      </c>
-      <c r="J10" s="7"/>
+        <v>79</v>
+      </c>
+      <c r="J10" s="7" t="s">
+        <v>110</v>
+      </c>
       <c r="K10" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="L10" s="7" t="s">
-        <v>229</v>
-      </c>
+        <v>219</v>
+      </c>
+      <c r="L10" s="7"/>
       <c r="M10" s="7" t="s">
-        <v>186</v>
-      </c>
-      <c r="N10" s="10" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+      <c r="N10" s="7" t="s">
+        <v>219</v>
+      </c>
+      <c r="O10" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="P10" s="10" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B11" s="7" t="s">
         <v>7</v>
@@ -1661,32 +1701,34 @@
       </c>
       <c r="E11" s="6"/>
       <c r="F11" s="6"/>
-      <c r="G11" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="H11" s="7" t="s">
-        <v>112</v>
-      </c>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
       <c r="I11" s="7" t="s">
-        <v>179</v>
-      </c>
-      <c r="J11" s="7"/>
+        <v>80</v>
+      </c>
+      <c r="J11" s="7" t="s">
+        <v>111</v>
+      </c>
       <c r="K11" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="L11" s="7" t="s">
-        <v>210</v>
-      </c>
+        <v>171</v>
+      </c>
+      <c r="L11" s="7"/>
       <c r="M11" s="7" t="s">
-        <v>139</v>
-      </c>
-      <c r="N11" s="10" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+      <c r="N11" s="7" t="s">
+        <v>202</v>
+      </c>
+      <c r="O11" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="P11" s="10" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B12" s="7" t="s">
         <v>8</v>
@@ -1697,32 +1739,34 @@
       </c>
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
-      <c r="G12" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="H12" s="7" t="s">
-        <v>113</v>
-      </c>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
       <c r="I12" s="7" t="s">
-        <v>179</v>
-      </c>
-      <c r="J12" s="7"/>
+        <v>81</v>
+      </c>
+      <c r="J12" s="7" t="s">
+        <v>112</v>
+      </c>
       <c r="K12" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="L12" s="7" t="s">
-        <v>210</v>
-      </c>
+        <v>171</v>
+      </c>
+      <c r="L12" s="7"/>
       <c r="M12" s="7" t="s">
-        <v>140</v>
-      </c>
-      <c r="N12" s="10" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+      <c r="N12" s="7" t="s">
+        <v>202</v>
+      </c>
+      <c r="O12" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="P12" s="10" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B13" s="7" t="s">
         <v>9</v>
@@ -1733,32 +1777,34 @@
       </c>
       <c r="E13" s="6"/>
       <c r="F13" s="6"/>
-      <c r="G13" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="H13" s="7" t="s">
-        <v>114</v>
-      </c>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
       <c r="I13" s="7" t="s">
-        <v>179</v>
-      </c>
-      <c r="J13" s="7"/>
+        <v>82</v>
+      </c>
+      <c r="J13" s="7" t="s">
+        <v>113</v>
+      </c>
       <c r="K13" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="L13" s="7" t="s">
-        <v>210</v>
-      </c>
+        <v>171</v>
+      </c>
+      <c r="L13" s="7"/>
       <c r="M13" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="N13" s="10" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+      <c r="N13" s="7" t="s">
+        <v>202</v>
+      </c>
+      <c r="O13" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="P13" s="10" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B14" s="7" t="s">
         <v>10</v>
@@ -1769,32 +1815,34 @@
       </c>
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
-      <c r="G14" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="H14" s="7" t="s">
-        <v>115</v>
-      </c>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
       <c r="I14" s="7" t="s">
-        <v>210</v>
-      </c>
-      <c r="J14" s="7"/>
+        <v>83</v>
+      </c>
+      <c r="J14" s="7" t="s">
+        <v>114</v>
+      </c>
       <c r="K14" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="L14" s="7" t="s">
-        <v>210</v>
-      </c>
+        <v>202</v>
+      </c>
+      <c r="L14" s="7"/>
       <c r="M14" s="7" t="s">
-        <v>188</v>
-      </c>
-      <c r="N14" s="10" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+      <c r="N14" s="7" t="s">
+        <v>202</v>
+      </c>
+      <c r="O14" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="P14" s="10" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B15" s="7" t="s">
         <v>11</v>
@@ -1805,32 +1853,34 @@
       </c>
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
-      <c r="G15" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="H15" s="7" t="s">
-        <v>116</v>
-      </c>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
       <c r="I15" s="7" t="s">
-        <v>227</v>
-      </c>
-      <c r="J15" s="7"/>
+        <v>84</v>
+      </c>
+      <c r="J15" s="7" t="s">
+        <v>115</v>
+      </c>
       <c r="K15" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="L15" s="7" t="s">
-        <v>227</v>
-      </c>
+        <v>217</v>
+      </c>
+      <c r="L15" s="7"/>
       <c r="M15" s="7" t="s">
-        <v>142</v>
-      </c>
-      <c r="N15" s="10" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" ht="105" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+      <c r="N15" s="7" t="s">
+        <v>217</v>
+      </c>
+      <c r="O15" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="P15" s="10" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" ht="105" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B16" s="7" t="s">
         <v>13</v>
@@ -1841,912 +1891,982 @@
       </c>
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
-      <c r="G16" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="H16" s="7" t="s">
-        <v>117</v>
-      </c>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
       <c r="I16" s="7" t="s">
-        <v>230</v>
-      </c>
-      <c r="J16" s="7"/>
+        <v>85</v>
+      </c>
+      <c r="J16" s="7" t="s">
+        <v>116</v>
+      </c>
       <c r="K16" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="L16" s="7" t="s">
-        <v>230</v>
-      </c>
+        <v>220</v>
+      </c>
+      <c r="L16" s="7"/>
       <c r="M16" s="7" t="s">
-        <v>190</v>
-      </c>
-      <c r="N16" s="10" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" ht="75" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+      <c r="N16" s="7" t="s">
+        <v>220</v>
+      </c>
+      <c r="O16" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="P16" s="10" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" ht="75" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C17" s="7"/>
       <c r="D17" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E17" s="6"/>
       <c r="F17" s="6"/>
-      <c r="G17" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="H17" s="7" t="s">
-        <v>118</v>
-      </c>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
       <c r="I17" s="7" t="s">
-        <v>178</v>
-      </c>
-      <c r="J17" s="7"/>
+        <v>86</v>
+      </c>
+      <c r="J17" s="7" t="s">
+        <v>117</v>
+      </c>
       <c r="K17" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="L17" s="7" t="s">
-        <v>210</v>
-      </c>
+        <v>170</v>
+      </c>
+      <c r="L17" s="7"/>
       <c r="M17" s="7" t="s">
-        <v>181</v>
-      </c>
-      <c r="N17" s="10" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+      <c r="N17" s="7" t="s">
+        <v>202</v>
+      </c>
+      <c r="O17" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="P17" s="10" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C18" s="7"/>
       <c r="D18" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E18" s="6"/>
       <c r="F18" s="6"/>
-      <c r="G18" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="H18" s="7" t="s">
-        <v>119</v>
-      </c>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
       <c r="I18" s="7" t="s">
-        <v>179</v>
-      </c>
-      <c r="J18" s="7"/>
+        <v>87</v>
+      </c>
+      <c r="J18" s="7" t="s">
+        <v>118</v>
+      </c>
       <c r="K18" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="L18" s="7" t="s">
-        <v>210</v>
-      </c>
+        <v>171</v>
+      </c>
+      <c r="L18" s="7"/>
       <c r="M18" s="7" t="s">
-        <v>143</v>
-      </c>
-      <c r="N18" s="10" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+      <c r="N18" s="7" t="s">
+        <v>202</v>
+      </c>
+      <c r="O18" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="P18" s="10" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C19" s="7"/>
       <c r="D19" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
-      <c r="G19" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="H19" s="7" t="s">
-        <v>120</v>
-      </c>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
       <c r="I19" s="7" t="s">
-        <v>179</v>
-      </c>
-      <c r="J19" s="7"/>
+        <v>88</v>
+      </c>
+      <c r="J19" s="7" t="s">
+        <v>119</v>
+      </c>
       <c r="K19" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="L19" s="7" t="s">
-        <v>210</v>
-      </c>
+        <v>171</v>
+      </c>
+      <c r="L19" s="7"/>
       <c r="M19" s="7" t="s">
-        <v>144</v>
-      </c>
-      <c r="N19" s="10" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+      <c r="N19" s="7" t="s">
+        <v>202</v>
+      </c>
+      <c r="O19" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="P19" s="10" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="18" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
       <c r="C20" s="11"/>
       <c r="D20" s="9" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
-      <c r="G20" s="7" t="s">
-        <v>197</v>
-      </c>
-      <c r="H20" s="7" t="s">
-        <v>198</v>
-      </c>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
       <c r="I20" s="7" t="s">
-        <v>210</v>
-      </c>
-      <c r="J20" s="7"/>
+        <v>189</v>
+      </c>
+      <c r="J20" s="7" t="s">
+        <v>190</v>
+      </c>
       <c r="K20" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="L20" s="7" t="s">
-        <v>210</v>
-      </c>
+        <v>202</v>
+      </c>
+      <c r="L20" s="7"/>
       <c r="M20" s="7" t="s">
-        <v>199</v>
-      </c>
-      <c r="N20" s="10" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+      <c r="N20" s="7" t="s">
+        <v>202</v>
+      </c>
+      <c r="O20" s="7" t="s">
+        <v>191</v>
+      </c>
+      <c r="P20" s="10" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="1" t="s">
-        <v>174</v>
+        <v>226</v>
       </c>
       <c r="E21" s="1">
         <v>22</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="I21" s="7" t="s">
-        <v>178</v>
-      </c>
-      <c r="J21" s="1"/>
-      <c r="K21" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="L21" s="7" t="s">
-        <v>210</v>
-      </c>
+        <v>232</v>
+      </c>
+      <c r="H21" s="20" t="s">
+        <v>232</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="K21" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="L21" s="1"/>
       <c r="M21" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="N21" s="10" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+      <c r="N21" s="7" t="s">
+        <v>202</v>
+      </c>
+      <c r="O21" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="P21" s="10" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="C22" s="1"/>
       <c r="D22" s="1" t="s">
-        <v>159</v>
+        <v>227</v>
       </c>
       <c r="E22" s="1">
         <v>22</v>
       </c>
       <c r="F22" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="H22" s="20" t="s">
+        <v>232</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="K22" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="L22" s="1"/>
+      <c r="M22" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="G22" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="H22" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="I22" s="7" t="s">
-        <v>226</v>
-      </c>
-      <c r="J22" s="1"/>
-      <c r="K22" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="L22" s="7" t="s">
-        <v>226</v>
-      </c>
-      <c r="M22" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="N22" s="10" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="N22" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="O22" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="P22" s="10" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C23" s="1"/>
       <c r="D23" s="1" t="s">
-        <v>175</v>
+        <v>228</v>
       </c>
       <c r="E23" s="1">
         <v>22</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="H23" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="I23" s="7" t="s">
-        <v>178</v>
-      </c>
-      <c r="J23" s="1"/>
-      <c r="K23" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="L23" s="7" t="s">
-        <v>210</v>
-      </c>
+        <v>232</v>
+      </c>
+      <c r="H23" s="20" t="s">
+        <v>232</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="K23" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="L23" s="1"/>
       <c r="M23" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="N23" s="10" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+      <c r="N23" s="7" t="s">
+        <v>202</v>
+      </c>
+      <c r="O23" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="P23" s="10" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C24" s="1"/>
       <c r="D24" s="1" t="s">
-        <v>45</v>
+        <v>228</v>
       </c>
       <c r="E24" s="1">
         <v>22</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="H24" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="I24" s="7" t="s">
-        <v>178</v>
-      </c>
-      <c r="J24" s="1"/>
-      <c r="K24" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="L24" s="7" t="s">
-        <v>210</v>
-      </c>
+        <v>232</v>
+      </c>
+      <c r="H24" s="20" t="s">
+        <v>232</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J24" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="K24" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="L24" s="1"/>
       <c r="M24" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="N24" s="10" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+      <c r="N24" s="7" t="s">
+        <v>202</v>
+      </c>
+      <c r="O24" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="P24" s="10" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C25" s="1"/>
       <c r="D25" s="1" t="s">
-        <v>176</v>
+        <v>229</v>
       </c>
       <c r="E25" s="1">
         <v>22</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="H25" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="I25" s="7" t="s">
+        <v>232</v>
+      </c>
+      <c r="H25" s="20" t="s">
+        <v>232</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="K25" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="L25" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="M25" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="N25" s="7" t="s">
+        <v>202</v>
+      </c>
+      <c r="O25" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="J25" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="K25" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="L25" s="7" t="s">
-        <v>210</v>
-      </c>
-      <c r="M25" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="N25" s="10" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="P25" s="10" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C26" s="1"/>
       <c r="D26" s="19" t="s">
-        <v>225</v>
+        <v>215</v>
       </c>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
-      <c r="G26" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="H26" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="I26" s="7" t="s">
-        <v>210</v>
-      </c>
-      <c r="J26" s="1"/>
-      <c r="K26" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="L26" s="7" t="s">
-        <v>210</v>
-      </c>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="J26" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="K26" s="7" t="s">
+        <v>202</v>
+      </c>
+      <c r="L26" s="1"/>
       <c r="M26" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="N26" s="10" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+      <c r="N26" s="7" t="s">
+        <v>202</v>
+      </c>
+      <c r="O26" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="P26" s="10" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
-      <c r="G27" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="H27" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="I27" s="7" t="s">
-        <v>178</v>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2"/>
+      <c r="I27" s="1" t="s">
+        <v>94</v>
       </c>
       <c r="J27" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="K27" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="L27" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="K27" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="L27" s="7" t="s">
-        <v>210</v>
-      </c>
       <c r="M27" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="N27" s="1"/>
-    </row>
-    <row r="28" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+      <c r="N27" s="7" t="s">
+        <v>202</v>
+      </c>
+      <c r="O27" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="P27" s="1"/>
+    </row>
+    <row r="28" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
-      <c r="G28" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="H28" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="I28" s="7" t="s">
-        <v>178</v>
-      </c>
-      <c r="J28" s="1">
+      <c r="G28" s="2"/>
+      <c r="H28" s="2"/>
+      <c r="I28" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="J28" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="K28" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="L28" s="1">
         <v>1234</v>
       </c>
-      <c r="K28" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="L28" s="7" t="s">
-        <v>210</v>
-      </c>
       <c r="M28" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="N28" s="1"/>
-    </row>
-    <row r="29" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+      <c r="N28" s="7" t="s">
+        <v>202</v>
+      </c>
+      <c r="O28" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="P28" s="1"/>
+    </row>
+    <row r="29" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
-      <c r="G29" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="H29" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="I29" s="7" t="s">
-        <v>178</v>
+      <c r="G29" s="2"/>
+      <c r="H29" s="2"/>
+      <c r="I29" s="1" t="s">
+        <v>96</v>
       </c>
       <c r="J29" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="K29" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="K29" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="L29" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="L29" s="7" t="s">
-        <v>210</v>
-      </c>
       <c r="M29" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="N29" s="1"/>
-    </row>
-    <row r="30" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+      <c r="N29" s="7" t="s">
+        <v>202</v>
+      </c>
+      <c r="O29" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="P29" s="1"/>
+    </row>
+    <row r="30" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
-      <c r="G30" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="H30" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="I30" s="7" t="s">
-        <v>226</v>
+      <c r="G30" s="2"/>
+      <c r="H30" s="2"/>
+      <c r="I30" s="1" t="s">
+        <v>161</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="K30" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="L30" s="7" t="s">
-        <v>226</v>
+        <v>163</v>
+      </c>
+      <c r="K30" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="L30" s="1" t="s">
+        <v>51</v>
       </c>
       <c r="M30" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="N30" s="1"/>
-    </row>
-    <row r="31" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+      <c r="N30" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="O30" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="P30" s="1"/>
+    </row>
+    <row r="31" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
       <c r="F31" s="2"/>
-      <c r="G31" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="H31" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="I31" s="7" t="s">
-        <v>210</v>
-      </c>
-      <c r="J31" s="7" t="s">
-        <v>200</v>
-      </c>
-      <c r="K31" s="1" t="s">
-        <v>49</v>
+      <c r="G31" s="2"/>
+      <c r="H31" s="2"/>
+      <c r="I31" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="J31" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="K31" s="7" t="s">
+        <v>202</v>
       </c>
       <c r="L31" s="7" t="s">
-        <v>210</v>
-      </c>
-      <c r="M31" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="N31" s="1"/>
-    </row>
-    <row r="32" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+        <v>192</v>
+      </c>
+      <c r="M31" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="N31" s="7" t="s">
+        <v>202</v>
+      </c>
+      <c r="O31" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="P31" s="1"/>
+    </row>
+    <row r="32" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>217</v>
+        <v>208</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
       <c r="F32" s="2"/>
-      <c r="G32" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="H32" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="I32" s="7" t="s">
+      <c r="G32" s="2"/>
+      <c r="H32" s="2"/>
+      <c r="I32" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="J32" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="J32" s="17" t="s">
-        <v>213</v>
-      </c>
-      <c r="K32" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="L32" s="7" t="s">
-        <v>210</v>
-      </c>
-      <c r="M32" s="3" t="s">
-        <v>214</v>
-      </c>
-      <c r="N32" s="1"/>
-    </row>
-    <row r="33" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+      <c r="K32" s="7" t="s">
+        <v>202</v>
+      </c>
+      <c r="L32" s="17" t="s">
+        <v>205</v>
+      </c>
+      <c r="M32" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="N32" s="7" t="s">
+        <v>202</v>
+      </c>
+      <c r="O32" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="P32" s="1"/>
+    </row>
+    <row r="33" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A33" s="16" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="C33" s="1"/>
       <c r="D33" s="15" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="E33" s="2"/>
       <c r="F33" s="2"/>
-      <c r="G33" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="H33" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="I33" s="7" t="s">
-        <v>210</v>
-      </c>
-      <c r="J33" s="1"/>
-      <c r="K33" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="L33" s="7" t="s">
-        <v>210</v>
-      </c>
-      <c r="M33" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="N33" s="10" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="34" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+      <c r="G33" s="2"/>
+      <c r="H33" s="2"/>
+      <c r="I33" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="J33" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="K33" s="7" t="s">
+        <v>202</v>
+      </c>
+      <c r="L33" s="1"/>
+      <c r="M33" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="N33" s="7" t="s">
+        <v>202</v>
+      </c>
+      <c r="O33" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="P33" s="10" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>24</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="D34" s="2"/>
       <c r="E34" s="2"/>
       <c r="F34" s="2"/>
-      <c r="G34" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="H34" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="I34" s="7" t="s">
-        <v>210</v>
-      </c>
-      <c r="J34" s="7" t="s">
-        <v>200</v>
-      </c>
-      <c r="K34" s="1" t="s">
-        <v>49</v>
+      <c r="G34" s="2"/>
+      <c r="H34" s="2"/>
+      <c r="I34" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="J34" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="K34" s="7" t="s">
+        <v>202</v>
       </c>
       <c r="L34" s="7" t="s">
-        <v>210</v>
-      </c>
-      <c r="M34" s="3" t="s">
-        <v>224</v>
-      </c>
-      <c r="N34" s="1"/>
-    </row>
-    <row r="35" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+        <v>192</v>
+      </c>
+      <c r="M34" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="N34" s="7" t="s">
+        <v>202</v>
+      </c>
+      <c r="O34" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="P34" s="1"/>
+    </row>
+    <row r="35" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
       <c r="D35" s="2"/>
       <c r="E35" s="2"/>
       <c r="F35" s="2"/>
-      <c r="G35" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="H35" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="I35" s="7" t="s">
-        <v>210</v>
-      </c>
-      <c r="J35" s="7" t="s">
-        <v>200</v>
-      </c>
-      <c r="K35" s="1" t="s">
-        <v>49</v>
+      <c r="G35" s="2"/>
+      <c r="H35" s="2"/>
+      <c r="I35" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="J35" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="K35" s="7" t="s">
+        <v>202</v>
       </c>
       <c r="L35" s="7" t="s">
-        <v>210</v>
-      </c>
-      <c r="M35" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="N35" s="1"/>
-    </row>
-    <row r="36" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+        <v>192</v>
+      </c>
+      <c r="M35" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="N35" s="7" t="s">
+        <v>202</v>
+      </c>
+      <c r="O35" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="P35" s="1"/>
+    </row>
+    <row r="36" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
       <c r="F36" s="2"/>
-      <c r="G36" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="H36" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="I36" s="7" t="s">
-        <v>210</v>
-      </c>
-      <c r="J36" s="7" t="s">
-        <v>200</v>
-      </c>
-      <c r="K36" s="1" t="s">
-        <v>49</v>
+      <c r="G36" s="2"/>
+      <c r="H36" s="2"/>
+      <c r="I36" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="J36" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="K36" s="7" t="s">
+        <v>202</v>
       </c>
       <c r="L36" s="7" t="s">
-        <v>210</v>
-      </c>
-      <c r="M36" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="N36" s="1"/>
-    </row>
-    <row r="37" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+        <v>192</v>
+      </c>
+      <c r="M36" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="N36" s="7" t="s">
+        <v>202</v>
+      </c>
+      <c r="O36" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="P36" s="1"/>
+    </row>
+    <row r="37" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>27</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="D37" s="2"/>
       <c r="E37" s="2"/>
       <c r="F37" s="2"/>
-      <c r="G37" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="H37" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="I37" s="7" t="s">
-        <v>226</v>
-      </c>
-      <c r="J37" s="1"/>
-      <c r="K37" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="L37" s="7" t="s">
-        <v>226</v>
-      </c>
+      <c r="G37" s="2"/>
+      <c r="H37" s="2"/>
+      <c r="I37" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="J37" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="K37" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="L37" s="1"/>
       <c r="M37" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="N37" s="1"/>
-    </row>
-    <row r="38" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+      <c r="N37" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="O37" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="P37" s="1"/>
+    </row>
+    <row r="38" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
       <c r="D38" s="2"/>
       <c r="E38" s="2"/>
       <c r="F38" s="2"/>
-      <c r="G38" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="H38" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="I38" s="7" t="s">
-        <v>230</v>
-      </c>
-      <c r="J38" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="K38" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="L38" s="7" t="s">
-        <v>230</v>
-      </c>
-      <c r="M38" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="N38" s="1"/>
-    </row>
-    <row r="39" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="G38" s="2"/>
+      <c r="H38" s="2"/>
+      <c r="I38" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="J38" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="K38" s="7" t="s">
+        <v>220</v>
+      </c>
+      <c r="L38" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="M38" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="N38" s="7" t="s">
+        <v>220</v>
+      </c>
+      <c r="O38" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="P38" s="1"/>
+    </row>
+    <row r="39" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="D39" s="2"/>
       <c r="E39" s="2"/>
       <c r="F39" s="2"/>
-      <c r="G39" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="H39" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="I39" s="7" t="s">
-        <v>230</v>
-      </c>
-      <c r="J39" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="K39" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="L39" s="7" t="s">
-        <v>230</v>
+      <c r="G39" s="2"/>
+      <c r="H39" s="2"/>
+      <c r="I39" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="J39" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="K39" s="7" t="s">
+        <v>220</v>
+      </c>
+      <c r="L39" s="14" t="s">
+        <v>53</v>
       </c>
       <c r="M39" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="N39" s="1"/>
-    </row>
-    <row r="40" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+      <c r="N39" s="7" t="s">
+        <v>220</v>
+      </c>
+      <c r="O39" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="P39" s="1"/>
+    </row>
+    <row r="40" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>29</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="D40" s="2"/>
       <c r="E40" s="2"/>
       <c r="F40" s="2"/>
-      <c r="G40" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="H40" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="I40" s="7" t="s">
-        <v>230</v>
-      </c>
-      <c r="J40" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="K40" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="L40" s="7" t="s">
-        <v>230</v>
-      </c>
-      <c r="M40" s="7" t="s">
-        <v>156</v>
-      </c>
-      <c r="N40" s="1"/>
+      <c r="G40" s="2"/>
+      <c r="H40" s="2"/>
+      <c r="I40" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="J40" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="K40" s="7" t="s">
+        <v>220</v>
+      </c>
+      <c r="L40" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="M40" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="N40" s="7" t="s">
+        <v>220</v>
+      </c>
+      <c r="O40" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="P40" s="1"/>
     </row>
     <row r="49" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C49" s="13"/>
@@ -2762,11 +2882,11 @@
     <hyperlink ref="D4" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
     <hyperlink ref="D6" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
     <hyperlink ref="D5" r:id="rId9" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="N2" r:id="rId10" xr:uid="{385C1F08-1E02-4F73-8B01-D02F0B619B84}"/>
-    <hyperlink ref="N3" r:id="rId11" xr:uid="{4E1DDD8D-774A-4073-81D6-BEDB3EFCD079}"/>
-    <hyperlink ref="N4:N26" r:id="rId12" display="rrhamachandran@unionbankph.com" xr:uid="{0B09F3EC-2224-4918-843C-25097DD2A45B}"/>
-    <hyperlink ref="N20" r:id="rId13" xr:uid="{AE271E2F-CCDD-4C24-9900-396BBF58413A}"/>
-    <hyperlink ref="N33" r:id="rId14" xr:uid="{6E7A3F64-9C89-45CF-B813-F7656E9F4231}"/>
+    <hyperlink ref="P2" r:id="rId10" xr:uid="{385C1F08-1E02-4F73-8B01-D02F0B619B84}"/>
+    <hyperlink ref="P3" r:id="rId11" xr:uid="{4E1DDD8D-774A-4073-81D6-BEDB3EFCD079}"/>
+    <hyperlink ref="P4:P26" r:id="rId12" display="rrhamachandran@unionbankph.com" xr:uid="{0B09F3EC-2224-4918-843C-25097DD2A45B}"/>
+    <hyperlink ref="P20" r:id="rId13" xr:uid="{AE271E2F-CCDD-4C24-9900-396BBF58413A}"/>
+    <hyperlink ref="P33" r:id="rId14" xr:uid="{6E7A3F64-9C89-45CF-B813-F7656E9F4231}"/>
     <hyperlink ref="D20" r:id="rId15" xr:uid="{CCBA97EB-AA4C-4510-8CF5-C3BEF6F5096A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Stage 2 Code Version 110520 22:30
</commit_message>
<xml_diff>
--- a/Prime_Job_Automation/Configuration/RuleFactory/Master Rule Factory.xlsx
+++ b/Prime_Job_Automation/Configuration/RuleFactory/Master Rule Factory.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\PJA\Prime_Job_Automation\Configuration\RuleFactory\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63B102DA-E2ED-4BA7-9994-337588FE4865}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49374323-6DBE-4DBB-89E2-D23E3E34608F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" tabRatio="351" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="234">
   <si>
     <t>Password</t>
   </si>
@@ -752,9 +752,6 @@
     <t>/ADA_Encan_Feedback/</t>
   </si>
   <si>
-    <t>/Billing/</t>
-  </si>
-  <si>
     <t>/</t>
   </si>
   <si>
@@ -765,6 +762,12 @@
   </si>
   <si>
     <t>sashankar</t>
+  </si>
+  <si>
+    <t>/Sun/Billing/</t>
+  </si>
+  <si>
+    <t>/Smart/Billing/</t>
   </si>
 </sst>
 </file>
@@ -1316,10 +1319,10 @@
         <v>46</v>
       </c>
       <c r="G1" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="H1" s="4" t="s">
         <v>230</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>231</v>
       </c>
       <c r="I1" s="4" t="s">
         <v>60</v>
@@ -2086,10 +2089,10 @@
         <v>47</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="H21" s="20" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="I21" s="1" t="s">
         <v>89</v>
@@ -2132,10 +2135,10 @@
         <v>47</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="H22" s="20" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="I22" s="1" t="s">
         <v>160</v>
@@ -2169,7 +2172,7 @@
       </c>
       <c r="C23" s="1"/>
       <c r="D23" s="1" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="E23" s="1">
         <v>22</v>
@@ -2178,10 +2181,10 @@
         <v>47</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="H23" s="20" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="I23" s="1" t="s">
         <v>90</v>
@@ -2215,7 +2218,7 @@
       </c>
       <c r="C24" s="1"/>
       <c r="D24" s="1" t="s">
-        <v>228</v>
+        <v>233</v>
       </c>
       <c r="E24" s="1">
         <v>22</v>
@@ -2224,10 +2227,10 @@
         <v>47</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="H24" s="20" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="I24" s="1" t="s">
         <v>91</v>
@@ -2261,7 +2264,7 @@
       </c>
       <c r="C25" s="1"/>
       <c r="D25" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E25" s="1">
         <v>22</v>
@@ -2270,10 +2273,10 @@
         <v>47</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="H25" s="20" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="I25" s="1" t="s">
         <v>92</v>

</xml_diff>

<commit_message>
Code Version 14052020 21:55
</commit_message>
<xml_diff>
--- a/Prime_Job_Automation/Configuration/RuleFactory/Master Rule Factory.xlsx
+++ b/Prime_Job_Automation/Configuration/RuleFactory/Master Rule Factory.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\PJA\Prime_Job_Automation\Configuration\RuleFactory\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0B65008-6EB2-4F80-9BD0-2F1F160625E7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4289EA25-98C4-492D-8B6C-337F7A4FC734}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" tabRatio="351" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="235">
   <si>
     <t>Password</t>
   </si>
@@ -494,9 +494,6 @@
     <t>^newtogetgoGG[2][0][2][0-9][0-1][0-9][0-3][0-9].xml$|^newtogetgoGGP[2][0][2][0-9][0-1][0-9][0-3][0-9].xml$</t>
   </si>
   <si>
-    <t>^visaB[a-lA-L][0-3][0-9].txt$</t>
-  </si>
-  <si>
     <t>^BP[0-1][0-9][0-3][0-9][2][0-9].F01$</t>
   </si>
   <si>
@@ -641,9 +638,6 @@
     <t>Archive\POS Settlement</t>
   </si>
   <si>
-    <t>^SF[2][0-9][0-1][0-9][0-3][0-9].SDF$</t>
-  </si>
-  <si>
     <t>mmddyy</t>
   </si>
   <si>
@@ -701,9 +695,6 @@
     <t>Archive\Upload Installment Cosmos Email</t>
   </si>
   <si>
-    <t>^UNION_[2][0][2][0-9][0-1][0-9][0-3][0-9].TXT$|^UBC[0-9][0-9][0-9][0-9][0-9]BRF.DAT$</t>
-  </si>
-  <si>
     <t>billingfilenotificationbayantelecommunication</t>
   </si>
   <si>
@@ -768,6 +759,18 @@
   </si>
   <si>
     <t>/Smart/Billing/</t>
+  </si>
+  <si>
+    <t>^SF[2][0][2][0-9][0-1][0-9][0-3][0-9].SDF$</t>
+  </si>
+  <si>
+    <t>^UNION_[2][0][2][0-9][0-1][0-9][0-3][0-9].TXT$</t>
+  </si>
+  <si>
+    <t>^UBC[0-9][0-9][0-9][0-9][0-9].BRF.DAT$</t>
+  </si>
+  <si>
+    <t>^visaB[0-9][0-3][0-9].txt$</t>
   </si>
 </sst>
 </file>
@@ -1319,10 +1322,10 @@
         <v>46</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="I1" s="4" t="s">
         <v>60</v>
@@ -1340,7 +1343,7 @@
         <v>63</v>
       </c>
       <c r="N1" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="O1" s="4" t="s">
         <v>65</v>
@@ -1371,20 +1374,20 @@
         <v>104</v>
       </c>
       <c r="K2" s="7" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="L2" s="7"/>
       <c r="M2" s="7" t="s">
         <v>49</v>
       </c>
       <c r="N2" s="7" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="O2" s="7" t="s">
-        <v>211</v>
+        <v>232</v>
       </c>
       <c r="P2" s="10" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="3" spans="1:16" ht="30" x14ac:dyDescent="0.25">
@@ -1392,7 +1395,7 @@
         <v>54</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C3" s="7"/>
       <c r="D3" s="8" t="s">
@@ -1403,26 +1406,26 @@
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
       <c r="I3" s="7" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="J3" s="7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="K3" s="7" t="s">
-        <v>202</v>
+        <v>213</v>
       </c>
       <c r="L3" s="7"/>
       <c r="M3" s="7" t="s">
         <v>48</v>
       </c>
       <c r="N3" s="7" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="O3" s="7" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="P3" s="10" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="4" spans="1:16" ht="30" x14ac:dyDescent="0.25">
@@ -1447,20 +1450,20 @@
         <v>105</v>
       </c>
       <c r="K4" s="7" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="L4" s="7"/>
       <c r="M4" s="7" t="s">
         <v>49</v>
       </c>
       <c r="N4" s="7" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="O4" s="7" t="s">
-        <v>211</v>
+        <v>233</v>
       </c>
       <c r="P4" s="10" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="5" spans="1:16" ht="45" x14ac:dyDescent="0.25">
@@ -1485,20 +1488,20 @@
         <v>106</v>
       </c>
       <c r="K5" s="7" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="L5" s="7"/>
       <c r="M5" s="7" t="s">
         <v>49</v>
       </c>
       <c r="N5" s="7" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="O5" s="7" t="s">
         <v>136</v>
       </c>
       <c r="P5" s="10" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="6" spans="1:16" ht="30" x14ac:dyDescent="0.25">
@@ -1506,7 +1509,7 @@
         <v>54</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C6" s="7"/>
       <c r="D6" s="8" t="s">
@@ -1517,26 +1520,26 @@
       <c r="G6" s="6"/>
       <c r="H6" s="6"/>
       <c r="I6" s="7" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="K6" s="7" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="L6" s="7"/>
       <c r="M6" s="7" t="s">
         <v>48</v>
       </c>
       <c r="N6" s="7" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="O6" s="7" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="P6" s="10" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="7" spans="1:16" ht="45" x14ac:dyDescent="0.25">
@@ -1561,20 +1564,20 @@
         <v>107</v>
       </c>
       <c r="K7" s="7" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="L7" s="7"/>
       <c r="M7" s="7" t="s">
         <v>49</v>
       </c>
       <c r="N7" s="7" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="O7" s="7" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="P7" s="10" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="8" spans="1:16" ht="30" x14ac:dyDescent="0.25">
@@ -1599,20 +1602,20 @@
         <v>108</v>
       </c>
       <c r="K8" s="7" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="L8" s="7"/>
       <c r="M8" s="7" t="s">
         <v>48</v>
       </c>
       <c r="N8" s="7" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="O8" s="7" t="s">
         <v>137</v>
       </c>
       <c r="P8" s="10" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="9" spans="1:16" ht="30" x14ac:dyDescent="0.25">
@@ -1637,20 +1640,20 @@
         <v>109</v>
       </c>
       <c r="K9" s="7" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="L9" s="7"/>
       <c r="M9" s="7" t="s">
         <v>48</v>
       </c>
       <c r="N9" s="7" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="O9" s="7" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="P9" s="10" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="10" spans="1:16" ht="60" x14ac:dyDescent="0.25">
@@ -1675,20 +1678,20 @@
         <v>110</v>
       </c>
       <c r="K10" s="7" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="L10" s="7"/>
       <c r="M10" s="7" t="s">
         <v>48</v>
       </c>
       <c r="N10" s="7" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="O10" s="7" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="P10" s="10" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="11" spans="1:16" ht="45" x14ac:dyDescent="0.25">
@@ -1713,20 +1716,20 @@
         <v>111</v>
       </c>
       <c r="K11" s="7" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="L11" s="7"/>
       <c r="M11" s="7" t="s">
         <v>49</v>
       </c>
       <c r="N11" s="7" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="O11" s="7" t="s">
         <v>138</v>
       </c>
       <c r="P11" s="10" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="12" spans="1:16" ht="45" x14ac:dyDescent="0.25">
@@ -1751,20 +1754,20 @@
         <v>112</v>
       </c>
       <c r="K12" s="7" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="L12" s="7"/>
       <c r="M12" s="7" t="s">
         <v>49</v>
       </c>
       <c r="N12" s="7" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="O12" s="7" t="s">
         <v>139</v>
       </c>
       <c r="P12" s="10" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="13" spans="1:16" ht="45" x14ac:dyDescent="0.25">
@@ -1789,20 +1792,20 @@
         <v>113</v>
       </c>
       <c r="K13" s="7" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="L13" s="7"/>
       <c r="M13" s="7" t="s">
         <v>49</v>
       </c>
       <c r="N13" s="7" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="O13" s="7" t="s">
         <v>140</v>
       </c>
       <c r="P13" s="10" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="14" spans="1:16" ht="45" x14ac:dyDescent="0.25">
@@ -1827,20 +1830,20 @@
         <v>114</v>
       </c>
       <c r="K14" s="7" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="L14" s="7"/>
       <c r="M14" s="7" t="s">
         <v>48</v>
       </c>
       <c r="N14" s="7" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="O14" s="7" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="P14" s="10" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="15" spans="1:16" ht="45" x14ac:dyDescent="0.25">
@@ -1865,20 +1868,20 @@
         <v>115</v>
       </c>
       <c r="K15" s="7" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="L15" s="7"/>
       <c r="M15" s="7" t="s">
         <v>48</v>
       </c>
       <c r="N15" s="7" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="O15" s="7" t="s">
         <v>141</v>
       </c>
       <c r="P15" s="10" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="16" spans="1:16" ht="105" x14ac:dyDescent="0.25">
@@ -1903,20 +1906,20 @@
         <v>116</v>
       </c>
       <c r="K16" s="7" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="L16" s="7"/>
       <c r="M16" s="7" t="s">
         <v>48</v>
       </c>
       <c r="N16" s="7" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="O16" s="7" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="P16" s="10" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="17" spans="1:16" ht="75" x14ac:dyDescent="0.25">
@@ -1941,20 +1944,20 @@
         <v>117</v>
       </c>
       <c r="K17" s="7" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="L17" s="7"/>
       <c r="M17" s="7" t="s">
         <v>49</v>
       </c>
       <c r="N17" s="7" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="O17" s="7" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="P17" s="10" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="18" spans="1:16" ht="45" x14ac:dyDescent="0.25">
@@ -1979,20 +1982,20 @@
         <v>118</v>
       </c>
       <c r="K18" s="7" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="L18" s="7"/>
       <c r="M18" s="7" t="s">
         <v>49</v>
       </c>
       <c r="N18" s="7" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="O18" s="7" t="s">
-        <v>142</v>
+        <v>234</v>
       </c>
       <c r="P18" s="10" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="19" spans="1:16" ht="45" x14ac:dyDescent="0.25">
@@ -2017,20 +2020,20 @@
         <v>119</v>
       </c>
       <c r="K19" s="7" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="L19" s="7"/>
       <c r="M19" s="7" t="s">
         <v>49</v>
       </c>
       <c r="N19" s="7" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="O19" s="7" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="P19" s="10" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="20" spans="1:16" ht="30" x14ac:dyDescent="0.25">
@@ -2038,37 +2041,37 @@
         <v>54</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C20" s="11"/>
       <c r="D20" s="9" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
       <c r="H20" s="6"/>
       <c r="I20" s="7" t="s">
+        <v>188</v>
+      </c>
+      <c r="J20" s="7" t="s">
         <v>189</v>
       </c>
-      <c r="J20" s="7" t="s">
-        <v>190</v>
-      </c>
       <c r="K20" s="7" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="L20" s="7"/>
       <c r="M20" s="7" t="s">
         <v>48</v>
       </c>
       <c r="N20" s="7" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="O20" s="7" t="s">
-        <v>191</v>
+        <v>231</v>
       </c>
       <c r="P20" s="10" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="21" spans="1:16" ht="30" x14ac:dyDescent="0.25">
@@ -2080,7 +2083,7 @@
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="1" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="E21" s="1">
         <v>22</v>
@@ -2089,10 +2092,10 @@
         <v>47</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="H21" s="20" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="I21" s="1" t="s">
         <v>89</v>
@@ -2101,20 +2104,20 @@
         <v>120</v>
       </c>
       <c r="K21" s="7" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="L21" s="1"/>
       <c r="M21" s="1" t="s">
         <v>49</v>
       </c>
       <c r="N21" s="7" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="O21" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="P21" s="10" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="22" spans="1:16" ht="30" x14ac:dyDescent="0.25">
@@ -2122,11 +2125,11 @@
         <v>55</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C22" s="1"/>
       <c r="D22" s="1" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="E22" s="1">
         <v>22</v>
@@ -2135,32 +2138,32 @@
         <v>47</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="H22" s="20" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="K22" s="7" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="L22" s="1"/>
       <c r="M22" s="1" t="s">
         <v>48</v>
       </c>
       <c r="N22" s="7" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="O22" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="P22" s="10" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="23" spans="1:16" ht="30" x14ac:dyDescent="0.25">
@@ -2172,7 +2175,7 @@
       </c>
       <c r="C23" s="1"/>
       <c r="D23" s="1" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="E23" s="1">
         <v>22</v>
@@ -2181,10 +2184,10 @@
         <v>47</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="H23" s="20" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="I23" s="1" t="s">
         <v>90</v>
@@ -2193,20 +2196,20 @@
         <v>121</v>
       </c>
       <c r="K23" s="7" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="L23" s="1"/>
       <c r="M23" s="1" t="s">
         <v>49</v>
       </c>
       <c r="N23" s="7" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="O23" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="P23" s="10" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="24" spans="1:16" ht="30" x14ac:dyDescent="0.25">
@@ -2218,7 +2221,7 @@
       </c>
       <c r="C24" s="1"/>
       <c r="D24" s="1" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="E24" s="1">
         <v>22</v>
@@ -2227,10 +2230,10 @@
         <v>47</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="H24" s="20" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="I24" s="1" t="s">
         <v>91</v>
@@ -2239,20 +2242,20 @@
         <v>122</v>
       </c>
       <c r="K24" s="7" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="L24" s="1"/>
       <c r="M24" s="1" t="s">
         <v>49</v>
       </c>
       <c r="N24" s="7" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="O24" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="P24" s="10" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="25" spans="1:16" ht="45" x14ac:dyDescent="0.25">
@@ -2264,7 +2267,7 @@
       </c>
       <c r="C25" s="1"/>
       <c r="D25" s="1" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="E25" s="1">
         <v>22</v>
@@ -2273,10 +2276,10 @@
         <v>47</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="H25" s="20" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="I25" s="1" t="s">
         <v>92</v>
@@ -2285,22 +2288,22 @@
         <v>123</v>
       </c>
       <c r="K25" s="7" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="L25" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="M25" s="1" t="s">
         <v>49</v>
       </c>
       <c r="N25" s="7" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="O25" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="P25" s="10" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="26" spans="1:16" ht="30" x14ac:dyDescent="0.25">
@@ -2312,7 +2315,7 @@
       </c>
       <c r="C26" s="1"/>
       <c r="D26" s="19" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
@@ -2325,20 +2328,20 @@
         <v>124</v>
       </c>
       <c r="K26" s="7" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="L26" s="1"/>
       <c r="M26" s="1" t="s">
         <v>48</v>
       </c>
       <c r="N26" s="7" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="O26" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="P26" s="10" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="27" spans="1:16" ht="30" x14ac:dyDescent="0.25">
@@ -2349,7 +2352,7 @@
         <v>20</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
@@ -2363,7 +2366,7 @@
         <v>125</v>
       </c>
       <c r="K27" s="7" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="L27" s="1" t="s">
         <v>30</v>
@@ -2372,10 +2375,10 @@
         <v>49</v>
       </c>
       <c r="N27" s="7" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="O27" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="P27" s="1"/>
     </row>
@@ -2387,7 +2390,7 @@
         <v>21</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
@@ -2401,7 +2404,7 @@
         <v>126</v>
       </c>
       <c r="K28" s="7" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="L28" s="1">
         <v>1234</v>
@@ -2410,10 +2413,10 @@
         <v>49</v>
       </c>
       <c r="N28" s="7" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="O28" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="P28" s="1"/>
     </row>
@@ -2425,7 +2428,7 @@
         <v>22</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
@@ -2439,7 +2442,7 @@
         <v>127</v>
       </c>
       <c r="K29" s="7" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="L29" s="1" t="s">
         <v>50</v>
@@ -2448,10 +2451,10 @@
         <v>49</v>
       </c>
       <c r="N29" s="7" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="O29" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="P29" s="1"/>
     </row>
@@ -2463,7 +2466,7 @@
         <v>23</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
@@ -2471,13 +2474,13 @@
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
       <c r="I30" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="K30" s="7" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="L30" s="1" t="s">
         <v>51</v>
@@ -2486,10 +2489,10 @@
         <v>48</v>
       </c>
       <c r="N30" s="7" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="O30" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="P30" s="1"/>
     </row>
@@ -2498,10 +2501,10 @@
         <v>56</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
@@ -2515,19 +2518,19 @@
         <v>128</v>
       </c>
       <c r="K31" s="7" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="L31" s="7" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="M31" s="1" t="s">
         <v>48</v>
       </c>
       <c r="N31" s="7" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="O31" s="3" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="P31" s="1"/>
     </row>
@@ -2536,10 +2539,10 @@
         <v>56</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
@@ -2547,25 +2550,25 @@
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
       <c r="I32" s="1" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="J32" s="1" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="K32" s="7" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="L32" s="17" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="M32" s="1" t="s">
         <v>48</v>
       </c>
       <c r="N32" s="7" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="O32" s="3" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="P32" s="1"/>
     </row>
@@ -2574,37 +2577,37 @@
         <v>54</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C33" s="1"/>
       <c r="D33" s="15" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="E33" s="2"/>
       <c r="F33" s="2"/>
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
       <c r="I33" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="J33" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="J33" s="1" t="s">
-        <v>185</v>
-      </c>
       <c r="K33" s="7" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="L33" s="1"/>
       <c r="M33" s="1" t="s">
         <v>48</v>
       </c>
       <c r="N33" s="7" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="O33" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="P33" s="10" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="34" spans="1:16" ht="45" x14ac:dyDescent="0.25">
@@ -2615,7 +2618,7 @@
         <v>24</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D34" s="2"/>
       <c r="E34" s="2"/>
@@ -2629,19 +2632,19 @@
         <v>129</v>
       </c>
       <c r="K34" s="7" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="L34" s="7" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="M34" s="1" t="s">
         <v>48</v>
       </c>
       <c r="N34" s="7" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="O34" s="3" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="P34" s="1"/>
     </row>
@@ -2653,7 +2656,7 @@
         <v>25</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D35" s="2"/>
       <c r="E35" s="2"/>
@@ -2661,25 +2664,25 @@
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
       <c r="I35" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="J35" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="K35" s="7" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="L35" s="7" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="M35" s="1" t="s">
         <v>48</v>
       </c>
       <c r="N35" s="7" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="O35" s="3" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="P35" s="1"/>
     </row>
@@ -2691,7 +2694,7 @@
         <v>26</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
@@ -2705,19 +2708,19 @@
         <v>130</v>
       </c>
       <c r="K36" s="7" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="L36" s="7" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="M36" s="1" t="s">
         <v>48</v>
       </c>
       <c r="N36" s="7" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="O36" s="3" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="P36" s="1"/>
     </row>
@@ -2729,7 +2732,7 @@
         <v>27</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="D37" s="2"/>
       <c r="E37" s="2"/>
@@ -2743,17 +2746,17 @@
         <v>131</v>
       </c>
       <c r="K37" s="7" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="L37" s="1"/>
       <c r="M37" s="1" t="s">
         <v>48</v>
       </c>
       <c r="N37" s="7" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="O37" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="P37" s="1"/>
     </row>
@@ -2765,7 +2768,7 @@
         <v>28</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D38" s="2"/>
       <c r="E38" s="2"/>
@@ -2779,7 +2782,7 @@
         <v>132</v>
       </c>
       <c r="K38" s="7" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="L38" s="12" t="s">
         <v>53</v>
@@ -2788,10 +2791,10 @@
         <v>48</v>
       </c>
       <c r="N38" s="7" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="O38" s="7" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="P38" s="1"/>
     </row>
@@ -2803,7 +2806,7 @@
         <v>12</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D39" s="2"/>
       <c r="E39" s="2"/>
@@ -2817,7 +2820,7 @@
         <v>134</v>
       </c>
       <c r="K39" s="7" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="L39" s="14" t="s">
         <v>53</v>
@@ -2826,10 +2829,10 @@
         <v>48</v>
       </c>
       <c r="N39" s="7" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="O39" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="P39" s="1"/>
     </row>
@@ -2841,7 +2844,7 @@
         <v>29</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D40" s="2"/>
       <c r="E40" s="2"/>
@@ -2855,7 +2858,7 @@
         <v>133</v>
       </c>
       <c r="K40" s="7" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="L40" s="12" t="s">
         <v>52</v>
@@ -2864,10 +2867,10 @@
         <v>48</v>
       </c>
       <c r="N40" s="7" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="O40" s="7" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="P40" s="1"/>
     </row>

</xml_diff>

<commit_message>
Code Version 18052020 19:52
</commit_message>
<xml_diff>
--- a/Prime_Job_Automation/Configuration/RuleFactory/Master Rule Factory.xlsx
+++ b/Prime_Job_Automation/Configuration/RuleFactory/Master Rule Factory.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\PJA\Prime_Job_Automation\Configuration\RuleFactory\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3D11FBD-A46E-4FE0-BD29-DC1F26CB23BE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B1ACFD0-1692-48C6-BAA2-1CD57F3112D4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" tabRatio="351" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1504,12 +1504,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:W49"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="N1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="N1" sqref="N1"/>
+      <pane xSplit="2" topLeftCell="M1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1607,7 +1606,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="2" spans="1:23" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>54</v>
       </c>
@@ -1664,7 +1663,7 @@
       </c>
       <c r="W2" s="21"/>
     </row>
-    <row r="3" spans="1:23" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>54</v>
       </c>
@@ -1721,7 +1720,7 @@
       </c>
       <c r="W3" s="21"/>
     </row>
-    <row r="4" spans="1:23" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>54</v>
       </c>
@@ -1778,7 +1777,7 @@
       </c>
       <c r="W4" s="21"/>
     </row>
-    <row r="5" spans="1:23" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>54</v>
       </c>
@@ -1829,7 +1828,7 @@
       <c r="V5" s="21"/>
       <c r="W5" s="21"/>
     </row>
-    <row r="6" spans="1:23" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>54</v>
       </c>
@@ -1886,7 +1885,7 @@
       </c>
       <c r="W6" s="21"/>
     </row>
-    <row r="7" spans="1:23" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:23" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>54</v>
       </c>
@@ -1937,7 +1936,7 @@
       <c r="V7" s="21"/>
       <c r="W7" s="21"/>
     </row>
-    <row r="8" spans="1:23" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>54</v>
       </c>
@@ -1988,7 +1987,7 @@
       <c r="V8" s="21"/>
       <c r="W8" s="21"/>
     </row>
-    <row r="9" spans="1:23" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:23" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>54</v>
       </c>
@@ -2039,7 +2038,7 @@
       <c r="V9" s="21"/>
       <c r="W9" s="21"/>
     </row>
-    <row r="10" spans="1:23" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:23" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>54</v>
       </c>
@@ -2090,7 +2089,7 @@
       <c r="V10" s="21"/>
       <c r="W10" s="21"/>
     </row>
-    <row r="11" spans="1:23" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:23" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>54</v>
       </c>
@@ -2141,7 +2140,7 @@
       <c r="V11" s="21"/>
       <c r="W11" s="21"/>
     </row>
-    <row r="12" spans="1:23" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:23" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>54</v>
       </c>
@@ -2192,7 +2191,7 @@
       <c r="V12" s="21"/>
       <c r="W12" s="21"/>
     </row>
-    <row r="13" spans="1:23" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:23" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>54</v>
       </c>
@@ -2243,7 +2242,7 @@
       <c r="V13" s="21"/>
       <c r="W13" s="21"/>
     </row>
-    <row r="14" spans="1:23" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:23" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>54</v>
       </c>
@@ -2294,7 +2293,7 @@
       <c r="V14" s="21"/>
       <c r="W14" s="21"/>
     </row>
-    <row r="15" spans="1:23" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:23" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>54</v>
       </c>
@@ -2351,7 +2350,7 @@
       </c>
       <c r="W15" s="21"/>
     </row>
-    <row r="16" spans="1:23" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:23" ht="105" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>54</v>
       </c>
@@ -2408,7 +2407,7 @@
       </c>
       <c r="W16" s="21"/>
     </row>
-    <row r="17" spans="1:23" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:23" ht="75" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>54</v>
       </c>
@@ -2465,7 +2464,7 @@
       </c>
       <c r="W17" s="21"/>
     </row>
-    <row r="18" spans="1:23" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:23" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>54</v>
       </c>
@@ -2516,7 +2515,7 @@
       <c r="V18" s="21"/>
       <c r="W18" s="21"/>
     </row>
-    <row r="19" spans="1:23" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:23" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>54</v>
       </c>
@@ -2567,7 +2566,7 @@
       <c r="V19" s="21"/>
       <c r="W19" s="21"/>
     </row>
-    <row r="20" spans="1:23" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:23" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="14" t="s">
         <v>54</v>
       </c>
@@ -2618,7 +2617,7 @@
       <c r="V20" s="21"/>
       <c r="W20" s="21"/>
     </row>
-    <row r="21" spans="1:23" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:23" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>55</v>
       </c>
@@ -2683,7 +2682,7 @@
       </c>
       <c r="W21" s="21"/>
     </row>
-    <row r="22" spans="1:23" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:23" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>55</v>
       </c>
@@ -2748,7 +2747,7 @@
       </c>
       <c r="W22" s="21"/>
     </row>
-    <row r="23" spans="1:23" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:23" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>55</v>
       </c>
@@ -2757,7 +2756,7 @@
       </c>
       <c r="C23" s="1"/>
       <c r="D23" s="1" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="E23" s="1">
         <v>22</v>
@@ -2813,7 +2812,7 @@
       </c>
       <c r="W23" s="21"/>
     </row>
-    <row r="24" spans="1:23" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:23" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>55</v>
       </c>
@@ -2822,7 +2821,7 @@
       </c>
       <c r="C24" s="1"/>
       <c r="D24" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E24" s="1">
         <v>22</v>
@@ -2878,7 +2877,7 @@
       </c>
       <c r="W24" s="21"/>
     </row>
-    <row r="25" spans="1:23" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:23" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>55</v>
       </c>
@@ -2939,7 +2938,7 @@
       <c r="V25" s="21"/>
       <c r="W25" s="21"/>
     </row>
-    <row r="26" spans="1:23" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:23" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>54</v>
       </c>
@@ -2990,7 +2989,7 @@
       <c r="V26" s="21"/>
       <c r="W26" s="21"/>
     </row>
-    <row r="27" spans="1:23" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:23" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>56</v>
       </c>
@@ -3049,7 +3048,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="28" spans="1:23" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:23" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>56</v>
       </c>
@@ -3108,7 +3107,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="29" spans="1:23" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:23" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>56</v>
       </c>
@@ -3167,7 +3166,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="30" spans="1:23" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:23" ht="45" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>56</v>
       </c>
@@ -3224,7 +3223,7 @@
       </c>
       <c r="W30" s="21"/>
     </row>
-    <row r="31" spans="1:23" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:23" ht="45" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>56</v>
       </c>
@@ -3397,7 +3396,7 @@
       </c>
       <c r="W33" s="21"/>
     </row>
-    <row r="34" spans="1:23" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:23" ht="45" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>56</v>
       </c>
@@ -3456,7 +3455,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="35" spans="1:23" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:23" ht="60" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>56</v>
       </c>
@@ -3515,7 +3514,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="36" spans="1:23" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:23" ht="45" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>56</v>
       </c>
@@ -3574,7 +3573,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="37" spans="1:23" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:23" ht="45" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>56</v>
       </c>
@@ -3631,7 +3630,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="38" spans="1:23" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:23" ht="45" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>56</v>
       </c>
@@ -3690,7 +3689,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="39" spans="1:23" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:23" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>56</v>
       </c>
@@ -3749,7 +3748,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="40" spans="1:23" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:23" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>56</v>
       </c>
@@ -3824,14 +3823,6 @@
       <c r="C49" s="12"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:W40" xr:uid="{B51B7F33-376B-4794-B970-BE0280E761F5}">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="Upload Installment - Cosmos"/>
-        <filter val="Upload Installment - Cosmos Email"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
     <hyperlink ref="D3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000003000000}"/>

</xml_diff>

<commit_message>
Code Version 20052020 23:25
</commit_message>
<xml_diff>
--- a/Prime_Job_Automation/Configuration/RuleFactory/Master Rule Factory.xlsx
+++ b/Prime_Job_Automation/Configuration/RuleFactory/Master Rule Factory.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\PJA\Prime_Job_Automation\Configuration\RuleFactory\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81028AFD-F60D-4FF1-B0B4-8FCA7C554B59}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFE03011-776D-4338-A20F-E119685312DB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" tabRatio="351" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="630" uniqueCount="299">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="630" uniqueCount="301">
   <si>
     <t>Password</t>
   </si>
@@ -260,9 +260,6 @@
     <t>Is_Conversion_Required?</t>
   </si>
   <si>
-    <t>PreBatch_Process</t>
-  </si>
-  <si>
     <t>Source_Filename_Pattern</t>
   </si>
   <si>
@@ -857,9 +854,6 @@
     <t>Return_File_Pattern</t>
   </si>
   <si>
-    <t>Email_Id</t>
-  </si>
-  <si>
     <t>AfterEOD</t>
   </si>
   <si>
@@ -963,6 +957,18 @@
   </si>
   <si>
     <t>useSMFileName</t>
+  </si>
+  <si>
+    <t>^R06_CLUBP_PH_MonetaryFileResponse_\d\d\d\D_\d\d\d\d\d\d\d\d_\d\d\d\d\d\d\d\d _\d\d\d\d\d\d.out$</t>
+  </si>
+  <si>
+    <t>^NON_AIR_TRN_\d\d\d\d\d\d\d\d_\d\d_\d\d_\d\d_UNIONCD.LOG$</t>
+  </si>
+  <si>
+    <t>Process_Name</t>
+  </si>
+  <si>
+    <t>Return_File_Email_Id</t>
   </si>
 </sst>
 </file>
@@ -1508,7 +1514,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="topRight" activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1540,7 +1546,7 @@
         <v>57</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>64</v>
+        <v>299</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>58</v>
@@ -1555,10 +1561,10 @@
         <v>46</v>
       </c>
       <c r="G1" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="H1" s="4" t="s">
         <v>223</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>224</v>
       </c>
       <c r="I1" s="4" t="s">
         <v>60</v>
@@ -1576,34 +1582,34 @@
         <v>63</v>
       </c>
       <c r="N1" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="O1" s="4" t="s">
+        <v>231</v>
+      </c>
+      <c r="P1" s="4" t="s">
         <v>232</v>
       </c>
-      <c r="P1" s="4" t="s">
-        <v>233</v>
-      </c>
       <c r="Q1" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="R1" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="S1" s="4" t="s">
+        <v>258</v>
+      </c>
+      <c r="T1" s="4" t="s">
+        <v>261</v>
+      </c>
+      <c r="U1" s="4" t="s">
         <v>259</v>
       </c>
-      <c r="T1" s="4" t="s">
-        <v>262</v>
-      </c>
-      <c r="U1" s="4" t="s">
+      <c r="V1" s="4" t="s">
         <v>260</v>
       </c>
-      <c r="V1" s="4" t="s">
-        <v>261</v>
-      </c>
       <c r="W1" s="4" t="s">
-        <v>263</v>
+        <v>300</v>
       </c>
     </row>
     <row r="2" spans="1:23" ht="30" x14ac:dyDescent="0.25">
@@ -1622,44 +1628,44 @@
       <c r="G2" s="6"/>
       <c r="H2" s="6"/>
       <c r="I2" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J2" s="7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="K2" s="7" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="L2" s="7"/>
       <c r="M2" s="7" t="s">
         <v>49</v>
       </c>
       <c r="N2" s="7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="O2" s="7" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="P2" s="7" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="Q2" s="7" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="R2" s="10" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="S2" s="24" t="s">
+        <v>262</v>
+      </c>
+      <c r="T2" s="21" t="s">
+        <v>263</v>
+      </c>
+      <c r="U2" s="25" t="s">
         <v>264</v>
       </c>
-      <c r="T2" s="21" t="s">
-        <v>265</v>
-      </c>
-      <c r="U2" s="25" t="s">
-        <v>266</v>
-      </c>
       <c r="V2" s="10" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="W2" s="21"/>
     </row>
@@ -1668,7 +1674,7 @@
         <v>54</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C3" s="7"/>
       <c r="D3" s="8" t="s">
@@ -1679,44 +1685,44 @@
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
       <c r="I3" s="7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="J3" s="7" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="K3" s="7" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="L3" s="7"/>
       <c r="M3" s="7" t="s">
         <v>48</v>
       </c>
       <c r="N3" s="7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="O3" s="7" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="P3" s="7" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="Q3" s="7" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="R3" s="10" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="S3" s="7" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="T3" s="21" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="U3" s="25" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="V3" s="10" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="W3" s="21"/>
     </row>
@@ -1736,44 +1742,44 @@
       <c r="G4" s="6"/>
       <c r="H4" s="6"/>
       <c r="I4" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J4" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K4" s="7" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="L4" s="7"/>
       <c r="M4" s="7" t="s">
         <v>49</v>
       </c>
       <c r="N4" s="7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="O4" s="7" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="P4" s="7" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="Q4" s="7" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="R4" s="10" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="S4" s="17" t="s">
+        <v>262</v>
+      </c>
+      <c r="T4" s="21" t="s">
+        <v>267</v>
+      </c>
+      <c r="U4" s="25" t="s">
         <v>264</v>
       </c>
-      <c r="T4" s="21" t="s">
-        <v>269</v>
-      </c>
-      <c r="U4" s="25" t="s">
-        <v>266</v>
-      </c>
       <c r="V4" s="10" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="W4" s="21"/>
     </row>
@@ -1786,42 +1792,42 @@
       </c>
       <c r="C5" s="7"/>
       <c r="D5" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E5" s="6"/>
       <c r="F5" s="6"/>
       <c r="G5" s="6"/>
       <c r="H5" s="6"/>
       <c r="I5" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J5" s="7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="K5" s="7" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="L5" s="7"/>
       <c r="M5" s="7" t="s">
         <v>49</v>
       </c>
       <c r="N5" s="7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="O5" s="7" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="P5" s="7" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="Q5" s="7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="R5" s="10" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="S5" s="17" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="T5" s="21"/>
       <c r="U5" s="21"/>
@@ -1833,7 +1839,7 @@
         <v>54</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C6" s="7"/>
       <c r="D6" s="8" t="s">
@@ -1844,44 +1850,44 @@
       <c r="G6" s="6"/>
       <c r="H6" s="6"/>
       <c r="I6" s="7" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="K6" s="7" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="L6" s="7"/>
       <c r="M6" s="7" t="s">
         <v>48</v>
       </c>
       <c r="N6" s="7" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="O6" s="7" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="P6" s="7" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="Q6" s="7" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="R6" s="10" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="S6" s="17" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="T6" s="21" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="U6" s="25" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="V6" s="10" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="W6" s="21"/>
     </row>
@@ -1901,35 +1907,35 @@
       <c r="G7" s="6"/>
       <c r="H7" s="6"/>
       <c r="I7" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J7" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="K7" s="7" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="L7" s="7"/>
       <c r="M7" s="7" t="s">
         <v>49</v>
       </c>
       <c r="N7" s="7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="O7" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="P7" s="7" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="Q7" s="7" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="R7" s="10" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="S7" s="17" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="T7" s="21"/>
       <c r="U7" s="21"/>
@@ -1952,35 +1958,35 @@
       <c r="G8" s="6"/>
       <c r="H8" s="6"/>
       <c r="I8" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J8" s="7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="K8" s="7" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="L8" s="7"/>
       <c r="M8" s="7" t="s">
         <v>48</v>
       </c>
       <c r="N8" s="7" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="O8" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="P8" s="7" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="Q8" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="R8" s="10" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="S8" s="17" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="T8" s="21"/>
       <c r="U8" s="21"/>
@@ -2003,35 +2009,35 @@
       <c r="G9" s="6"/>
       <c r="H9" s="6"/>
       <c r="I9" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J9" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="K9" s="7" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="L9" s="7"/>
       <c r="M9" s="7" t="s">
         <v>48</v>
       </c>
       <c r="N9" s="7" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="O9" s="7" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="P9" s="7" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="Q9" s="7" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="R9" s="10" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="S9" s="17" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="T9" s="21"/>
       <c r="U9" s="21"/>
@@ -2054,35 +2060,35 @@
       <c r="G10" s="6"/>
       <c r="H10" s="6"/>
       <c r="I10" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J10" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="K10" s="7" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="L10" s="7"/>
       <c r="M10" s="7" t="s">
         <v>48</v>
       </c>
       <c r="N10" s="7" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="O10" s="7" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="P10" s="7" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="Q10" s="7" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="R10" s="10" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="S10" s="17" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="T10" s="21"/>
       <c r="U10" s="21"/>
@@ -2105,35 +2111,35 @@
       <c r="G11" s="6"/>
       <c r="H11" s="6"/>
       <c r="I11" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J11" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K11" s="7" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="L11" s="7"/>
       <c r="M11" s="7" t="s">
         <v>49</v>
       </c>
       <c r="N11" s="7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="O11" s="7" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="P11" s="7" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="Q11" s="7" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="R11" s="10" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="S11" s="17" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="T11" s="21"/>
       <c r="U11" s="21"/>
@@ -2156,35 +2162,35 @@
       <c r="G12" s="6"/>
       <c r="H12" s="6"/>
       <c r="I12" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J12" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="K12" s="7" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="L12" s="7"/>
       <c r="M12" s="7" t="s">
         <v>49</v>
       </c>
       <c r="N12" s="7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="O12" s="7" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="P12" s="7" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="Q12" s="7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="R12" s="10" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="S12" s="17" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="T12" s="21"/>
       <c r="U12" s="21"/>
@@ -2207,35 +2213,35 @@
       <c r="G13" s="6"/>
       <c r="H13" s="6"/>
       <c r="I13" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J13" s="7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K13" s="7" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="L13" s="7"/>
       <c r="M13" s="7" t="s">
         <v>49</v>
       </c>
       <c r="N13" s="7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="O13" s="7" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="P13" s="7" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="Q13" s="7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="R13" s="10" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="S13" s="17" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="T13" s="21"/>
       <c r="U13" s="21"/>
@@ -2258,35 +2264,35 @@
       <c r="G14" s="6"/>
       <c r="H14" s="6"/>
       <c r="I14" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J14" s="7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="K14" s="7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="L14" s="7"/>
       <c r="M14" s="7" t="s">
         <v>48</v>
       </c>
       <c r="N14" s="7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="O14" s="7" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="P14" s="7" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="Q14" s="7" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="R14" s="10" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="S14" s="17" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="T14" s="21"/>
       <c r="U14" s="21"/>
@@ -2309,44 +2315,44 @@
       <c r="G15" s="6"/>
       <c r="H15" s="6"/>
       <c r="I15" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J15" s="7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="K15" s="7" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="L15" s="7"/>
       <c r="M15" s="7" t="s">
         <v>48</v>
       </c>
       <c r="N15" s="7" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="O15" s="7" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="P15" s="7" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="Q15" s="7" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="R15" s="10" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="S15" s="7" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="T15" s="21" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="U15" s="21" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="V15" s="10" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="W15" s="21"/>
     </row>
@@ -2366,44 +2372,44 @@
       <c r="G16" s="6"/>
       <c r="H16" s="6"/>
       <c r="I16" s="7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J16" s="7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K16" s="7" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="L16" s="7"/>
       <c r="M16" s="7" t="s">
         <v>48</v>
       </c>
       <c r="N16" s="7" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="O16" s="7" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="P16" s="7" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="Q16" s="7" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="R16" s="10" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="S16" s="17" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="T16" s="21" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="U16" s="21" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="V16" s="10" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="W16" s="21"/>
     </row>
@@ -2412,55 +2418,55 @@
         <v>54</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C17" s="7"/>
       <c r="D17" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E17" s="6"/>
       <c r="F17" s="6"/>
       <c r="G17" s="6"/>
       <c r="H17" s="6"/>
       <c r="I17" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J17" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="K17" s="7" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="L17" s="7"/>
       <c r="M17" s="7" t="s">
         <v>49</v>
       </c>
       <c r="N17" s="7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="O17" s="7" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="P17" s="7" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="Q17" s="7" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="R17" s="10" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="S17" s="17" t="s">
+        <v>262</v>
+      </c>
+      <c r="T17" s="21" t="s">
+        <v>272</v>
+      </c>
+      <c r="U17" s="25" t="s">
         <v>264</v>
       </c>
-      <c r="T17" s="21" t="s">
-        <v>274</v>
-      </c>
-      <c r="U17" s="25" t="s">
-        <v>266</v>
-      </c>
       <c r="V17" s="10" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="W17" s="21"/>
     </row>
@@ -2469,46 +2475,46 @@
         <v>54</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C18" s="7"/>
       <c r="D18" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E18" s="6"/>
       <c r="F18" s="6"/>
       <c r="G18" s="6"/>
       <c r="H18" s="6"/>
       <c r="I18" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="J18" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="K18" s="7" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="L18" s="7"/>
       <c r="M18" s="7" t="s">
         <v>49</v>
       </c>
       <c r="N18" s="7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="O18" s="7" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="P18" s="7" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="Q18" s="7" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="R18" s="10" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="S18" s="17" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="T18" s="21"/>
       <c r="U18" s="21"/>
@@ -2520,46 +2526,46 @@
         <v>54</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C19" s="7"/>
       <c r="D19" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
       <c r="H19" s="6"/>
       <c r="I19" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J19" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="K19" s="7" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="L19" s="7"/>
       <c r="M19" s="7" t="s">
         <v>49</v>
       </c>
       <c r="N19" s="7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="O19" s="7" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="P19" s="7" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="Q19" s="7" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="R19" s="10" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="S19" s="17" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="T19" s="21"/>
       <c r="U19" s="21"/>
@@ -2571,46 +2577,46 @@
         <v>54</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C20" s="11"/>
       <c r="D20" s="9" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
       <c r="H20" s="6"/>
       <c r="I20" s="7" t="s">
+        <v>186</v>
+      </c>
+      <c r="J20" s="7" t="s">
         <v>187</v>
       </c>
-      <c r="J20" s="7" t="s">
-        <v>188</v>
-      </c>
       <c r="K20" s="7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="L20" s="7"/>
       <c r="M20" s="7" t="s">
         <v>48</v>
       </c>
       <c r="N20" s="7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="O20" s="7" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="P20" s="7" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="Q20" s="7" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="R20" s="10" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="S20" s="17" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="T20" s="21"/>
       <c r="U20" s="21"/>
@@ -2626,7 +2632,7 @@
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E21" s="1">
         <v>22</v>
@@ -2635,50 +2641,50 @@
         <v>47</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="H21" s="15" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="K21" s="7" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="L21" s="1"/>
       <c r="M21" s="1" t="s">
         <v>49</v>
       </c>
       <c r="N21" s="7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="O21" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="P21" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="P21" s="1" t="s">
-        <v>235</v>
-      </c>
       <c r="Q21" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="R21" s="10" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="S21" s="17" t="s">
+        <v>262</v>
+      </c>
+      <c r="T21" s="21" t="s">
+        <v>273</v>
+      </c>
+      <c r="U21" s="25" t="s">
         <v>264</v>
       </c>
-      <c r="T21" s="21" t="s">
-        <v>275</v>
-      </c>
-      <c r="U21" s="25" t="s">
-        <v>266</v>
-      </c>
       <c r="V21" s="21" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="W21" s="21"/>
     </row>
@@ -2687,11 +2693,11 @@
         <v>55</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C22" s="1"/>
       <c r="D22" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E22" s="1">
         <v>22</v>
@@ -2700,50 +2706,50 @@
         <v>47</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="H22" s="15" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="K22" s="7" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="L22" s="1"/>
       <c r="M22" s="1" t="s">
         <v>48</v>
       </c>
       <c r="N22" s="7" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="O22" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="P22" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="Q22" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="R22" s="10" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="S22" s="17" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="T22" s="21" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="U22" s="25" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="V22" s="21" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="W22" s="21"/>
     </row>
@@ -2756,7 +2762,7 @@
       </c>
       <c r="C23" s="1"/>
       <c r="D23" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E23" s="1">
         <v>22</v>
@@ -2765,50 +2771,50 @@
         <v>47</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="H23" s="15" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="K23" s="7" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="L23" s="1"/>
       <c r="M23" s="1" t="s">
         <v>49</v>
       </c>
       <c r="N23" s="7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="O23" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="P23" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="Q23" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="R23" s="10" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="S23" s="19" t="s">
+        <v>262</v>
+      </c>
+      <c r="T23" s="21" t="s">
+        <v>277</v>
+      </c>
+      <c r="U23" s="25" t="s">
         <v>264</v>
       </c>
-      <c r="T23" s="21" t="s">
-        <v>279</v>
-      </c>
-      <c r="U23" s="25" t="s">
-        <v>266</v>
-      </c>
       <c r="V23" s="21" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="W23" s="21"/>
     </row>
@@ -2821,7 +2827,7 @@
       </c>
       <c r="C24" s="1"/>
       <c r="D24" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E24" s="1">
         <v>22</v>
@@ -2830,50 +2836,50 @@
         <v>47</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="H24" s="15" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="K24" s="7" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="L24" s="1"/>
       <c r="M24" s="1" t="s">
         <v>49</v>
       </c>
       <c r="N24" s="7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="O24" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="P24" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="Q24" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="R24" s="10" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="S24" s="19" t="s">
+        <v>262</v>
+      </c>
+      <c r="T24" s="21" t="s">
+        <v>279</v>
+      </c>
+      <c r="U24" s="25" t="s">
         <v>264</v>
       </c>
-      <c r="T24" s="21" t="s">
-        <v>281</v>
-      </c>
-      <c r="U24" s="25" t="s">
-        <v>266</v>
-      </c>
       <c r="V24" s="21" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="W24" s="21"/>
     </row>
@@ -2886,7 +2892,7 @@
       </c>
       <c r="C25" s="1"/>
       <c r="D25" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E25" s="1">
         <v>22</v>
@@ -2895,43 +2901,43 @@
         <v>47</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="H25" s="15" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="K25" s="7" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="L25" s="1" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="M25" s="1" t="s">
         <v>49</v>
       </c>
       <c r="N25" s="7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="O25" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="P25" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="Q25" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="R25" s="10" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="S25" s="17" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="T25" s="21"/>
       <c r="U25" s="21"/>
@@ -2947,42 +2953,42 @@
       </c>
       <c r="C26" s="1"/>
       <c r="D26" s="19" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
       <c r="I26" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="K26" s="7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="L26" s="1"/>
       <c r="M26" s="1" t="s">
         <v>48</v>
       </c>
       <c r="N26" s="7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="O26" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="P26" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="Q26" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="R26" s="10" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="S26" s="17" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="T26" s="21"/>
       <c r="U26" s="21"/>
@@ -2997,7 +3003,7 @@
         <v>20</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
@@ -3005,13 +3011,13 @@
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
       <c r="I27" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="K27" s="7" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="L27" s="1" t="s">
         <v>30</v>
@@ -3020,32 +3026,32 @@
         <v>49</v>
       </c>
       <c r="N27" s="7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="O27" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="P27" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="Q27" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="R27" s="1"/>
       <c r="S27" s="19" t="s">
+        <v>262</v>
+      </c>
+      <c r="T27" s="21" t="s">
+        <v>280</v>
+      </c>
+      <c r="U27" s="25" t="s">
         <v>264</v>
-      </c>
-      <c r="T27" s="21" t="s">
-        <v>282</v>
-      </c>
-      <c r="U27" s="25" t="s">
-        <v>266</v>
       </c>
       <c r="V27" s="21" t="s">
         <v>56</v>
       </c>
       <c r="W27" s="10" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="28" spans="1:23" ht="30" x14ac:dyDescent="0.25">
@@ -3056,7 +3062,7 @@
         <v>21</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
@@ -3064,13 +3070,13 @@
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
       <c r="I28" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="K28" s="7" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="L28" s="1">
         <v>1234</v>
@@ -3079,32 +3085,32 @@
         <v>49</v>
       </c>
       <c r="N28" s="7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="O28" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="P28" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="Q28" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="R28" s="1"/>
       <c r="S28" s="19" t="s">
+        <v>262</v>
+      </c>
+      <c r="T28" s="21" t="s">
+        <v>282</v>
+      </c>
+      <c r="U28" s="25" t="s">
         <v>264</v>
-      </c>
-      <c r="T28" s="21" t="s">
-        <v>284</v>
-      </c>
-      <c r="U28" s="25" t="s">
-        <v>266</v>
       </c>
       <c r="V28" s="21" t="s">
         <v>56</v>
       </c>
       <c r="W28" s="10" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="29" spans="1:23" ht="30" x14ac:dyDescent="0.25">
@@ -3115,7 +3121,7 @@
         <v>22</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
@@ -3123,13 +3129,13 @@
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
       <c r="I29" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J29" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K29" s="7" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="L29" s="1" t="s">
         <v>50</v>
@@ -3138,32 +3144,32 @@
         <v>49</v>
       </c>
       <c r="N29" s="7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="O29" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="P29" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="Q29" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="R29" s="1"/>
       <c r="S29" s="19" t="s">
+        <v>262</v>
+      </c>
+      <c r="T29" s="21" t="s">
+        <v>283</v>
+      </c>
+      <c r="U29" s="25" t="s">
         <v>264</v>
-      </c>
-      <c r="T29" s="21" t="s">
-        <v>285</v>
-      </c>
-      <c r="U29" s="25" t="s">
-        <v>266</v>
       </c>
       <c r="V29" s="21" t="s">
         <v>56</v>
       </c>
       <c r="W29" s="10" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="30" spans="1:23" ht="45" x14ac:dyDescent="0.25">
@@ -3174,7 +3180,7 @@
         <v>23</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
@@ -3182,13 +3188,13 @@
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
       <c r="I30" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="K30" s="7" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="L30" s="1" t="s">
         <v>51</v>
@@ -3197,26 +3203,26 @@
         <v>48</v>
       </c>
       <c r="N30" s="7" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="O30" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="P30" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="Q30" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="R30" s="1"/>
       <c r="S30" s="19" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="T30" s="21" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="U30" s="25" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="V30" s="21" t="s">
         <v>56</v>
@@ -3228,10 +3234,10 @@
         <v>56</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
@@ -3239,47 +3245,47 @@
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
       <c r="I31" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="J31" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="K31" s="7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="L31" s="7" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="M31" s="1" t="s">
         <v>48</v>
       </c>
       <c r="N31" s="7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="O31" s="3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="P31" s="3" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="Q31" s="3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="R31" s="1"/>
       <c r="S31" s="19" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="T31" s="3" t="s">
-        <v>216</v>
+        <v>297</v>
       </c>
       <c r="U31" s="21" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="V31" s="21" t="s">
         <v>56</v>
       </c>
       <c r="W31" s="10" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="32" spans="1:23" ht="45" x14ac:dyDescent="0.25">
@@ -3287,10 +3293,10 @@
         <v>56</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
@@ -3298,45 +3304,45 @@
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
       <c r="I32" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="J32" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="J32" s="1" t="s">
-        <v>206</v>
-      </c>
       <c r="K32" s="7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="L32" s="18" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="M32" s="1" t="s">
         <v>48</v>
       </c>
       <c r="N32" s="7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="O32" s="3" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="P32" s="3" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="Q32" s="3" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="R32" s="1"/>
       <c r="S32" s="20" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="T32" s="26" t="s">
         <v>297</v>
       </c>
       <c r="U32" s="19" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="V32" s="19"/>
       <c r="W32" s="10" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="33" spans="1:23" ht="45" x14ac:dyDescent="0.25">
@@ -3344,55 +3350,55 @@
         <v>54</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C33" s="1"/>
       <c r="D33" s="19" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E33" s="2"/>
       <c r="F33" s="2"/>
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
       <c r="I33" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="J33" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="J33" s="1" t="s">
-        <v>184</v>
-      </c>
       <c r="K33" s="7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="L33" s="1"/>
       <c r="M33" s="1" t="s">
         <v>48</v>
       </c>
       <c r="N33" s="7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="O33" s="3" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="P33" s="3" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="Q33" s="3" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="R33" s="10" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="S33" s="19" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="T33" s="3" t="s">
         <v>297</v>
       </c>
       <c r="U33" s="21" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="V33" s="10" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="W33" s="21"/>
     </row>
@@ -3404,7 +3410,7 @@
         <v>24</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D34" s="2"/>
       <c r="E34" s="2"/>
@@ -3412,50 +3418,50 @@
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
       <c r="I34" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="J34" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="K34" s="7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="L34" s="7" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="M34" s="1" t="s">
         <v>48</v>
       </c>
       <c r="N34" s="7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="O34" s="3" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="P34" s="3" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="Q34" s="3" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="R34" s="1"/>
       <c r="S34" s="19" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="T34" s="3" t="s">
-        <v>217</v>
+        <v>297</v>
       </c>
       <c r="U34" s="21" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="V34" s="21" t="s">
         <v>56</v>
       </c>
       <c r="W34" s="10" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="35" spans="1:23" ht="60" x14ac:dyDescent="0.25">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="35" spans="1:23" ht="45" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>56</v>
       </c>
@@ -3463,7 +3469,7 @@
         <v>25</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D35" s="2"/>
       <c r="E35" s="2"/>
@@ -3471,47 +3477,47 @@
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
       <c r="I35" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="J35" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="K35" s="7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="L35" s="7" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="M35" s="1" t="s">
         <v>48</v>
       </c>
       <c r="N35" s="7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="O35" s="3" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="P35" s="3" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="Q35" s="3" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="R35" s="1"/>
       <c r="S35" s="19" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="T35" s="3" t="s">
-        <v>219</v>
+        <v>297</v>
       </c>
       <c r="U35" s="21" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="V35" s="21" t="s">
         <v>56</v>
       </c>
       <c r="W35" s="10" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="36" spans="1:23" ht="45" x14ac:dyDescent="0.25">
@@ -3522,7 +3528,7 @@
         <v>26</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
@@ -3530,47 +3536,47 @@
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
       <c r="I36" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J36" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="K36" s="7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="L36" s="7" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="M36" s="1" t="s">
         <v>48</v>
       </c>
       <c r="N36" s="7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="O36" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="P36" s="3" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="Q36" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="R36" s="1"/>
       <c r="S36" s="19" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="T36" s="3" t="s">
-        <v>218</v>
+        <v>297</v>
       </c>
       <c r="U36" s="21" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="V36" s="21" t="s">
         <v>56</v>
       </c>
       <c r="W36" s="10" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="37" spans="1:23" ht="45" x14ac:dyDescent="0.25">
@@ -3581,7 +3587,7 @@
         <v>27</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D37" s="2"/>
       <c r="E37" s="2"/>
@@ -3589,45 +3595,45 @@
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
       <c r="I37" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J37" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="K37" s="7" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="L37" s="1"/>
       <c r="M37" s="1" t="s">
         <v>48</v>
       </c>
       <c r="N37" s="7" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="O37" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="P37" s="1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="Q37" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="R37" s="1"/>
       <c r="S37" s="19" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="T37" s="1" t="s">
-        <v>180</v>
+        <v>298</v>
       </c>
       <c r="U37" s="21" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="V37" s="21" t="s">
         <v>56</v>
       </c>
       <c r="W37" s="10" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="38" spans="1:23" ht="45" x14ac:dyDescent="0.25">
@@ -3638,7 +3644,7 @@
         <v>28</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D38" s="2"/>
       <c r="E38" s="2"/>
@@ -3646,13 +3652,13 @@
       <c r="G38" s="2"/>
       <c r="H38" s="2"/>
       <c r="I38" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J38" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="K38" s="7" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="L38" s="20" t="s">
         <v>53</v>
@@ -3661,32 +3667,32 @@
         <v>48</v>
       </c>
       <c r="N38" s="7" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="O38" s="7" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="P38" s="7" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="Q38" s="7" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="R38" s="1"/>
       <c r="S38" s="19" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="T38" s="21" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="U38" s="21" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="V38" s="21" t="s">
         <v>56</v>
       </c>
       <c r="W38" s="10" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="39" spans="1:23" ht="30" x14ac:dyDescent="0.25">
@@ -3697,7 +3703,7 @@
         <v>12</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D39" s="2"/>
       <c r="E39" s="2"/>
@@ -3705,13 +3711,13 @@
       <c r="G39" s="2"/>
       <c r="H39" s="2"/>
       <c r="I39" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J39" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="K39" s="7" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="L39" s="20" t="s">
         <v>53</v>
@@ -3720,32 +3726,32 @@
         <v>48</v>
       </c>
       <c r="N39" s="7" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="O39" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="P39" s="7" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="Q39" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="R39" s="1"/>
       <c r="S39" s="19" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="T39" s="21" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="U39" s="21" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="V39" s="21" t="s">
         <v>56</v>
       </c>
       <c r="W39" s="10" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="40" spans="1:23" ht="30" x14ac:dyDescent="0.25">
@@ -3756,7 +3762,7 @@
         <v>29</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D40" s="2"/>
       <c r="E40" s="2"/>
@@ -3764,13 +3770,13 @@
       <c r="G40" s="2"/>
       <c r="H40" s="2"/>
       <c r="I40" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="J40" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="K40" s="7" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="L40" s="20" t="s">
         <v>52</v>
@@ -3779,32 +3785,32 @@
         <v>48</v>
       </c>
       <c r="N40" s="7" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="O40" s="7" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="P40" s="7" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="Q40" s="7" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="R40" s="1"/>
       <c r="S40" s="19" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="T40" s="21" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="U40" s="21" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="V40" s="21" t="s">
         <v>56</v>
       </c>
       <c r="W40" s="10" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="41" spans="1:23" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Code Version 2205202 13:02
</commit_message>
<xml_diff>
--- a/Prime_Job_Automation/Configuration/RuleFactory/Master Rule Factory.xlsx
+++ b/Prime_Job_Automation/Configuration/RuleFactory/Master Rule Factory.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\PJA\Prime_Job_Automation\Configuration\RuleFactory\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFE03011-776D-4338-A20F-E119685312DB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D357C2E-3DC5-4FE6-8D77-0D8A222E7211}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" tabRatio="351" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1514,7 +1514,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D1" sqref="D1"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Code Version 2205202 21:11
</commit_message>
<xml_diff>
--- a/Prime_Job_Automation/Configuration/RuleFactory/Master Rule Factory.xlsx
+++ b/Prime_Job_Automation/Configuration/RuleFactory/Master Rule Factory.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\PJA\Prime_Job_Automation\Configuration\RuleFactory\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D357C2E-3DC5-4FE6-8D77-0D8A222E7211}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22FF7554-2E04-4B60-8C86-C8EAF10FD19E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" tabRatio="351" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -812,12 +812,6 @@
     <t>^TransactionMonetary_bayantel_\d\d\d\d\d\d\d\d.dat$</t>
   </si>
   <si>
-    <t>UBP Enr Response Maynilad</t>
-  </si>
-  <si>
-    <t>UBP Enr Response Veco Enrollment</t>
-  </si>
-  <si>
     <t>Bridge File</t>
   </si>
   <si>
@@ -827,12 +821,6 @@
     <t>IPM Incoming file</t>
   </si>
   <si>
-    <t>UBP Enr Response Meralco</t>
-  </si>
-  <si>
-    <t>UBP Enr Response Bayantel</t>
-  </si>
-  <si>
     <t>UBP Getgo Accrual Response</t>
   </si>
   <si>
@@ -969,6 +957,18 @@
   </si>
   <si>
     <t>Return_File_Email_Id</t>
+  </si>
+  <si>
+    <t>UBP Enr Response (MAYNILAD)</t>
+  </si>
+  <si>
+    <t>UBP Enr Response (MERALCO)</t>
+  </si>
+  <si>
+    <t>UBP Enr Response (BAYANTEL)</t>
+  </si>
+  <si>
+    <t>UBP Enr Response (VECO)</t>
   </si>
 </sst>
 </file>
@@ -1546,7 +1546,7 @@
         <v>57</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>58</v>
@@ -1597,19 +1597,19 @@
         <v>134</v>
       </c>
       <c r="S1" s="4" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="T1" s="4" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="U1" s="4" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="V1" s="4" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="W1" s="4" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
     </row>
     <row r="2" spans="1:23" ht="30" x14ac:dyDescent="0.25">
@@ -1656,16 +1656,16 @@
         <v>152</v>
       </c>
       <c r="S2" s="24" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="T2" s="21" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="U2" s="25" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="V2" s="10" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="W2" s="21"/>
     </row>
@@ -1704,7 +1704,7 @@
         <v>172</v>
       </c>
       <c r="P3" s="7" t="s">
-        <v>248</v>
+        <v>297</v>
       </c>
       <c r="Q3" s="7" t="s">
         <v>172</v>
@@ -1713,16 +1713,16 @@
         <v>152</v>
       </c>
       <c r="S3" s="7" t="s">
+        <v>258</v>
+      </c>
+      <c r="T3" s="21" t="s">
+        <v>261</v>
+      </c>
+      <c r="U3" s="25" t="s">
         <v>262</v>
       </c>
-      <c r="T3" s="21" t="s">
-        <v>265</v>
-      </c>
-      <c r="U3" s="25" t="s">
-        <v>266</v>
-      </c>
       <c r="V3" s="10" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="W3" s="21"/>
     </row>
@@ -1770,16 +1770,16 @@
         <v>152</v>
       </c>
       <c r="S4" s="17" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="T4" s="21" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="U4" s="25" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="V4" s="10" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="W4" s="21"/>
     </row>
@@ -1827,7 +1827,7 @@
         <v>152</v>
       </c>
       <c r="S5" s="17" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="T5" s="21"/>
       <c r="U5" s="21"/>
@@ -1869,7 +1869,7 @@
         <v>173</v>
       </c>
       <c r="P6" s="7" t="s">
-        <v>249</v>
+        <v>300</v>
       </c>
       <c r="Q6" s="7" t="s">
         <v>173</v>
@@ -1878,16 +1878,16 @@
         <v>152</v>
       </c>
       <c r="S6" s="17" t="s">
+        <v>258</v>
+      </c>
+      <c r="T6" s="21" t="s">
+        <v>265</v>
+      </c>
+      <c r="U6" s="25" t="s">
         <v>262</v>
       </c>
-      <c r="T6" s="21" t="s">
-        <v>269</v>
-      </c>
-      <c r="U6" s="25" t="s">
-        <v>266</v>
-      </c>
       <c r="V6" s="10" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="W6" s="21"/>
     </row>
@@ -1935,7 +1935,7 @@
         <v>152</v>
       </c>
       <c r="S7" s="17" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="T7" s="21"/>
       <c r="U7" s="21"/>
@@ -1977,7 +1977,7 @@
         <v>136</v>
       </c>
       <c r="P8" s="7" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="Q8" s="7" t="s">
         <v>136</v>
@@ -1986,7 +1986,7 @@
         <v>152</v>
       </c>
       <c r="S8" s="17" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="T8" s="21"/>
       <c r="U8" s="21"/>
@@ -2028,7 +2028,7 @@
         <v>175</v>
       </c>
       <c r="P9" s="7" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="Q9" s="7" t="s">
         <v>175</v>
@@ -2037,7 +2037,7 @@
         <v>152</v>
       </c>
       <c r="S9" s="17" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="T9" s="21"/>
       <c r="U9" s="21"/>
@@ -2079,7 +2079,7 @@
         <v>176</v>
       </c>
       <c r="P10" s="7" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="Q10" s="7" t="s">
         <v>176</v>
@@ -2088,7 +2088,7 @@
         <v>152</v>
       </c>
       <c r="S10" s="17" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="T10" s="21"/>
       <c r="U10" s="21"/>
@@ -2139,7 +2139,7 @@
         <v>152</v>
       </c>
       <c r="S11" s="17" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="T11" s="21"/>
       <c r="U11" s="21"/>
@@ -2190,7 +2190,7 @@
         <v>152</v>
       </c>
       <c r="S12" s="17" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="T12" s="21"/>
       <c r="U12" s="21"/>
@@ -2241,7 +2241,7 @@
         <v>152</v>
       </c>
       <c r="S13" s="17" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="T13" s="21"/>
       <c r="U13" s="21"/>
@@ -2292,7 +2292,7 @@
         <v>152</v>
       </c>
       <c r="S14" s="17" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="T14" s="21"/>
       <c r="U14" s="21"/>
@@ -2334,7 +2334,7 @@
         <v>140</v>
       </c>
       <c r="P15" s="7" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="Q15" s="7" t="s">
         <v>140</v>
@@ -2343,16 +2343,16 @@
         <v>152</v>
       </c>
       <c r="S15" s="7" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="T15" s="21" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="U15" s="21" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="V15" s="10" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="W15" s="21"/>
     </row>
@@ -2391,7 +2391,7 @@
         <v>180</v>
       </c>
       <c r="P16" s="7" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="Q16" s="7" t="s">
         <v>180</v>
@@ -2400,16 +2400,16 @@
         <v>152</v>
       </c>
       <c r="S16" s="17" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="T16" s="21" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="U16" s="21" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="V16" s="10" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="W16" s="21"/>
     </row>
@@ -2457,16 +2457,16 @@
         <v>152</v>
       </c>
       <c r="S17" s="17" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="T17" s="21" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="U17" s="25" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="V17" s="10" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="W17" s="21"/>
     </row>
@@ -2514,7 +2514,7 @@
         <v>152</v>
       </c>
       <c r="S18" s="17" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="T18" s="21"/>
       <c r="U18" s="21"/>
@@ -2565,7 +2565,7 @@
         <v>152</v>
       </c>
       <c r="S19" s="17" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="T19" s="21"/>
       <c r="U19" s="21"/>
@@ -2616,7 +2616,7 @@
         <v>152</v>
       </c>
       <c r="S20" s="17" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="T20" s="21"/>
       <c r="U20" s="21"/>
@@ -2675,16 +2675,16 @@
         <v>152</v>
       </c>
       <c r="S21" s="17" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="T21" s="21" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="U21" s="25" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="V21" s="21" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="W21" s="21"/>
     </row>
@@ -2731,7 +2731,7 @@
         <v>143</v>
       </c>
       <c r="P22" s="1" t="s">
-        <v>253</v>
+        <v>298</v>
       </c>
       <c r="Q22" s="1" t="s">
         <v>143</v>
@@ -2740,16 +2740,16 @@
         <v>152</v>
       </c>
       <c r="S22" s="17" t="s">
+        <v>258</v>
+      </c>
+      <c r="T22" s="21" t="s">
+        <v>271</v>
+      </c>
+      <c r="U22" s="25" t="s">
         <v>262</v>
       </c>
-      <c r="T22" s="21" t="s">
-        <v>275</v>
-      </c>
-      <c r="U22" s="25" t="s">
-        <v>266</v>
-      </c>
       <c r="V22" s="21" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="W22" s="21"/>
     </row>
@@ -2805,16 +2805,16 @@
         <v>152</v>
       </c>
       <c r="S23" s="19" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="T23" s="21" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="U23" s="25" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="V23" s="21" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="W23" s="21"/>
     </row>
@@ -2870,16 +2870,16 @@
         <v>152</v>
       </c>
       <c r="S24" s="19" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="T24" s="21" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="U24" s="25" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="V24" s="21" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="W24" s="21"/>
     </row>
@@ -2916,7 +2916,7 @@
         <v>169</v>
       </c>
       <c r="L25" s="1" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="M25" s="1" t="s">
         <v>49</v>
@@ -2937,7 +2937,7 @@
         <v>152</v>
       </c>
       <c r="S25" s="17" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="T25" s="21"/>
       <c r="U25" s="21"/>
@@ -2988,7 +2988,7 @@
         <v>152</v>
       </c>
       <c r="S26" s="17" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="T26" s="21"/>
       <c r="U26" s="21"/>
@@ -3039,19 +3039,19 @@
       </c>
       <c r="R27" s="1"/>
       <c r="S27" s="19" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="T27" s="21" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="U27" s="25" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="V27" s="21" t="s">
         <v>56</v>
       </c>
       <c r="W27" s="10" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
     </row>
     <row r="28" spans="1:23" ht="30" x14ac:dyDescent="0.25">
@@ -3098,19 +3098,19 @@
       </c>
       <c r="R28" s="1"/>
       <c r="S28" s="19" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="T28" s="21" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="U28" s="25" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="V28" s="21" t="s">
         <v>56</v>
       </c>
       <c r="W28" s="10" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
     </row>
     <row r="29" spans="1:23" ht="30" x14ac:dyDescent="0.25">
@@ -3157,19 +3157,19 @@
       </c>
       <c r="R29" s="1"/>
       <c r="S29" s="19" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="T29" s="21" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="U29" s="25" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="V29" s="21" t="s">
         <v>56</v>
       </c>
       <c r="W29" s="10" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
     </row>
     <row r="30" spans="1:23" ht="45" x14ac:dyDescent="0.25">
@@ -3209,20 +3209,20 @@
         <v>148</v>
       </c>
       <c r="P30" s="1" t="s">
-        <v>254</v>
+        <v>299</v>
       </c>
       <c r="Q30" s="1" t="s">
         <v>148</v>
       </c>
       <c r="R30" s="1"/>
       <c r="S30" s="19" t="s">
+        <v>258</v>
+      </c>
+      <c r="T30" s="21" t="s">
+        <v>280</v>
+      </c>
+      <c r="U30" s="25" t="s">
         <v>262</v>
-      </c>
-      <c r="T30" s="21" t="s">
-        <v>284</v>
-      </c>
-      <c r="U30" s="25" t="s">
-        <v>266</v>
       </c>
       <c r="V30" s="21" t="s">
         <v>56</v>
@@ -3273,19 +3273,19 @@
       </c>
       <c r="R31" s="1"/>
       <c r="S31" s="19" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="T31" s="3" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="U31" s="21" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="V31" s="21" t="s">
         <v>56</v>
       </c>
       <c r="W31" s="10" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
     </row>
     <row r="32" spans="1:23" ht="45" x14ac:dyDescent="0.25">
@@ -3322,27 +3322,27 @@
         <v>198</v>
       </c>
       <c r="O32" s="3" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="P32" s="3" t="s">
         <v>234</v>
       </c>
       <c r="Q32" s="3" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="R32" s="1"/>
       <c r="S32" s="20" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="T32" s="26" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="U32" s="19" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="V32" s="19"/>
       <c r="W32" s="10" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
     </row>
     <row r="33" spans="1:23" ht="45" x14ac:dyDescent="0.25">
@@ -3377,28 +3377,28 @@
         <v>198</v>
       </c>
       <c r="O33" s="3" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="P33" s="3" t="s">
         <v>234</v>
       </c>
       <c r="Q33" s="3" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="R33" s="10" t="s">
         <v>152</v>
       </c>
       <c r="S33" s="19" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="T33" s="3" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="U33" s="21" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="V33" s="10" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="W33" s="21"/>
     </row>
@@ -3446,19 +3446,19 @@
       </c>
       <c r="R34" s="1"/>
       <c r="S34" s="19" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="T34" s="3" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="U34" s="21" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="V34" s="21" t="s">
         <v>56</v>
       </c>
       <c r="W34" s="10" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
     </row>
     <row r="35" spans="1:23" ht="45" x14ac:dyDescent="0.25">
@@ -3505,19 +3505,19 @@
       </c>
       <c r="R35" s="1"/>
       <c r="S35" s="19" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="T35" s="3" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="U35" s="21" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="V35" s="21" t="s">
         <v>56</v>
       </c>
       <c r="W35" s="10" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
     </row>
     <row r="36" spans="1:23" ht="45" x14ac:dyDescent="0.25">
@@ -3564,19 +3564,19 @@
       </c>
       <c r="R36" s="1"/>
       <c r="S36" s="19" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="T36" s="3" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="U36" s="21" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="V36" s="21" t="s">
         <v>56</v>
       </c>
       <c r="W36" s="10" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
     </row>
     <row r="37" spans="1:23" ht="45" x14ac:dyDescent="0.25">
@@ -3614,26 +3614,26 @@
         <v>179</v>
       </c>
       <c r="P37" s="1" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="Q37" s="1" t="s">
         <v>179</v>
       </c>
       <c r="R37" s="1"/>
       <c r="S37" s="19" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="T37" s="1" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="U37" s="21" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="V37" s="21" t="s">
         <v>56</v>
       </c>
       <c r="W37" s="10" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
     </row>
     <row r="38" spans="1:23" ht="45" x14ac:dyDescent="0.25">
@@ -3673,26 +3673,26 @@
         <v>149</v>
       </c>
       <c r="P38" s="7" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="Q38" s="7" t="s">
         <v>149</v>
       </c>
       <c r="R38" s="1"/>
       <c r="S38" s="19" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="T38" s="21" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="U38" s="21" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="V38" s="21" t="s">
         <v>56</v>
       </c>
       <c r="W38" s="10" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
     </row>
     <row r="39" spans="1:23" ht="30" x14ac:dyDescent="0.25">
@@ -3732,26 +3732,26 @@
         <v>151</v>
       </c>
       <c r="P39" s="7" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="Q39" s="1" t="s">
         <v>151</v>
       </c>
       <c r="R39" s="1"/>
       <c r="S39" s="19" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="T39" s="21" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="U39" s="21" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="V39" s="21" t="s">
         <v>56</v>
       </c>
       <c r="W39" s="10" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
     </row>
     <row r="40" spans="1:23" ht="30" x14ac:dyDescent="0.25">
@@ -3791,26 +3791,26 @@
         <v>150</v>
       </c>
       <c r="P40" s="7" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="Q40" s="7" t="s">
         <v>150</v>
       </c>
       <c r="R40" s="1"/>
       <c r="S40" s="19" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="T40" s="21" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="U40" s="21" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="V40" s="21" t="s">
         <v>56</v>
       </c>
       <c r="W40" s="10" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
     </row>
     <row r="41" spans="1:23" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Code Version 26052020 1654
</commit_message>
<xml_diff>
--- a/Prime_Job_Automation/Configuration/RuleFactory/Master Rule Factory.xlsx
+++ b/Prime_Job_Automation/Configuration/RuleFactory/Master Rule Factory.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\PJA\Prime_Job_Automation\Configuration\RuleFactory\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A016CD3B-73BC-4CA2-BA27-4D2487B7EC1D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E9467F9-55F5-4621-BC00-08FCB7ED92C8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" tabRatio="351" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1514,7 +1514,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="topRight" activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Code Version 29052020 0234
</commit_message>
<xml_diff>
--- a/Prime_Job_Automation/Configuration/RuleFactory/Master Rule Factory.xlsx
+++ b/Prime_Job_Automation/Configuration/RuleFactory/Master Rule Factory.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\PJA\Prime_Job_Automation\Configuration\RuleFactory\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E9467F9-55F5-4621-BC00-08FCB7ED92C8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30E2AD08-7B51-4EA4-B410-AFEB652114DD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" tabRatio="351" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -767,51 +767,9 @@
     <t>TSYS_PJA_Menu_Hierarchy</t>
   </si>
   <si>
-    <t>^TransactionMonetary_meralco_\d\d\d\d\d\d\d\d.dat$</t>
-  </si>
-  <si>
     <t>Monetary Transaction Interface</t>
   </si>
   <si>
-    <t>^TransactionMonetary_maynilad_\d\d\d\d\d\d\d\d.dat$</t>
-  </si>
-  <si>
-    <t>^TransactionMonetary_smart_\d\d\d\d\d\d\d\d.dat$</t>
-  </si>
-  <si>
-    <t>^TransactionMonetary_sun_cellular_\d\d\d\d\d\d\d\d.dat$</t>
-  </si>
-  <si>
-    <t>^TransactionMonetary_sm_\d\d\d\d\d\d\d\d.dat$</t>
-  </si>
-  <si>
-    <t>^TransactionMonetary_branch_payment_\d\d\d\d\d\d\d\d.dat$</t>
-  </si>
-  <si>
-    <t>^TransactionMonetary_veco_\d\d\d\d\d\d\d\d.dat$</t>
-  </si>
-  <si>
-    <t>^TransactionMonetary_auto_debit_\d\d\d\d\d\d\d\d.dat$</t>
-  </si>
-  <si>
-    <t>^TransactionMonetary_pldt_\d\d\d\d\d\d\d\d.dat$</t>
-  </si>
-  <si>
-    <t>^TransactionMonetary_bpi_\d\d\d\d\d\d\d\d.dat$</t>
-  </si>
-  <si>
-    <t>^TransactionMonetary_cash_advance_\d\d\d\d\d\d\d\d.dat$</t>
-  </si>
-  <si>
-    <t>^TransactionMonetary_sky_cable_\d\d\d\d\d\d\d\d.dat$</t>
-  </si>
-  <si>
-    <t>^TransactionMonetary_globe_\d\d\d\d\d\d\d\d.dat$</t>
-  </si>
-  <si>
-    <t>^TransactionMonetary_bayantel_\d\d\d\d\d\d\d\d.dat$</t>
-  </si>
-  <si>
     <t>Bridge File</t>
   </si>
   <si>
@@ -969,6 +927,48 @@
   </si>
   <si>
     <t>UBP Enr Response (VECO)</t>
+  </si>
+  <si>
+    <t>^TransactionMonetary_maynilad_\d\d\d\d\d\d\d\d\d\d\d\d\d\d.dat$</t>
+  </si>
+  <si>
+    <t>^TransactionMonetary_veco_\d\d\d\d\d\d\d\d\d\d\d\d\d\d.dat$</t>
+  </si>
+  <si>
+    <t>^TransactionMonetary_branch_payment_\d\d\d\d\d\d\d\d\d\d\d\d\d\d.dat$</t>
+  </si>
+  <si>
+    <t>^TransactionMonetary_auto_debit_\d\d\d\d\d\d\d\d\d\d\d\d\d\d.dat$</t>
+  </si>
+  <si>
+    <t>^TransactionMonetary_cash_advance_\d\d\d\d\d\d\d\d\d\d\d\d\d\d.dat$</t>
+  </si>
+  <si>
+    <t>^TransactionMonetary_pldt_\d\d\d\d\d\d\d\d\d\d\d\d\d\d.dat$</t>
+  </si>
+  <si>
+    <t>^TransactionMonetary_bpi_\d\d\d\d\d\d\d\d\d\d\d\d\d\d.dat$</t>
+  </si>
+  <si>
+    <t>^TransactionMonetary_meralco_\d\d\d\d\d\d\d\d\d\d\d\d\d\d.dat$</t>
+  </si>
+  <si>
+    <t>^TransactionMonetary_smart_\d\d\d\d\d\d\d\d\d\d\d\d\d\d.dat$</t>
+  </si>
+  <si>
+    <t>^TransactionMonetary_sun_cellular_\d\d\d\d\d\d\d\d\d\d\d\d\d\d.dat$</t>
+  </si>
+  <si>
+    <t>^TransactionMonetary_sm_\d\d\d\d\d\d\d\d\d\d\d\d\d\d.dat$</t>
+  </si>
+  <si>
+    <t>^TransactionMonetary_sky_cable_\d\d\d\d\d\d\d\d\d\d\d\d\d\d.dat$</t>
+  </si>
+  <si>
+    <t>^TransactionMonetary_globe_\d\d\d\d\d\d\d\d\d\d\d\d\d\d.dat$</t>
+  </si>
+  <si>
+    <t>^TransactionMonetary_bayantel_\d\d\d\d\d\d\d\d\d\d\d\d\d\d.dat$</t>
   </si>
 </sst>
 </file>
@@ -1514,7 +1514,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A41" sqref="A41"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1546,7 +1546,7 @@
         <v>57</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>295</v>
+        <v>281</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>58</v>
@@ -1597,19 +1597,19 @@
         <v>134</v>
       </c>
       <c r="S1" s="4" t="s">
-        <v>254</v>
+        <v>240</v>
       </c>
       <c r="T1" s="4" t="s">
-        <v>257</v>
+        <v>243</v>
       </c>
       <c r="U1" s="4" t="s">
-        <v>255</v>
+        <v>241</v>
       </c>
       <c r="V1" s="4" t="s">
-        <v>256</v>
+        <v>242</v>
       </c>
       <c r="W1" s="4" t="s">
-        <v>296</v>
+        <v>282</v>
       </c>
     </row>
     <row r="2" spans="1:23" ht="30" x14ac:dyDescent="0.25">
@@ -1644,10 +1644,10 @@
         <v>198</v>
       </c>
       <c r="O2" s="7" t="s">
-        <v>235</v>
+        <v>287</v>
       </c>
       <c r="P2" s="7" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="Q2" s="7" t="s">
         <v>228</v>
@@ -1656,16 +1656,16 @@
         <v>152</v>
       </c>
       <c r="S2" s="24" t="s">
-        <v>258</v>
+        <v>244</v>
       </c>
       <c r="T2" s="21" t="s">
-        <v>259</v>
+        <v>245</v>
       </c>
       <c r="U2" s="25" t="s">
-        <v>260</v>
+        <v>246</v>
       </c>
       <c r="V2" s="10" t="s">
-        <v>285</v>
+        <v>271</v>
       </c>
       <c r="W2" s="21"/>
     </row>
@@ -1704,7 +1704,7 @@
         <v>172</v>
       </c>
       <c r="P3" s="7" t="s">
-        <v>297</v>
+        <v>283</v>
       </c>
       <c r="Q3" s="7" t="s">
         <v>172</v>
@@ -1713,16 +1713,16 @@
         <v>152</v>
       </c>
       <c r="S3" s="7" t="s">
-        <v>258</v>
+        <v>244</v>
       </c>
       <c r="T3" s="21" t="s">
-        <v>261</v>
+        <v>247</v>
       </c>
       <c r="U3" s="25" t="s">
-        <v>262</v>
+        <v>248</v>
       </c>
       <c r="V3" s="10" t="s">
-        <v>286</v>
+        <v>272</v>
       </c>
       <c r="W3" s="21"/>
     </row>
@@ -1758,10 +1758,10 @@
         <v>198</v>
       </c>
       <c r="O4" s="7" t="s">
-        <v>240</v>
+        <v>288</v>
       </c>
       <c r="P4" s="7" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="Q4" s="7" t="s">
         <v>229</v>
@@ -1770,16 +1770,16 @@
         <v>152</v>
       </c>
       <c r="S4" s="17" t="s">
-        <v>258</v>
+        <v>244</v>
       </c>
       <c r="T4" s="21" t="s">
-        <v>263</v>
+        <v>249</v>
       </c>
       <c r="U4" s="25" t="s">
-        <v>260</v>
+        <v>246</v>
       </c>
       <c r="V4" s="10" t="s">
-        <v>287</v>
+        <v>273</v>
       </c>
       <c r="W4" s="21"/>
     </row>
@@ -1815,10 +1815,10 @@
         <v>198</v>
       </c>
       <c r="O5" s="7" t="s">
-        <v>239</v>
+        <v>289</v>
       </c>
       <c r="P5" s="7" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="Q5" s="7" t="s">
         <v>135</v>
@@ -1827,7 +1827,7 @@
         <v>152</v>
       </c>
       <c r="S5" s="17" t="s">
-        <v>264</v>
+        <v>250</v>
       </c>
       <c r="T5" s="21"/>
       <c r="U5" s="21"/>
@@ -1869,7 +1869,7 @@
         <v>173</v>
       </c>
       <c r="P6" s="7" t="s">
-        <v>300</v>
+        <v>286</v>
       </c>
       <c r="Q6" s="7" t="s">
         <v>173</v>
@@ -1878,16 +1878,16 @@
         <v>152</v>
       </c>
       <c r="S6" s="17" t="s">
-        <v>258</v>
+        <v>244</v>
       </c>
       <c r="T6" s="21" t="s">
-        <v>265</v>
+        <v>251</v>
       </c>
       <c r="U6" s="25" t="s">
-        <v>262</v>
+        <v>248</v>
       </c>
       <c r="V6" s="10" t="s">
-        <v>288</v>
+        <v>274</v>
       </c>
       <c r="W6" s="21"/>
     </row>
@@ -1923,10 +1923,10 @@
         <v>198</v>
       </c>
       <c r="O7" s="7" t="s">
-        <v>241</v>
+        <v>290</v>
       </c>
       <c r="P7" s="7" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="Q7" s="7" t="s">
         <v>174</v>
@@ -1935,7 +1935,7 @@
         <v>152</v>
       </c>
       <c r="S7" s="17" t="s">
-        <v>264</v>
+        <v>250</v>
       </c>
       <c r="T7" s="21"/>
       <c r="U7" s="21"/>
@@ -1977,7 +1977,7 @@
         <v>136</v>
       </c>
       <c r="P8" s="7" t="s">
-        <v>248</v>
+        <v>234</v>
       </c>
       <c r="Q8" s="7" t="s">
         <v>136</v>
@@ -1986,7 +1986,7 @@
         <v>152</v>
       </c>
       <c r="S8" s="17" t="s">
-        <v>264</v>
+        <v>250</v>
       </c>
       <c r="T8" s="21"/>
       <c r="U8" s="21"/>
@@ -2028,7 +2028,7 @@
         <v>175</v>
       </c>
       <c r="P9" s="7" t="s">
-        <v>249</v>
+        <v>235</v>
       </c>
       <c r="Q9" s="7" t="s">
         <v>175</v>
@@ -2037,7 +2037,7 @@
         <v>152</v>
       </c>
       <c r="S9" s="17" t="s">
-        <v>264</v>
+        <v>250</v>
       </c>
       <c r="T9" s="21"/>
       <c r="U9" s="21"/>
@@ -2079,7 +2079,7 @@
         <v>176</v>
       </c>
       <c r="P10" s="7" t="s">
-        <v>250</v>
+        <v>236</v>
       </c>
       <c r="Q10" s="7" t="s">
         <v>176</v>
@@ -2088,7 +2088,7 @@
         <v>152</v>
       </c>
       <c r="S10" s="17" t="s">
-        <v>264</v>
+        <v>250</v>
       </c>
       <c r="T10" s="21"/>
       <c r="U10" s="21"/>
@@ -2127,10 +2127,10 @@
         <v>198</v>
       </c>
       <c r="O11" s="7" t="s">
-        <v>244</v>
+        <v>291</v>
       </c>
       <c r="P11" s="7" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="Q11" s="7" t="s">
         <v>137</v>
@@ -2139,7 +2139,7 @@
         <v>152</v>
       </c>
       <c r="S11" s="17" t="s">
-        <v>264</v>
+        <v>250</v>
       </c>
       <c r="T11" s="21"/>
       <c r="U11" s="21"/>
@@ -2178,10 +2178,10 @@
         <v>198</v>
       </c>
       <c r="O12" s="7" t="s">
-        <v>239</v>
+        <v>289</v>
       </c>
       <c r="P12" s="7" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="Q12" s="7" t="s">
         <v>138</v>
@@ -2190,7 +2190,7 @@
         <v>152</v>
       </c>
       <c r="S12" s="17" t="s">
-        <v>264</v>
+        <v>250</v>
       </c>
       <c r="T12" s="21"/>
       <c r="U12" s="21"/>
@@ -2229,10 +2229,10 @@
         <v>198</v>
       </c>
       <c r="O13" s="7" t="s">
-        <v>239</v>
+        <v>289</v>
       </c>
       <c r="P13" s="7" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="Q13" s="7" t="s">
         <v>139</v>
@@ -2241,7 +2241,7 @@
         <v>152</v>
       </c>
       <c r="S13" s="17" t="s">
-        <v>264</v>
+        <v>250</v>
       </c>
       <c r="T13" s="21"/>
       <c r="U13" s="21"/>
@@ -2283,7 +2283,7 @@
         <v>178</v>
       </c>
       <c r="P14" s="7" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="Q14" s="7" t="s">
         <v>178</v>
@@ -2292,7 +2292,7 @@
         <v>152</v>
       </c>
       <c r="S14" s="17" t="s">
-        <v>264</v>
+        <v>250</v>
       </c>
       <c r="T14" s="21"/>
       <c r="U14" s="21"/>
@@ -2334,7 +2334,7 @@
         <v>140</v>
       </c>
       <c r="P15" s="7" t="s">
-        <v>248</v>
+        <v>234</v>
       </c>
       <c r="Q15" s="7" t="s">
         <v>140</v>
@@ -2343,16 +2343,16 @@
         <v>152</v>
       </c>
       <c r="S15" s="7" t="s">
-        <v>266</v>
+        <v>252</v>
       </c>
       <c r="T15" s="21" t="s">
-        <v>264</v>
+        <v>250</v>
       </c>
       <c r="U15" s="21" t="s">
-        <v>267</v>
+        <v>253</v>
       </c>
       <c r="V15" s="10" t="s">
-        <v>283</v>
+        <v>269</v>
       </c>
       <c r="W15" s="21"/>
     </row>
@@ -2391,7 +2391,7 @@
         <v>180</v>
       </c>
       <c r="P16" s="7" t="s">
-        <v>290</v>
+        <v>276</v>
       </c>
       <c r="Q16" s="7" t="s">
         <v>180</v>
@@ -2400,16 +2400,16 @@
         <v>152</v>
       </c>
       <c r="S16" s="17" t="s">
-        <v>266</v>
+        <v>252</v>
       </c>
       <c r="T16" s="21" t="s">
-        <v>264</v>
+        <v>250</v>
       </c>
       <c r="U16" s="21" t="s">
-        <v>267</v>
+        <v>253</v>
       </c>
       <c r="V16" s="10" t="s">
-        <v>282</v>
+        <v>268</v>
       </c>
       <c r="W16" s="21"/>
     </row>
@@ -2445,10 +2445,10 @@
         <v>198</v>
       </c>
       <c r="O17" s="7" t="s">
-        <v>242</v>
+        <v>292</v>
       </c>
       <c r="P17" s="7" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="Q17" s="7" t="s">
         <v>171</v>
@@ -2457,16 +2457,16 @@
         <v>152</v>
       </c>
       <c r="S17" s="17" t="s">
-        <v>258</v>
+        <v>244</v>
       </c>
       <c r="T17" s="21" t="s">
-        <v>268</v>
+        <v>254</v>
       </c>
       <c r="U17" s="25" t="s">
-        <v>260</v>
+        <v>246</v>
       </c>
       <c r="V17" s="10" t="s">
-        <v>289</v>
+        <v>275</v>
       </c>
       <c r="W17" s="21"/>
     </row>
@@ -2502,10 +2502,10 @@
         <v>198</v>
       </c>
       <c r="O18" s="7" t="s">
-        <v>239</v>
+        <v>289</v>
       </c>
       <c r="P18" s="7" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="Q18" s="7" t="s">
         <v>230</v>
@@ -2514,7 +2514,7 @@
         <v>152</v>
       </c>
       <c r="S18" s="17" t="s">
-        <v>264</v>
+        <v>250</v>
       </c>
       <c r="T18" s="21"/>
       <c r="U18" s="21"/>
@@ -2553,10 +2553,10 @@
         <v>198</v>
       </c>
       <c r="O19" s="7" t="s">
-        <v>243</v>
+        <v>293</v>
       </c>
       <c r="P19" s="7" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="Q19" s="7" t="s">
         <v>141</v>
@@ -2565,7 +2565,7 @@
         <v>152</v>
       </c>
       <c r="S19" s="17" t="s">
-        <v>264</v>
+        <v>250</v>
       </c>
       <c r="T19" s="21"/>
       <c r="U19" s="21"/>
@@ -2607,7 +2607,7 @@
         <v>227</v>
       </c>
       <c r="P20" s="7" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="Q20" s="7" t="s">
         <v>227</v>
@@ -2616,7 +2616,7 @@
         <v>152</v>
       </c>
       <c r="S20" s="17" t="s">
-        <v>264</v>
+        <v>250</v>
       </c>
       <c r="T20" s="21"/>
       <c r="U20" s="21"/>
@@ -2663,10 +2663,10 @@
         <v>198</v>
       </c>
       <c r="O21" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="P21" s="1" t="s">
         <v>233</v>
-      </c>
-      <c r="P21" s="1" t="s">
-        <v>234</v>
       </c>
       <c r="Q21" s="1" t="s">
         <v>142</v>
@@ -2675,16 +2675,16 @@
         <v>152</v>
       </c>
       <c r="S21" s="17" t="s">
-        <v>258</v>
+        <v>244</v>
       </c>
       <c r="T21" s="21" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="U21" s="25" t="s">
-        <v>260</v>
+        <v>246</v>
       </c>
       <c r="V21" s="21" t="s">
-        <v>270</v>
+        <v>256</v>
       </c>
       <c r="W21" s="21"/>
     </row>
@@ -2731,7 +2731,7 @@
         <v>143</v>
       </c>
       <c r="P22" s="1" t="s">
-        <v>298</v>
+        <v>284</v>
       </c>
       <c r="Q22" s="1" t="s">
         <v>143</v>
@@ -2740,16 +2740,16 @@
         <v>152</v>
       </c>
       <c r="S22" s="17" t="s">
+        <v>244</v>
+      </c>
+      <c r="T22" s="21" t="s">
+        <v>257</v>
+      </c>
+      <c r="U22" s="25" t="s">
+        <v>248</v>
+      </c>
+      <c r="V22" s="21" t="s">
         <v>258</v>
-      </c>
-      <c r="T22" s="21" t="s">
-        <v>271</v>
-      </c>
-      <c r="U22" s="25" t="s">
-        <v>262</v>
-      </c>
-      <c r="V22" s="21" t="s">
-        <v>272</v>
       </c>
       <c r="W22" s="21"/>
     </row>
@@ -2793,10 +2793,10 @@
         <v>198</v>
       </c>
       <c r="O23" s="1" t="s">
-        <v>236</v>
+        <v>295</v>
       </c>
       <c r="P23" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="Q23" s="1" t="s">
         <v>144</v>
@@ -2805,16 +2805,16 @@
         <v>152</v>
       </c>
       <c r="S23" s="19" t="s">
-        <v>258</v>
+        <v>244</v>
       </c>
       <c r="T23" s="21" t="s">
-        <v>273</v>
+        <v>259</v>
       </c>
       <c r="U23" s="25" t="s">
+        <v>246</v>
+      </c>
+      <c r="V23" s="21" t="s">
         <v>260</v>
-      </c>
-      <c r="V23" s="21" t="s">
-        <v>274</v>
       </c>
       <c r="W23" s="21"/>
     </row>
@@ -2858,10 +2858,10 @@
         <v>198</v>
       </c>
       <c r="O24" s="1" t="s">
-        <v>237</v>
+        <v>296</v>
       </c>
       <c r="P24" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="Q24" s="1" t="s">
         <v>145</v>
@@ -2870,16 +2870,16 @@
         <v>152</v>
       </c>
       <c r="S24" s="19" t="s">
-        <v>258</v>
+        <v>244</v>
       </c>
       <c r="T24" s="21" t="s">
-        <v>275</v>
+        <v>261</v>
       </c>
       <c r="U24" s="25" t="s">
+        <v>246</v>
+      </c>
+      <c r="V24" s="21" t="s">
         <v>260</v>
-      </c>
-      <c r="V24" s="21" t="s">
-        <v>274</v>
       </c>
       <c r="W24" s="21"/>
     </row>
@@ -2916,7 +2916,7 @@
         <v>169</v>
       </c>
       <c r="L25" s="1" t="s">
-        <v>292</v>
+        <v>278</v>
       </c>
       <c r="M25" s="1" t="s">
         <v>49</v>
@@ -2925,10 +2925,10 @@
         <v>198</v>
       </c>
       <c r="O25" s="1" t="s">
-        <v>238</v>
+        <v>297</v>
       </c>
       <c r="P25" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="Q25" s="1" t="s">
         <v>177</v>
@@ -2937,7 +2937,7 @@
         <v>152</v>
       </c>
       <c r="S25" s="17" t="s">
-        <v>264</v>
+        <v>250</v>
       </c>
       <c r="T25" s="21"/>
       <c r="U25" s="21"/>
@@ -2979,7 +2979,7 @@
         <v>146</v>
       </c>
       <c r="P26" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="Q26" s="1" t="s">
         <v>146</v>
@@ -2988,7 +2988,7 @@
         <v>152</v>
       </c>
       <c r="S26" s="17" t="s">
-        <v>264</v>
+        <v>250</v>
       </c>
       <c r="T26" s="21"/>
       <c r="U26" s="21"/>
@@ -3029,29 +3029,29 @@
         <v>198</v>
       </c>
       <c r="O27" s="1" t="s">
-        <v>245</v>
+        <v>298</v>
       </c>
       <c r="P27" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="Q27" s="1" t="s">
         <v>166</v>
       </c>
       <c r="R27" s="1"/>
       <c r="S27" s="19" t="s">
-        <v>258</v>
+        <v>244</v>
       </c>
       <c r="T27" s="21" t="s">
-        <v>276</v>
+        <v>262</v>
       </c>
       <c r="U27" s="25" t="s">
-        <v>260</v>
+        <v>246</v>
       </c>
       <c r="V27" s="21" t="s">
         <v>56</v>
       </c>
       <c r="W27" s="10" t="s">
-        <v>277</v>
+        <v>263</v>
       </c>
     </row>
     <row r="28" spans="1:23" ht="30" x14ac:dyDescent="0.25">
@@ -3088,29 +3088,29 @@
         <v>198</v>
       </c>
       <c r="O28" s="1" t="s">
-        <v>246</v>
+        <v>299</v>
       </c>
       <c r="P28" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="Q28" s="1" t="s">
         <v>170</v>
       </c>
       <c r="R28" s="1"/>
       <c r="S28" s="19" t="s">
-        <v>258</v>
+        <v>244</v>
       </c>
       <c r="T28" s="21" t="s">
-        <v>278</v>
+        <v>264</v>
       </c>
       <c r="U28" s="25" t="s">
-        <v>260</v>
+        <v>246</v>
       </c>
       <c r="V28" s="21" t="s">
         <v>56</v>
       </c>
       <c r="W28" s="10" t="s">
-        <v>277</v>
+        <v>263</v>
       </c>
     </row>
     <row r="29" spans="1:23" ht="30" x14ac:dyDescent="0.25">
@@ -3147,29 +3147,29 @@
         <v>198</v>
       </c>
       <c r="O29" s="1" t="s">
-        <v>247</v>
+        <v>300</v>
       </c>
       <c r="P29" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="Q29" s="1" t="s">
         <v>147</v>
       </c>
       <c r="R29" s="1"/>
       <c r="S29" s="19" t="s">
-        <v>258</v>
+        <v>244</v>
       </c>
       <c r="T29" s="21" t="s">
-        <v>279</v>
+        <v>265</v>
       </c>
       <c r="U29" s="25" t="s">
-        <v>260</v>
+        <v>246</v>
       </c>
       <c r="V29" s="21" t="s">
         <v>56</v>
       </c>
       <c r="W29" s="10" t="s">
-        <v>277</v>
+        <v>263</v>
       </c>
     </row>
     <row r="30" spans="1:23" ht="45" x14ac:dyDescent="0.25">
@@ -3209,20 +3209,20 @@
         <v>148</v>
       </c>
       <c r="P30" s="1" t="s">
-        <v>299</v>
+        <v>285</v>
       </c>
       <c r="Q30" s="1" t="s">
         <v>148</v>
       </c>
       <c r="R30" s="1"/>
       <c r="S30" s="19" t="s">
-        <v>258</v>
+        <v>244</v>
       </c>
       <c r="T30" s="21" t="s">
-        <v>280</v>
+        <v>266</v>
       </c>
       <c r="U30" s="25" t="s">
-        <v>262</v>
+        <v>248</v>
       </c>
       <c r="V30" s="21" t="s">
         <v>56</v>
@@ -3266,26 +3266,26 @@
         <v>215</v>
       </c>
       <c r="P31" s="3" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="Q31" s="3" t="s">
         <v>215</v>
       </c>
       <c r="R31" s="1"/>
       <c r="S31" s="19" t="s">
-        <v>266</v>
+        <v>252</v>
       </c>
       <c r="T31" s="3" t="s">
-        <v>293</v>
+        <v>279</v>
       </c>
       <c r="U31" s="21" t="s">
-        <v>281</v>
+        <v>267</v>
       </c>
       <c r="V31" s="21" t="s">
         <v>56</v>
       </c>
       <c r="W31" s="10" t="s">
-        <v>277</v>
+        <v>263</v>
       </c>
     </row>
     <row r="32" spans="1:23" ht="45" x14ac:dyDescent="0.25">
@@ -3322,27 +3322,27 @@
         <v>198</v>
       </c>
       <c r="O32" s="3" t="s">
-        <v>291</v>
+        <v>277</v>
       </c>
       <c r="P32" s="3" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="Q32" s="3" t="s">
-        <v>291</v>
+        <v>277</v>
       </c>
       <c r="R32" s="1"/>
       <c r="S32" s="20" t="s">
-        <v>266</v>
+        <v>252</v>
       </c>
       <c r="T32" s="26" t="s">
-        <v>293</v>
+        <v>279</v>
       </c>
       <c r="U32" s="19" t="s">
-        <v>281</v>
+        <v>267</v>
       </c>
       <c r="V32" s="19"/>
       <c r="W32" s="10" t="s">
-        <v>277</v>
+        <v>263</v>
       </c>
     </row>
     <row r="33" spans="1:23" ht="45" x14ac:dyDescent="0.25">
@@ -3377,28 +3377,28 @@
         <v>198</v>
       </c>
       <c r="O33" s="3" t="s">
-        <v>291</v>
+        <v>277</v>
       </c>
       <c r="P33" s="3" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="Q33" s="3" t="s">
-        <v>291</v>
+        <v>277</v>
       </c>
       <c r="R33" s="10" t="s">
         <v>152</v>
       </c>
       <c r="S33" s="19" t="s">
-        <v>266</v>
+        <v>252</v>
       </c>
       <c r="T33" s="3" t="s">
-        <v>293</v>
+        <v>279</v>
       </c>
       <c r="U33" s="21" t="s">
-        <v>281</v>
+        <v>267</v>
       </c>
       <c r="V33" s="10" t="s">
-        <v>284</v>
+        <v>270</v>
       </c>
       <c r="W33" s="21"/>
     </row>
@@ -3439,26 +3439,26 @@
         <v>216</v>
       </c>
       <c r="P34" s="3" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="Q34" s="3" t="s">
         <v>216</v>
       </c>
       <c r="R34" s="1"/>
       <c r="S34" s="19" t="s">
-        <v>266</v>
+        <v>252</v>
       </c>
       <c r="T34" s="3" t="s">
-        <v>293</v>
+        <v>279</v>
       </c>
       <c r="U34" s="21" t="s">
-        <v>281</v>
+        <v>267</v>
       </c>
       <c r="V34" s="21" t="s">
         <v>56</v>
       </c>
       <c r="W34" s="10" t="s">
-        <v>277</v>
+        <v>263</v>
       </c>
     </row>
     <row r="35" spans="1:23" ht="45" x14ac:dyDescent="0.25">
@@ -3498,26 +3498,26 @@
         <v>218</v>
       </c>
       <c r="P35" s="3" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="Q35" s="3" t="s">
         <v>218</v>
       </c>
       <c r="R35" s="1"/>
       <c r="S35" s="19" t="s">
-        <v>266</v>
+        <v>252</v>
       </c>
       <c r="T35" s="3" t="s">
-        <v>293</v>
+        <v>279</v>
       </c>
       <c r="U35" s="21" t="s">
-        <v>281</v>
+        <v>267</v>
       </c>
       <c r="V35" s="21" t="s">
         <v>56</v>
       </c>
       <c r="W35" s="10" t="s">
-        <v>277</v>
+        <v>263</v>
       </c>
     </row>
     <row r="36" spans="1:23" ht="45" x14ac:dyDescent="0.25">
@@ -3557,26 +3557,26 @@
         <v>217</v>
       </c>
       <c r="P36" s="3" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="Q36" s="3" t="s">
         <v>217</v>
       </c>
       <c r="R36" s="1"/>
       <c r="S36" s="19" t="s">
-        <v>266</v>
+        <v>252</v>
       </c>
       <c r="T36" s="3" t="s">
-        <v>293</v>
+        <v>279</v>
       </c>
       <c r="U36" s="21" t="s">
-        <v>281</v>
+        <v>267</v>
       </c>
       <c r="V36" s="21" t="s">
         <v>56</v>
       </c>
       <c r="W36" s="10" t="s">
-        <v>277</v>
+        <v>263</v>
       </c>
     </row>
     <row r="37" spans="1:23" ht="45" x14ac:dyDescent="0.25">
@@ -3614,26 +3614,26 @@
         <v>179</v>
       </c>
       <c r="P37" s="1" t="s">
-        <v>251</v>
+        <v>237</v>
       </c>
       <c r="Q37" s="1" t="s">
         <v>179</v>
       </c>
       <c r="R37" s="1"/>
       <c r="S37" s="19" t="s">
-        <v>266</v>
+        <v>252</v>
       </c>
       <c r="T37" s="1" t="s">
-        <v>294</v>
+        <v>280</v>
       </c>
       <c r="U37" s="21" t="s">
-        <v>281</v>
+        <v>267</v>
       </c>
       <c r="V37" s="21" t="s">
         <v>56</v>
       </c>
       <c r="W37" s="10" t="s">
-        <v>277</v>
+        <v>263</v>
       </c>
     </row>
     <row r="38" spans="1:23" ht="45" x14ac:dyDescent="0.25">
@@ -3673,26 +3673,26 @@
         <v>149</v>
       </c>
       <c r="P38" s="7" t="s">
-        <v>252</v>
+        <v>238</v>
       </c>
       <c r="Q38" s="7" t="s">
         <v>149</v>
       </c>
       <c r="R38" s="1"/>
       <c r="S38" s="19" t="s">
-        <v>266</v>
+        <v>252</v>
       </c>
       <c r="T38" s="21" t="s">
-        <v>264</v>
+        <v>250</v>
       </c>
       <c r="U38" s="21" t="s">
-        <v>267</v>
+        <v>253</v>
       </c>
       <c r="V38" s="21" t="s">
         <v>56</v>
       </c>
       <c r="W38" s="10" t="s">
-        <v>277</v>
+        <v>263</v>
       </c>
     </row>
     <row r="39" spans="1:23" ht="30" x14ac:dyDescent="0.25">
@@ -3732,26 +3732,26 @@
         <v>151</v>
       </c>
       <c r="P39" s="7" t="s">
-        <v>290</v>
+        <v>276</v>
       </c>
       <c r="Q39" s="1" t="s">
         <v>151</v>
       </c>
       <c r="R39" s="1"/>
       <c r="S39" s="19" t="s">
-        <v>266</v>
+        <v>252</v>
       </c>
       <c r="T39" s="21" t="s">
-        <v>264</v>
+        <v>250</v>
       </c>
       <c r="U39" s="21" t="s">
-        <v>267</v>
+        <v>253</v>
       </c>
       <c r="V39" s="21" t="s">
         <v>56</v>
       </c>
       <c r="W39" s="10" t="s">
-        <v>277</v>
+        <v>263</v>
       </c>
     </row>
     <row r="40" spans="1:23" ht="30" x14ac:dyDescent="0.25">
@@ -3791,26 +3791,26 @@
         <v>150</v>
       </c>
       <c r="P40" s="7" t="s">
-        <v>253</v>
+        <v>239</v>
       </c>
       <c r="Q40" s="7" t="s">
         <v>150</v>
       </c>
       <c r="R40" s="1"/>
       <c r="S40" s="19" t="s">
-        <v>266</v>
+        <v>252</v>
       </c>
       <c r="T40" s="21" t="s">
-        <v>264</v>
+        <v>250</v>
       </c>
       <c r="U40" s="21" t="s">
-        <v>267</v>
+        <v>253</v>
       </c>
       <c r="V40" s="21" t="s">
         <v>56</v>
       </c>
       <c r="W40" s="10" t="s">
-        <v>277</v>
+        <v>263</v>
       </c>
     </row>
     <row r="41" spans="1:23" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Code Version 01062020 22:20
</commit_message>
<xml_diff>
--- a/Prime_Job_Automation/Configuration/RuleFactory/Master Rule Factory.xlsx
+++ b/Prime_Job_Automation/Configuration/RuleFactory/Master Rule Factory.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\PJA\Prime_Job_Automation\Configuration\RuleFactory\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1B068B9-407D-48AF-B988-EE41A464BA5A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2C6FDE5-2624-495C-9DC6-B3C5A95E8489}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" tabRatio="351" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1513,8 +1513,8 @@
   <dimension ref="A1:W49"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <pane xSplit="2" topLeftCell="I1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1698,7 +1698,7 @@
         <v>48</v>
       </c>
       <c r="N3" s="7" t="s">
-        <v>198</v>
+        <v>210</v>
       </c>
       <c r="O3" s="7" t="s">
         <v>172</v>

</xml_diff>